<commit_message>
15th April 4th update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/state/ncov19state_long.xlsx
+++ b/covid19_data/excel/state/ncov19state_long.xlsx
@@ -927,7 +927,7 @@
       </c>
       <c r="AE4"/>
       <c r="AF4" t="n">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="AG4"/>
       <c r="AH4"/>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="AE13"/>
       <c r="AF13" t="n">
-        <v>45</v>
+        <v>116</v>
       </c>
       <c r="AG13"/>
       <c r="AH13"/>
@@ -1746,7 +1746,9 @@
         <v>2</v>
       </c>
       <c r="AE14"/>
-      <c r="AF14"/>
+      <c r="AF14" t="n">
+        <v>6</v>
+      </c>
       <c r="AG14"/>
       <c r="AH14" t="n">
         <v>1</v>
@@ -1839,7 +1841,9 @@
         <v>1</v>
       </c>
       <c r="AE15"/>
-      <c r="AF15"/>
+      <c r="AF15" t="n">
+        <v>2</v>
+      </c>
       <c r="AG15"/>
       <c r="AH15"/>
       <c r="AI15"/>
@@ -1928,7 +1932,9 @@
         <v>8</v>
       </c>
       <c r="AE16"/>
-      <c r="AF16"/>
+      <c r="AF16" t="n">
+        <v>22</v>
+      </c>
       <c r="AG16" t="n">
         <v>1</v>
       </c>
@@ -2019,7 +2025,9 @@
         <v>3</v>
       </c>
       <c r="AE17"/>
-      <c r="AF17"/>
+      <c r="AF17" t="n">
+        <v>1</v>
+      </c>
       <c r="AG17"/>
       <c r="AH17"/>
       <c r="AI17"/>
@@ -2111,7 +2119,7 @@
       </c>
       <c r="AE18"/>
       <c r="AF18" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AG18" t="n">
         <v>1</v>
@@ -2239,7 +2247,9 @@
       <c r="AE19" t="n">
         <v>2</v>
       </c>
-      <c r="AF19"/>
+      <c r="AF19" t="n">
+        <v>1</v>
+      </c>
       <c r="AG19" t="n">
         <v>3</v>
       </c>
@@ -2419,7 +2429,9 @@
         <v>127</v>
       </c>
       <c r="AE21"/>
-      <c r="AF21"/>
+      <c r="AF21" t="n">
+        <v>197</v>
+      </c>
       <c r="AG21"/>
       <c r="AH21"/>
       <c r="AI21"/>
@@ -2532,7 +2544,9 @@
       <c r="AE22" t="n">
         <v>6</v>
       </c>
-      <c r="AF22"/>
+      <c r="AF22" t="n">
+        <v>232</v>
+      </c>
       <c r="AG22" t="n">
         <v>7</v>
       </c>
@@ -2676,7 +2690,9 @@
       <c r="AC24"/>
       <c r="AD24"/>
       <c r="AE24"/>
-      <c r="AF24"/>
+      <c r="AF24" t="n">
+        <v>6</v>
+      </c>
       <c r="AG24"/>
       <c r="AH24"/>
       <c r="AI24"/>
@@ -3013,7 +3029,9 @@
         <v>8</v>
       </c>
       <c r="AE29"/>
-      <c r="AF29"/>
+      <c r="AF29" t="n">
+        <v>2</v>
+      </c>
       <c r="AG29"/>
       <c r="AH29"/>
       <c r="AI29"/>
@@ -3125,7 +3143,7 @@
       </c>
       <c r="AE30"/>
       <c r="AF30" t="n">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="AG30"/>
       <c r="AH30"/>
@@ -3235,7 +3253,9 @@
         <v>31</v>
       </c>
       <c r="AE31"/>
-      <c r="AF31"/>
+      <c r="AF31" t="n">
+        <v>38</v>
+      </c>
       <c r="AG31"/>
       <c r="AH31"/>
       <c r="AI31" t="n">
@@ -3348,7 +3368,9 @@
       <c r="AE32" t="n">
         <v>1</v>
       </c>
-      <c r="AF32"/>
+      <c r="AF32" t="n">
+        <v>6</v>
+      </c>
       <c r="AG32" t="n">
         <v>1</v>
       </c>
@@ -3528,7 +3550,9 @@
         <v>102</v>
       </c>
       <c r="AE34"/>
-      <c r="AF34"/>
+      <c r="AF34" t="n">
+        <v>75</v>
+      </c>
       <c r="AG34"/>
       <c r="AH34" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
16th April 2nd update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/state/ncov19state_long.xlsx
+++ b/covid19_data/excel/state/ncov19state_long.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t xml:space="preserve">detectedstate</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t xml:space="preserve">16/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">17/03/2020</t>
@@ -743,10 +746,13 @@
       <c r="AW1" t="s">
         <v>48</v>
       </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
@@ -798,10 +804,11 @@
       <c r="AU2"/>
       <c r="AV2"/>
       <c r="AW2"/>
+      <c r="AX2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -846,25 +853,26 @@
       <c r="AN3"/>
       <c r="AO3"/>
       <c r="AP3"/>
-      <c r="AQ3" t="n">
-        <v>1</v>
-      </c>
+      <c r="AQ3"/>
       <c r="AR3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS3" t="n">
         <v>5</v>
       </c>
-      <c r="AS3" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT3"/>
+      <c r="AT3" t="n">
+        <v>3</v>
+      </c>
       <c r="AU3"/>
-      <c r="AV3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW3"/>
+      <c r="AV3"/>
+      <c r="AW3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B4" t="n">
         <v>67</v>
@@ -932,15 +940,13 @@
       <c r="AG4"/>
       <c r="AH4"/>
       <c r="AI4"/>
-      <c r="AJ4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AK4"/>
-      <c r="AL4" t="n">
-        <v>2</v>
-      </c>
+      <c r="AJ4"/>
+      <c r="AK4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL4"/>
       <c r="AM4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN4" t="n">
         <v>1</v>
@@ -949,31 +955,34 @@
         <v>1</v>
       </c>
       <c r="AP4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT4" t="n">
         <v>6</v>
       </c>
-      <c r="AT4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AU4"/>
-      <c r="AV4" t="n">
-        <v>2</v>
-      </c>
+      <c r="AU4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV4"/>
       <c r="AW4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX4" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -1025,10 +1034,11 @@
       <c r="AU5"/>
       <c r="AV5"/>
       <c r="AW5"/>
+      <c r="AX5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B6" t="n">
         <v>15</v>
@@ -1091,13 +1101,14 @@
       <c r="AT6"/>
       <c r="AU6"/>
       <c r="AV6"/>
-      <c r="AW6" t="n">
+      <c r="AW6"/>
+      <c r="AX6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -1150,7 +1161,7 @@
       <c r="AD7"/>
       <c r="AE7"/>
       <c r="AF7" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AG7"/>
       <c r="AH7"/>
@@ -1158,37 +1169,38 @@
       <c r="AJ7"/>
       <c r="AK7"/>
       <c r="AL7"/>
-      <c r="AM7" t="n">
-        <v>2</v>
-      </c>
+      <c r="AM7"/>
       <c r="AN7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO7"/>
-      <c r="AP7" t="n">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP7"/>
       <c r="AQ7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AR7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AS7" t="n">
         <v>2</v>
       </c>
       <c r="AT7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU7" t="n">
         <v>4</v>
       </c>
-      <c r="AU7"/>
       <c r="AV7"/>
-      <c r="AW7" t="n">
+      <c r="AW7"/>
+      <c r="AX7" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -1232,38 +1244,39 @@
       <c r="AG8"/>
       <c r="AH8"/>
       <c r="AI8"/>
-      <c r="AJ8" t="n">
-        <v>1</v>
-      </c>
+      <c r="AJ8"/>
       <c r="AK8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL8" t="n">
         <v>4</v>
       </c>
-      <c r="AL8"/>
-      <c r="AM8" t="n">
-        <v>1</v>
-      </c>
+      <c r="AM8"/>
       <c r="AN8" t="n">
         <v>1</v>
       </c>
-      <c r="AO8"/>
+      <c r="AO8" t="n">
+        <v>1</v>
+      </c>
       <c r="AP8"/>
       <c r="AQ8"/>
-      <c r="AR8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS8"/>
+      <c r="AR8"/>
+      <c r="AS8" t="n">
+        <v>1</v>
+      </c>
       <c r="AT8"/>
       <c r="AU8"/>
-      <c r="AV8" t="n">
+      <c r="AV8"/>
+      <c r="AW8" t="n">
         <v>5</v>
       </c>
-      <c r="AW8" t="n">
+      <c r="AX8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -1309,36 +1322,37 @@
       <c r="AG9"/>
       <c r="AH9"/>
       <c r="AI9"/>
-      <c r="AJ9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK9"/>
+      <c r="AJ9"/>
+      <c r="AK9" t="n">
+        <v>1</v>
+      </c>
       <c r="AL9"/>
       <c r="AM9"/>
       <c r="AN9"/>
       <c r="AO9"/>
-      <c r="AP9" t="n">
-        <v>2</v>
-      </c>
+      <c r="AP9"/>
       <c r="AQ9" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR9"/>
-      <c r="AS9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT9"/>
+        <v>2</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS9"/>
+      <c r="AT9" t="n">
+        <v>1</v>
+      </c>
       <c r="AU9"/>
-      <c r="AV9" t="n">
-        <v>1</v>
-      </c>
+      <c r="AV9"/>
       <c r="AW9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B10"/>
       <c r="C10"/>
@@ -1390,10 +1404,11 @@
       <c r="AU10"/>
       <c r="AV10"/>
       <c r="AW10"/>
+      <c r="AX10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B11" t="n">
         <v>32</v>
@@ -1467,56 +1482,59 @@
         <v>51</v>
       </c>
       <c r="AE11"/>
-      <c r="AF11"/>
+      <c r="AF11" t="n">
+        <v>17</v>
+      </c>
       <c r="AG11"/>
-      <c r="AH11" t="n">
-        <v>3</v>
-      </c>
+      <c r="AH11"/>
       <c r="AI11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AJ11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AK11" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL11" t="n">
         <v>6</v>
       </c>
-      <c r="AL11" t="n">
+      <c r="AM11" t="n">
         <v>7</v>
       </c>
-      <c r="AM11" t="n">
-        <v>1</v>
-      </c>
       <c r="AN11" t="n">
-        <v>2</v>
-      </c>
-      <c r="AO11"/>
-      <c r="AP11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP11"/>
+      <c r="AQ11" t="n">
         <v>5</v>
       </c>
-      <c r="AQ11" t="n">
+      <c r="AR11" t="n">
         <v>4</v>
       </c>
-      <c r="AR11" t="n">
-        <v>1</v>
-      </c>
       <c r="AS11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT11" t="n">
         <v>9</v>
       </c>
-      <c r="AT11" t="n">
+      <c r="AU11" t="n">
         <v>23</v>
       </c>
-      <c r="AU11"/>
-      <c r="AV11" t="n">
+      <c r="AV11"/>
+      <c r="AW11" t="n">
         <v>25</v>
       </c>
-      <c r="AW11" t="n">
+      <c r="AX11" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B12"/>
       <c r="C12"/>
@@ -1562,22 +1580,23 @@
       <c r="AM12"/>
       <c r="AN12"/>
       <c r="AO12"/>
-      <c r="AP12" t="n">
-        <v>3</v>
-      </c>
-      <c r="AQ12"/>
+      <c r="AP12"/>
+      <c r="AQ12" t="n">
+        <v>3</v>
+      </c>
       <c r="AR12"/>
       <c r="AS12"/>
-      <c r="AT12" t="n">
-        <v>2</v>
-      </c>
-      <c r="AU12"/>
+      <c r="AT12"/>
+      <c r="AU12" t="n">
+        <v>2</v>
+      </c>
       <c r="AV12"/>
       <c r="AW12"/>
+      <c r="AX12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B13" t="n">
         <v>13</v>
@@ -1641,52 +1660,55 @@
         <v>116</v>
       </c>
       <c r="AG13"/>
-      <c r="AH13"/>
+      <c r="AH13" t="n">
+        <v>105</v>
+      </c>
       <c r="AI13"/>
-      <c r="AJ13" t="n">
-        <v>2</v>
-      </c>
+      <c r="AJ13"/>
       <c r="AK13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL13" t="n">
         <v>5</v>
       </c>
-      <c r="AL13" t="n">
+      <c r="AM13" t="n">
         <v>7</v>
       </c>
-      <c r="AM13" t="n">
+      <c r="AN13" t="n">
         <v>4</v>
       </c>
-      <c r="AN13" t="n">
+      <c r="AO13" t="n">
         <v>12</v>
       </c>
-      <c r="AO13" t="n">
+      <c r="AP13" t="n">
         <v>6</v>
       </c>
-      <c r="AP13" t="n">
-        <v>2</v>
-      </c>
       <c r="AQ13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR13" t="n">
         <v>6</v>
       </c>
-      <c r="AR13" t="n">
-        <v>3</v>
-      </c>
       <c r="AS13" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AT13" t="n">
         <v>8</v>
       </c>
-      <c r="AU13"/>
-      <c r="AV13" t="n">
+      <c r="AU13" t="n">
+        <v>8</v>
+      </c>
+      <c r="AV13"/>
+      <c r="AW13" t="n">
         <v>7</v>
       </c>
-      <c r="AW13" t="n">
+      <c r="AX13" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -1750,28 +1772,26 @@
         <v>6</v>
       </c>
       <c r="AG14"/>
-      <c r="AH14" t="n">
-        <v>1</v>
-      </c>
+      <c r="AH14"/>
       <c r="AI14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ14"/>
-      <c r="AK14" t="n">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK14"/>
       <c r="AL14" t="n">
         <v>2</v>
       </c>
-      <c r="AM14"/>
-      <c r="AN14" t="n">
+      <c r="AM14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN14"/>
+      <c r="AO14" t="n">
         <v>7</v>
       </c>
-      <c r="AO14" t="n">
-        <v>2</v>
-      </c>
       <c r="AP14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AQ14" t="n">
         <v>1</v>
@@ -1780,20 +1800,23 @@
         <v>1</v>
       </c>
       <c r="AS14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AT14"/>
+        <v>1</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>2</v>
+      </c>
       <c r="AU14"/>
-      <c r="AV14" t="n">
-        <v>1</v>
-      </c>
+      <c r="AV14"/>
       <c r="AW14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX14" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -1848,15 +1871,15 @@
       <c r="AH15"/>
       <c r="AI15"/>
       <c r="AJ15"/>
-      <c r="AK15" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL15"/>
+      <c r="AK15"/>
+      <c r="AL15" t="n">
+        <v>2</v>
+      </c>
       <c r="AM15"/>
-      <c r="AN15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO15"/>
+      <c r="AN15"/>
+      <c r="AO15" t="n">
+        <v>1</v>
+      </c>
       <c r="AP15"/>
       <c r="AQ15"/>
       <c r="AR15"/>
@@ -1865,10 +1888,11 @@
       <c r="AU15"/>
       <c r="AV15"/>
       <c r="AW15"/>
+      <c r="AX15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" t="n">
         <v>7</v>
@@ -1939,43 +1963,44 @@
         <v>1</v>
       </c>
       <c r="AH16"/>
-      <c r="AI16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ16"/>
+      <c r="AI16"/>
+      <c r="AJ16" t="n">
+        <v>1</v>
+      </c>
       <c r="AK16"/>
       <c r="AL16"/>
       <c r="AM16"/>
       <c r="AN16"/>
-      <c r="AO16" t="n">
-        <v>2</v>
-      </c>
+      <c r="AO16"/>
       <c r="AP16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ16" t="n">
         <v>5</v>
       </c>
-      <c r="AQ16" t="n">
-        <v>3</v>
-      </c>
       <c r="AR16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS16" t="n">
         <v>6</v>
       </c>
-      <c r="AS16" t="n">
+      <c r="AT16" t="n">
         <v>13</v>
       </c>
-      <c r="AT16" t="n">
+      <c r="AU16" t="n">
         <v>5</v>
       </c>
-      <c r="AU16"/>
-      <c r="AV16" t="n">
+      <c r="AV16"/>
+      <c r="AW16" t="n">
         <v>11</v>
       </c>
-      <c r="AW16" t="n">
+      <c r="AX16" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -2044,13 +2069,14 @@
       <c r="AT17"/>
       <c r="AU17"/>
       <c r="AV17"/>
-      <c r="AW17" t="n">
+      <c r="AW17"/>
+      <c r="AX17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B18" t="n">
         <v>9</v>
@@ -2124,54 +2150,55 @@
       <c r="AG18" t="n">
         <v>1</v>
       </c>
-      <c r="AH18" t="n">
+      <c r="AH18"/>
+      <c r="AI18" t="n">
         <v>4</v>
       </c>
-      <c r="AI18" t="n">
-        <v>3</v>
-      </c>
       <c r="AJ18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK18"/>
-      <c r="AL18" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL18"/>
+      <c r="AM18" t="n">
         <v>5</v>
       </c>
-      <c r="AM18" t="n">
+      <c r="AN18" t="n">
         <v>6</v>
       </c>
-      <c r="AN18" t="n">
+      <c r="AO18" t="n">
         <v>7</v>
       </c>
-      <c r="AO18" t="n">
+      <c r="AP18" t="n">
         <v>8</v>
       </c>
-      <c r="AP18" t="n">
+      <c r="AQ18" t="n">
         <v>10</v>
       </c>
-      <c r="AQ18" t="n">
+      <c r="AR18" t="n">
         <v>4</v>
       </c>
-      <c r="AR18" t="n">
+      <c r="AS18" t="n">
         <v>9</v>
       </c>
-      <c r="AS18" t="n">
+      <c r="AT18" t="n">
         <v>12</v>
       </c>
-      <c r="AT18" t="n">
+      <c r="AU18" t="n">
         <v>7</v>
       </c>
-      <c r="AU18"/>
-      <c r="AV18" t="n">
+      <c r="AV18"/>
+      <c r="AW18" t="n">
         <v>5</v>
       </c>
-      <c r="AW18" t="n">
+      <c r="AX18" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B19" t="n">
         <v>24</v>
@@ -2255,52 +2282,53 @@
       </c>
       <c r="AH19"/>
       <c r="AI19"/>
-      <c r="AJ19" t="n">
-        <v>1</v>
-      </c>
+      <c r="AJ19"/>
       <c r="AK19" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="AL19" t="n">
         <v>12</v>
       </c>
       <c r="AM19" t="n">
+        <v>12</v>
+      </c>
+      <c r="AN19" t="n">
         <v>15</v>
       </c>
-      <c r="AN19" t="n">
+      <c r="AO19" t="n">
         <v>28</v>
       </c>
-      <c r="AO19" t="n">
+      <c r="AP19" t="n">
         <v>14</v>
       </c>
-      <c r="AP19" t="n">
+      <c r="AQ19" t="n">
         <v>9</v>
       </c>
-      <c r="AQ19" t="n">
+      <c r="AR19" t="n">
         <v>19</v>
       </c>
-      <c r="AR19" t="n">
+      <c r="AS19" t="n">
         <v>39</v>
       </c>
-      <c r="AS19" t="n">
+      <c r="AT19" t="n">
         <v>6</v>
       </c>
-      <c r="AT19" t="n">
+      <c r="AU19" t="n">
         <v>20</v>
       </c>
-      <c r="AU19" t="n">
-        <v>1</v>
-      </c>
       <c r="AV19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW19" t="n">
         <v>32</v>
       </c>
-      <c r="AW19" t="n">
+      <c r="AX19" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B20"/>
       <c r="C20"/>
@@ -2342,20 +2370,22 @@
       <c r="AC20"/>
       <c r="AD20"/>
       <c r="AE20"/>
-      <c r="AF20"/>
+      <c r="AF20" t="n">
+        <v>1</v>
+      </c>
       <c r="AG20"/>
-      <c r="AH20" t="n">
+      <c r="AH20"/>
+      <c r="AI20" t="n">
         <v>5</v>
       </c>
-      <c r="AI20"/>
       <c r="AJ20"/>
-      <c r="AK20" t="n">
-        <v>2</v>
-      </c>
+      <c r="AK20"/>
       <c r="AL20" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM20"/>
+        <v>2</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>3</v>
+      </c>
       <c r="AN20"/>
       <c r="AO20"/>
       <c r="AP20"/>
@@ -2366,10 +2396,11 @@
       <c r="AU20"/>
       <c r="AV20"/>
       <c r="AW20"/>
+      <c r="AX20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B21" t="n">
         <v>32</v>
@@ -2433,44 +2464,47 @@
         <v>197</v>
       </c>
       <c r="AG21"/>
-      <c r="AH21"/>
+      <c r="AH21" t="n">
+        <v>42</v>
+      </c>
       <c r="AI21"/>
       <c r="AJ21"/>
-      <c r="AK21" t="n">
+      <c r="AK21"/>
+      <c r="AL21" t="n">
         <v>4</v>
       </c>
-      <c r="AL21"/>
-      <c r="AM21" t="n">
-        <v>2</v>
-      </c>
-      <c r="AN21"/>
-      <c r="AO21" t="n">
-        <v>1</v>
-      </c>
+      <c r="AM21"/>
+      <c r="AN21" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO21"/>
       <c r="AP21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ21" t="n">
         <v>8</v>
       </c>
-      <c r="AQ21" t="n">
+      <c r="AR21" t="n">
         <v>5</v>
       </c>
-      <c r="AR21" t="n">
+      <c r="AS21" t="n">
         <v>9</v>
       </c>
-      <c r="AS21" t="n">
+      <c r="AT21" t="n">
         <v>10</v>
       </c>
-      <c r="AT21"/>
       <c r="AU21"/>
-      <c r="AV21" t="n">
+      <c r="AV21"/>
+      <c r="AW21" t="n">
         <v>8</v>
       </c>
-      <c r="AW21" t="n">
+      <c r="AX21" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B22" t="n">
         <v>33</v>
@@ -2550,56 +2584,57 @@
       <c r="AG22" t="n">
         <v>7</v>
       </c>
-      <c r="AH22" t="n">
-        <v>2</v>
-      </c>
+      <c r="AH22"/>
       <c r="AI22" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ22" t="n">
         <v>4</v>
       </c>
-      <c r="AJ22" t="n">
-        <v>3</v>
-      </c>
       <c r="AK22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL22" t="n">
         <v>4</v>
       </c>
-      <c r="AL22" t="n">
+      <c r="AM22" t="n">
         <v>12</v>
       </c>
-      <c r="AM22" t="n">
+      <c r="AN22" t="n">
         <v>10</v>
       </c>
-      <c r="AN22" t="n">
+      <c r="AO22" t="n">
         <v>15</v>
       </c>
-      <c r="AO22" t="n">
+      <c r="AP22" t="n">
         <v>18</v>
       </c>
-      <c r="AP22" t="n">
+      <c r="AQ22" t="n">
         <v>15</v>
       </c>
-      <c r="AQ22" t="n">
-        <v>3</v>
-      </c>
       <c r="AR22" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="AS22" t="n">
         <v>28</v>
       </c>
       <c r="AT22" t="n">
+        <v>28</v>
+      </c>
+      <c r="AU22" t="n">
         <v>22</v>
       </c>
-      <c r="AU22"/>
-      <c r="AV22" t="n">
+      <c r="AV22"/>
+      <c r="AW22" t="n">
         <v>17</v>
       </c>
-      <c r="AW22" t="n">
+      <c r="AX22" t="n">
         <v>82</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -2642,10 +2677,10 @@
       <c r="AL23"/>
       <c r="AM23"/>
       <c r="AN23"/>
-      <c r="AO23" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP23"/>
+      <c r="AO23"/>
+      <c r="AP23" t="n">
+        <v>1</v>
+      </c>
       <c r="AQ23"/>
       <c r="AR23"/>
       <c r="AS23"/>
@@ -2653,10 +2688,11 @@
       <c r="AU23"/>
       <c r="AV23"/>
       <c r="AW23"/>
+      <c r="AX23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -2710,10 +2746,11 @@
       <c r="AU24"/>
       <c r="AV24"/>
       <c r="AW24"/>
+      <c r="AX24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -2755,20 +2792,21 @@
       <c r="AM25"/>
       <c r="AN25"/>
       <c r="AO25"/>
-      <c r="AP25" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ25"/>
+      <c r="AP25"/>
+      <c r="AQ25" t="n">
+        <v>1</v>
+      </c>
       <c r="AR25"/>
       <c r="AS25"/>
       <c r="AT25"/>
       <c r="AU25"/>
       <c r="AV25"/>
       <c r="AW25"/>
+      <c r="AX25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B26"/>
       <c r="C26"/>
@@ -2820,10 +2858,11 @@
       <c r="AU26"/>
       <c r="AV26"/>
       <c r="AW26"/>
+      <c r="AX26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B27" t="n">
         <v>1</v>
@@ -2883,30 +2922,31 @@
       </c>
       <c r="AH27"/>
       <c r="AI27"/>
-      <c r="AJ27" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK27"/>
+      <c r="AJ27"/>
+      <c r="AK27" t="n">
+        <v>1</v>
+      </c>
       <c r="AL27"/>
       <c r="AM27"/>
       <c r="AN27"/>
       <c r="AO27"/>
       <c r="AP27"/>
-      <c r="AQ27" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR27"/>
+      <c r="AQ27"/>
+      <c r="AR27" t="n">
+        <v>1</v>
+      </c>
       <c r="AS27"/>
       <c r="AT27"/>
       <c r="AU27"/>
       <c r="AV27"/>
-      <c r="AW27" t="n">
+      <c r="AW27"/>
+      <c r="AX27" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B28" t="n">
         <v>2</v>
@@ -2946,10 +2986,10 @@
       <c r="AE28"/>
       <c r="AF28"/>
       <c r="AG28"/>
-      <c r="AH28" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI28"/>
+      <c r="AH28"/>
+      <c r="AI28" t="n">
+        <v>1</v>
+      </c>
       <c r="AJ28"/>
       <c r="AK28"/>
       <c r="AL28"/>
@@ -2964,10 +3004,11 @@
       <c r="AU28"/>
       <c r="AV28"/>
       <c r="AW28"/>
+      <c r="AX28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B29" t="n">
         <v>4</v>
@@ -3035,46 +3076,47 @@
       <c r="AG29"/>
       <c r="AH29"/>
       <c r="AI29"/>
-      <c r="AJ29" t="n">
-        <v>1</v>
-      </c>
+      <c r="AJ29"/>
       <c r="AK29" t="n">
         <v>1</v>
       </c>
       <c r="AL29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM29" t="n">
         <v>10</v>
       </c>
-      <c r="AM29" t="n">
+      <c r="AN29" t="n">
         <v>8</v>
       </c>
-      <c r="AN29" t="n">
-        <v>2</v>
-      </c>
       <c r="AO29" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP29" t="n">
         <v>6</v>
       </c>
-      <c r="AP29" t="n">
-        <v>2</v>
-      </c>
       <c r="AQ29" t="n">
         <v>2</v>
       </c>
       <c r="AR29" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS29" t="n">
         <v>5</v>
       </c>
-      <c r="AS29"/>
       <c r="AT29"/>
       <c r="AU29"/>
-      <c r="AV29" t="n">
-        <v>3</v>
-      </c>
+      <c r="AV29"/>
       <c r="AW29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX29" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B30" t="n">
         <v>27</v>
@@ -3143,55 +3185,58 @@
       </c>
       <c r="AE30"/>
       <c r="AF30" t="n">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="AG30"/>
-      <c r="AH30"/>
-      <c r="AI30" t="n">
-        <v>3</v>
-      </c>
+      <c r="AH30" t="n">
+        <v>25</v>
+      </c>
+      <c r="AI30"/>
       <c r="AJ30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AK30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL30" t="n">
         <v>8</v>
       </c>
-      <c r="AL30" t="n">
+      <c r="AM30" t="n">
         <v>7</v>
       </c>
-      <c r="AM30" t="n">
+      <c r="AN30" t="n">
         <v>5</v>
       </c>
-      <c r="AN30" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO30"/>
-      <c r="AP30" t="n">
+      <c r="AO30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP30"/>
+      <c r="AQ30" t="n">
         <v>6</v>
       </c>
-      <c r="AQ30" t="n">
+      <c r="AR30" t="n">
         <v>5</v>
       </c>
-      <c r="AR30" t="n">
+      <c r="AS30" t="n">
         <v>7</v>
       </c>
-      <c r="AS30" t="n">
+      <c r="AT30" t="n">
         <v>4</v>
       </c>
-      <c r="AT30" t="n">
+      <c r="AU30" t="n">
         <v>5</v>
       </c>
-      <c r="AU30"/>
-      <c r="AV30" t="n">
+      <c r="AV30"/>
+      <c r="AW30" t="n">
         <v>20</v>
       </c>
-      <c r="AW30" t="n">
+      <c r="AX30" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B31" t="n">
         <v>110</v>
@@ -3258,16 +3303,14 @@
       </c>
       <c r="AG31"/>
       <c r="AH31"/>
-      <c r="AI31" t="n">
-        <v>1</v>
-      </c>
+      <c r="AI31"/>
       <c r="AJ31" t="n">
         <v>1</v>
       </c>
-      <c r="AK31"/>
-      <c r="AL31" t="n">
-        <v>3</v>
-      </c>
+      <c r="AK31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL31"/>
       <c r="AM31" t="n">
         <v>3</v>
       </c>
@@ -3275,34 +3318,37 @@
         <v>3</v>
       </c>
       <c r="AO31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP31" t="n">
         <v>6</v>
       </c>
-      <c r="AP31" t="n">
+      <c r="AQ31" t="n">
         <v>8</v>
       </c>
-      <c r="AQ31" t="n">
-        <v>3</v>
-      </c>
       <c r="AR31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS31" t="n">
         <v>9</v>
       </c>
-      <c r="AS31" t="n">
+      <c r="AT31" t="n">
         <v>4</v>
       </c>
-      <c r="AT31" t="n">
+      <c r="AU31" t="n">
         <v>8</v>
       </c>
-      <c r="AU31"/>
-      <c r="AV31" t="n">
+      <c r="AV31"/>
+      <c r="AW31" t="n">
         <v>17</v>
       </c>
-      <c r="AW31" t="n">
+      <c r="AX31" t="n">
         <v>57</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B32" t="n">
         <v>30</v>
@@ -3374,23 +3420,21 @@
       <c r="AG32" t="n">
         <v>1</v>
       </c>
-      <c r="AH32" t="n">
-        <v>1</v>
-      </c>
+      <c r="AH32"/>
       <c r="AI32" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ32" t="n">
         <v>8</v>
       </c>
-      <c r="AJ32" t="n">
-        <v>3</v>
-      </c>
       <c r="AK32" t="n">
         <v>3</v>
       </c>
       <c r="AL32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AM32" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AN32" t="n">
         <v>6</v>
@@ -3399,31 +3443,34 @@
         <v>6</v>
       </c>
       <c r="AP32" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AQ32" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR32" t="n">
         <v>4</v>
       </c>
-      <c r="AR32" t="n">
+      <c r="AS32" t="n">
         <v>14</v>
       </c>
-      <c r="AS32" t="n">
+      <c r="AT32" t="n">
         <v>8</v>
       </c>
-      <c r="AT32" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU32"/>
-      <c r="AV32" t="n">
+      <c r="AU32" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV32"/>
+      <c r="AW32" t="n">
         <v>7</v>
       </c>
-      <c r="AW32" t="n">
+      <c r="AX32" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
@@ -3477,10 +3524,11 @@
       <c r="AU33"/>
       <c r="AV33"/>
       <c r="AW33"/>
+      <c r="AX33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B34" t="n">
         <v>13</v>
@@ -3554,56 +3602,57 @@
         <v>75</v>
       </c>
       <c r="AG34"/>
-      <c r="AH34" t="n">
-        <v>2</v>
-      </c>
+      <c r="AH34"/>
       <c r="AI34" t="n">
         <v>2</v>
       </c>
       <c r="AJ34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AK34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AL34" t="n">
         <v>4</v>
       </c>
       <c r="AM34" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AN34" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO34" t="n">
         <v>4</v>
       </c>
-      <c r="AO34" t="n">
-        <v>1</v>
-      </c>
       <c r="AP34" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AQ34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AR34" t="n">
         <v>4</v>
       </c>
-      <c r="AR34" t="n">
+      <c r="AS34" t="n">
         <v>7</v>
       </c>
-      <c r="AS34" t="n">
+      <c r="AT34" t="n">
         <v>16</v>
       </c>
-      <c r="AT34" t="n">
+      <c r="AU34" t="n">
         <v>7</v>
       </c>
-      <c r="AU34"/>
-      <c r="AV34" t="n">
+      <c r="AV34"/>
+      <c r="AW34" t="n">
         <v>24</v>
       </c>
-      <c r="AW34" t="n">
+      <c r="AX34" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B35"/>
       <c r="C35"/>
@@ -3655,34 +3704,35 @@
       <c r="AG35"/>
       <c r="AH35"/>
       <c r="AI35"/>
-      <c r="AJ35" t="n">
-        <v>2</v>
-      </c>
-      <c r="AK35"/>
+      <c r="AJ35"/>
+      <c r="AK35" t="n">
+        <v>2</v>
+      </c>
       <c r="AL35"/>
       <c r="AM35"/>
-      <c r="AN35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO35"/>
-      <c r="AP35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ35"/>
+      <c r="AN35"/>
+      <c r="AO35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP35"/>
+      <c r="AQ35" t="n">
+        <v>1</v>
+      </c>
       <c r="AR35"/>
-      <c r="AS35" t="n">
-        <v>1</v>
-      </c>
+      <c r="AS35"/>
       <c r="AT35" t="n">
         <v>1</v>
       </c>
-      <c r="AU35"/>
+      <c r="AU35" t="n">
+        <v>1</v>
+      </c>
       <c r="AV35"/>
       <c r="AW35"/>
+      <c r="AX35"/>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B36"/>
       <c r="C36"/>
@@ -3739,41 +3789,44 @@
       </c>
       <c r="AG36"/>
       <c r="AH36" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI36"/>
+        <v>18</v>
+      </c>
+      <c r="AI36" t="n">
+        <v>1</v>
+      </c>
       <c r="AJ36"/>
-      <c r="AK36" t="n">
-        <v>1</v>
-      </c>
+      <c r="AK36"/>
       <c r="AL36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AM36" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN36"/>
-      <c r="AO36" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP36"/>
-      <c r="AQ36" t="n">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AN36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO36"/>
+      <c r="AP36" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ36"/>
       <c r="AR36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS36" t="n">
         <v>5</v>
       </c>
-      <c r="AS36" t="n">
-        <v>3</v>
-      </c>
       <c r="AT36" t="n">
         <v>3</v>
       </c>
-      <c r="AU36"/>
-      <c r="AV36" t="n">
-        <v>1</v>
-      </c>
+      <c r="AU36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV36"/>
       <c r="AW36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX36" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
17th April 2nd update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/state/ncov19state_long.xlsx
+++ b/covid19_data/excel/state/ncov19state_long.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t xml:space="preserve">detectedstate</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t xml:space="preserve">17/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">18/03/2020</t>
@@ -749,10 +752,13 @@
       <c r="AX1" t="s">
         <v>49</v>
       </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
@@ -805,10 +811,11 @@
       <c r="AV2"/>
       <c r="AW2"/>
       <c r="AX2"/>
+      <c r="AY2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -846,7 +853,9 @@
       <c r="AG3"/>
       <c r="AH3"/>
       <c r="AI3"/>
-      <c r="AJ3"/>
+      <c r="AJ3" t="n">
+        <v>1</v>
+      </c>
       <c r="AK3"/>
       <c r="AL3"/>
       <c r="AM3"/>
@@ -854,25 +863,26 @@
       <c r="AO3"/>
       <c r="AP3"/>
       <c r="AQ3"/>
-      <c r="AR3" t="n">
-        <v>1</v>
-      </c>
+      <c r="AR3"/>
       <c r="AS3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT3" t="n">
         <v>5</v>
       </c>
-      <c r="AT3" t="n">
-        <v>3</v>
-      </c>
-      <c r="AU3"/>
+      <c r="AU3" t="n">
+        <v>3</v>
+      </c>
       <c r="AV3"/>
-      <c r="AW3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX3"/>
+      <c r="AW3"/>
+      <c r="AX3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="n">
         <v>67</v>
@@ -942,16 +952,16 @@
         <v>9</v>
       </c>
       <c r="AI4"/>
-      <c r="AJ4"/>
-      <c r="AK4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL4"/>
-      <c r="AM4" t="n">
-        <v>2</v>
-      </c>
+      <c r="AJ4" t="n">
+        <v>38</v>
+      </c>
+      <c r="AK4"/>
+      <c r="AL4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM4"/>
       <c r="AN4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO4" t="n">
         <v>1</v>
@@ -960,31 +970,34 @@
         <v>1</v>
       </c>
       <c r="AQ4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AS4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU4" t="n">
         <v>6</v>
       </c>
-      <c r="AU4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AV4"/>
-      <c r="AW4" t="n">
-        <v>2</v>
-      </c>
+      <c r="AV4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AW4"/>
       <c r="AX4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AY4" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -1037,10 +1050,11 @@
       <c r="AV5"/>
       <c r="AW5"/>
       <c r="AX5"/>
+      <c r="AY5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B6" t="n">
         <v>15</v>
@@ -1106,13 +1120,14 @@
       <c r="AU6"/>
       <c r="AV6"/>
       <c r="AW6"/>
-      <c r="AX6" t="n">
+      <c r="AX6"/>
+      <c r="AY6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -1169,44 +1184,45 @@
       </c>
       <c r="AG7"/>
       <c r="AH7" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="AI7"/>
       <c r="AJ7"/>
       <c r="AK7"/>
       <c r="AL7"/>
       <c r="AM7"/>
-      <c r="AN7" t="n">
-        <v>2</v>
-      </c>
+      <c r="AN7"/>
       <c r="AO7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP7"/>
-      <c r="AQ7" t="n">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ7"/>
       <c r="AR7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AS7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AT7" t="n">
         <v>2</v>
       </c>
       <c r="AU7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV7" t="n">
         <v>4</v>
       </c>
-      <c r="AV7"/>
       <c r="AW7"/>
-      <c r="AX7" t="n">
+      <c r="AX7"/>
+      <c r="AY7" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -1251,38 +1267,39 @@
       <c r="AH8"/>
       <c r="AI8"/>
       <c r="AJ8"/>
-      <c r="AK8" t="n">
-        <v>1</v>
-      </c>
+      <c r="AK8"/>
       <c r="AL8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM8" t="n">
         <v>4</v>
       </c>
-      <c r="AM8"/>
-      <c r="AN8" t="n">
-        <v>1</v>
-      </c>
+      <c r="AN8"/>
       <c r="AO8" t="n">
         <v>1</v>
       </c>
-      <c r="AP8"/>
+      <c r="AP8" t="n">
+        <v>1</v>
+      </c>
       <c r="AQ8"/>
       <c r="AR8"/>
-      <c r="AS8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT8"/>
+      <c r="AS8"/>
+      <c r="AT8" t="n">
+        <v>1</v>
+      </c>
       <c r="AU8"/>
       <c r="AV8"/>
-      <c r="AW8" t="n">
+      <c r="AW8"/>
+      <c r="AX8" t="n">
         <v>5</v>
       </c>
-      <c r="AX8" t="n">
+      <c r="AY8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -1326,39 +1343,42 @@
       <c r="AE9"/>
       <c r="AF9"/>
       <c r="AG9"/>
-      <c r="AH9"/>
+      <c r="AH9" t="n">
+        <v>3</v>
+      </c>
       <c r="AI9"/>
       <c r="AJ9"/>
-      <c r="AK9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL9"/>
+      <c r="AK9"/>
+      <c r="AL9" t="n">
+        <v>1</v>
+      </c>
       <c r="AM9"/>
       <c r="AN9"/>
       <c r="AO9"/>
       <c r="AP9"/>
-      <c r="AQ9" t="n">
-        <v>2</v>
-      </c>
+      <c r="AQ9"/>
       <c r="AR9" t="n">
-        <v>3</v>
-      </c>
-      <c r="AS9"/>
-      <c r="AT9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU9"/>
+        <v>2</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT9"/>
+      <c r="AU9" t="n">
+        <v>1</v>
+      </c>
       <c r="AV9"/>
-      <c r="AW9" t="n">
-        <v>1</v>
-      </c>
+      <c r="AW9"/>
       <c r="AX9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B10"/>
       <c r="C10"/>
@@ -1411,10 +1431,11 @@
       <c r="AV10"/>
       <c r="AW10"/>
       <c r="AX10"/>
+      <c r="AY10"/>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B11" t="n">
         <v>32</v>
@@ -1492,55 +1513,58 @@
         <v>17</v>
       </c>
       <c r="AG11"/>
-      <c r="AH11"/>
+      <c r="AH11" t="n">
+        <v>62</v>
+      </c>
       <c r="AI11" t="n">
         <v>3</v>
       </c>
-      <c r="AJ11" t="n">
-        <v>1</v>
-      </c>
+      <c r="AJ11"/>
       <c r="AK11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AL11" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM11" t="n">
         <v>6</v>
       </c>
-      <c r="AM11" t="n">
+      <c r="AN11" t="n">
         <v>7</v>
       </c>
-      <c r="AN11" t="n">
-        <v>1</v>
-      </c>
       <c r="AO11" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP11"/>
-      <c r="AQ11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ11"/>
+      <c r="AR11" t="n">
         <v>5</v>
       </c>
-      <c r="AR11" t="n">
+      <c r="AS11" t="n">
         <v>4</v>
       </c>
-      <c r="AS11" t="n">
-        <v>1</v>
-      </c>
       <c r="AT11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU11" t="n">
         <v>9</v>
       </c>
-      <c r="AU11" t="n">
+      <c r="AV11" t="n">
         <v>23</v>
       </c>
-      <c r="AV11"/>
-      <c r="AW11" t="n">
+      <c r="AW11"/>
+      <c r="AX11" t="n">
         <v>25</v>
       </c>
-      <c r="AX11" t="n">
+      <c r="AY11" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B12"/>
       <c r="C12"/>
@@ -1587,22 +1611,23 @@
       <c r="AN12"/>
       <c r="AO12"/>
       <c r="AP12"/>
-      <c r="AQ12" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR12"/>
+      <c r="AQ12"/>
+      <c r="AR12" t="n">
+        <v>3</v>
+      </c>
       <c r="AS12"/>
       <c r="AT12"/>
-      <c r="AU12" t="n">
-        <v>2</v>
-      </c>
-      <c r="AV12"/>
+      <c r="AU12"/>
+      <c r="AV12" t="n">
+        <v>2</v>
+      </c>
       <c r="AW12"/>
       <c r="AX12"/>
+      <c r="AY12"/>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B13" t="n">
         <v>13</v>
@@ -1667,54 +1692,57 @@
       </c>
       <c r="AG13"/>
       <c r="AH13" t="n">
-        <v>105</v>
+        <v>163</v>
       </c>
       <c r="AI13"/>
-      <c r="AJ13"/>
-      <c r="AK13" t="n">
-        <v>2</v>
-      </c>
+      <c r="AJ13" t="n">
+        <v>92</v>
+      </c>
+      <c r="AK13"/>
       <c r="AL13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM13" t="n">
         <v>5</v>
       </c>
-      <c r="AM13" t="n">
+      <c r="AN13" t="n">
         <v>7</v>
       </c>
-      <c r="AN13" t="n">
+      <c r="AO13" t="n">
         <v>4</v>
       </c>
-      <c r="AO13" t="n">
+      <c r="AP13" t="n">
         <v>12</v>
       </c>
-      <c r="AP13" t="n">
+      <c r="AQ13" t="n">
         <v>6</v>
       </c>
-      <c r="AQ13" t="n">
-        <v>2</v>
-      </c>
       <c r="AR13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS13" t="n">
         <v>6</v>
       </c>
-      <c r="AS13" t="n">
-        <v>3</v>
-      </c>
       <c r="AT13" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AU13" t="n">
         <v>8</v>
       </c>
-      <c r="AV13"/>
-      <c r="AW13" t="n">
+      <c r="AV13" t="n">
+        <v>8</v>
+      </c>
+      <c r="AW13"/>
+      <c r="AX13" t="n">
         <v>7</v>
       </c>
-      <c r="AX13" t="n">
+      <c r="AY13" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -1784,25 +1812,23 @@
       <c r="AI14" t="n">
         <v>1</v>
       </c>
-      <c r="AJ14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AK14"/>
-      <c r="AL14" t="n">
-        <v>2</v>
-      </c>
+      <c r="AJ14"/>
+      <c r="AK14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL14"/>
       <c r="AM14" t="n">
         <v>2</v>
       </c>
-      <c r="AN14"/>
-      <c r="AO14" t="n">
+      <c r="AN14" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO14"/>
+      <c r="AP14" t="n">
         <v>7</v>
       </c>
-      <c r="AP14" t="n">
-        <v>2</v>
-      </c>
       <c r="AQ14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AR14" t="n">
         <v>1</v>
@@ -1811,20 +1837,23 @@
         <v>1</v>
       </c>
       <c r="AT14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AU14"/>
+        <v>1</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>2</v>
+      </c>
       <c r="AV14"/>
-      <c r="AW14" t="n">
-        <v>1</v>
-      </c>
+      <c r="AW14"/>
       <c r="AX14" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY14" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -1880,15 +1909,15 @@
       <c r="AI15"/>
       <c r="AJ15"/>
       <c r="AK15"/>
-      <c r="AL15" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM15"/>
+      <c r="AL15"/>
+      <c r="AM15" t="n">
+        <v>2</v>
+      </c>
       <c r="AN15"/>
-      <c r="AO15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP15"/>
+      <c r="AO15"/>
+      <c r="AP15" t="n">
+        <v>1</v>
+      </c>
       <c r="AQ15"/>
       <c r="AR15"/>
       <c r="AS15"/>
@@ -1897,10 +1926,11 @@
       <c r="AV15"/>
       <c r="AW15"/>
       <c r="AX15"/>
+      <c r="AY15"/>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B16" t="n">
         <v>7</v>
@@ -1974,43 +2004,44 @@
         <v>14</v>
       </c>
       <c r="AI16"/>
-      <c r="AJ16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK16"/>
+      <c r="AJ16"/>
+      <c r="AK16" t="n">
+        <v>1</v>
+      </c>
       <c r="AL16"/>
       <c r="AM16"/>
       <c r="AN16"/>
       <c r="AO16"/>
-      <c r="AP16" t="n">
-        <v>2</v>
-      </c>
+      <c r="AP16"/>
       <c r="AQ16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR16" t="n">
         <v>5</v>
       </c>
-      <c r="AR16" t="n">
-        <v>3</v>
-      </c>
       <c r="AS16" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT16" t="n">
         <v>6</v>
       </c>
-      <c r="AT16" t="n">
+      <c r="AU16" t="n">
         <v>13</v>
       </c>
-      <c r="AU16" t="n">
+      <c r="AV16" t="n">
         <v>5</v>
       </c>
-      <c r="AV16"/>
-      <c r="AW16" t="n">
+      <c r="AW16"/>
+      <c r="AX16" t="n">
         <v>11</v>
       </c>
-      <c r="AX16" t="n">
+      <c r="AY16" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B17"/>
       <c r="C17"/>
@@ -2082,13 +2113,14 @@
       <c r="AU17"/>
       <c r="AV17"/>
       <c r="AW17"/>
-      <c r="AX17" t="n">
+      <c r="AX17"/>
+      <c r="AY17" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B18" t="n">
         <v>9</v>
@@ -2169,50 +2201,53 @@
         <v>4</v>
       </c>
       <c r="AJ18" t="n">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="AK18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL18"/>
-      <c r="AM18" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM18"/>
+      <c r="AN18" t="n">
         <v>5</v>
       </c>
-      <c r="AN18" t="n">
+      <c r="AO18" t="n">
         <v>6</v>
       </c>
-      <c r="AO18" t="n">
+      <c r="AP18" t="n">
         <v>7</v>
       </c>
-      <c r="AP18" t="n">
+      <c r="AQ18" t="n">
         <v>8</v>
       </c>
-      <c r="AQ18" t="n">
+      <c r="AR18" t="n">
         <v>10</v>
       </c>
-      <c r="AR18" t="n">
+      <c r="AS18" t="n">
         <v>4</v>
       </c>
-      <c r="AS18" t="n">
+      <c r="AT18" t="n">
         <v>9</v>
       </c>
-      <c r="AT18" t="n">
+      <c r="AU18" t="n">
         <v>12</v>
       </c>
-      <c r="AU18" t="n">
+      <c r="AV18" t="n">
         <v>7</v>
       </c>
-      <c r="AV18"/>
-      <c r="AW18" t="n">
+      <c r="AW18"/>
+      <c r="AX18" t="n">
         <v>5</v>
       </c>
-      <c r="AX18" t="n">
+      <c r="AY18" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B19" t="n">
         <v>24</v>
@@ -2299,52 +2334,53 @@
       </c>
       <c r="AI19"/>
       <c r="AJ19"/>
-      <c r="AK19" t="n">
-        <v>1</v>
-      </c>
+      <c r="AK19"/>
       <c r="AL19" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="AM19" t="n">
         <v>12</v>
       </c>
       <c r="AN19" t="n">
+        <v>12</v>
+      </c>
+      <c r="AO19" t="n">
         <v>15</v>
       </c>
-      <c r="AO19" t="n">
+      <c r="AP19" t="n">
         <v>28</v>
       </c>
-      <c r="AP19" t="n">
+      <c r="AQ19" t="n">
         <v>14</v>
       </c>
-      <c r="AQ19" t="n">
+      <c r="AR19" t="n">
         <v>9</v>
       </c>
-      <c r="AR19" t="n">
+      <c r="AS19" t="n">
         <v>19</v>
       </c>
-      <c r="AS19" t="n">
+      <c r="AT19" t="n">
         <v>39</v>
       </c>
-      <c r="AT19" t="n">
+      <c r="AU19" t="n">
         <v>6</v>
       </c>
-      <c r="AU19" t="n">
+      <c r="AV19" t="n">
         <v>20</v>
       </c>
-      <c r="AV19" t="n">
-        <v>1</v>
-      </c>
       <c r="AW19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX19" t="n">
         <v>32</v>
       </c>
-      <c r="AX19" t="n">
+      <c r="AY19" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B20"/>
       <c r="C20"/>
@@ -2396,13 +2432,13 @@
       </c>
       <c r="AJ20"/>
       <c r="AK20"/>
-      <c r="AL20" t="n">
-        <v>2</v>
-      </c>
+      <c r="AL20"/>
       <c r="AM20" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN20"/>
+        <v>2</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>3</v>
+      </c>
       <c r="AO20"/>
       <c r="AP20"/>
       <c r="AQ20"/>
@@ -2413,10 +2449,11 @@
       <c r="AV20"/>
       <c r="AW20"/>
       <c r="AX20"/>
+      <c r="AY20"/>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B21" t="n">
         <v>32</v>
@@ -2481,46 +2518,47 @@
       </c>
       <c r="AG21"/>
       <c r="AH21" t="n">
-        <v>182</v>
+        <v>226</v>
       </c>
       <c r="AI21"/>
       <c r="AJ21"/>
       <c r="AK21"/>
-      <c r="AL21" t="n">
+      <c r="AL21"/>
+      <c r="AM21" t="n">
         <v>4</v>
       </c>
-      <c r="AM21"/>
-      <c r="AN21" t="n">
-        <v>2</v>
-      </c>
-      <c r="AO21"/>
-      <c r="AP21" t="n">
-        <v>1</v>
-      </c>
+      <c r="AN21"/>
+      <c r="AO21" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP21"/>
       <c r="AQ21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR21" t="n">
         <v>8</v>
       </c>
-      <c r="AR21" t="n">
+      <c r="AS21" t="n">
         <v>5</v>
       </c>
-      <c r="AS21" t="n">
+      <c r="AT21" t="n">
         <v>9</v>
       </c>
-      <c r="AT21" t="n">
+      <c r="AU21" t="n">
         <v>10</v>
       </c>
-      <c r="AU21"/>
       <c r="AV21"/>
-      <c r="AW21" t="n">
+      <c r="AW21"/>
+      <c r="AX21" t="n">
         <v>8</v>
       </c>
-      <c r="AX21" t="n">
+      <c r="AY21" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B22" t="n">
         <v>33</v>
@@ -2601,58 +2639,59 @@
         <v>7</v>
       </c>
       <c r="AH22" t="n">
-        <v>165</v>
+        <v>286</v>
       </c>
       <c r="AI22" t="n">
         <v>2</v>
       </c>
-      <c r="AJ22" t="n">
+      <c r="AJ22"/>
+      <c r="AK22" t="n">
         <v>4</v>
       </c>
-      <c r="AK22" t="n">
-        <v>3</v>
-      </c>
       <c r="AL22" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM22" t="n">
         <v>4</v>
       </c>
-      <c r="AM22" t="n">
+      <c r="AN22" t="n">
         <v>12</v>
       </c>
-      <c r="AN22" t="n">
+      <c r="AO22" t="n">
         <v>10</v>
       </c>
-      <c r="AO22" t="n">
+      <c r="AP22" t="n">
         <v>15</v>
       </c>
-      <c r="AP22" t="n">
+      <c r="AQ22" t="n">
         <v>18</v>
       </c>
-      <c r="AQ22" t="n">
+      <c r="AR22" t="n">
         <v>15</v>
       </c>
-      <c r="AR22" t="n">
-        <v>3</v>
-      </c>
       <c r="AS22" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="AT22" t="n">
         <v>28</v>
       </c>
       <c r="AU22" t="n">
+        <v>28</v>
+      </c>
+      <c r="AV22" t="n">
         <v>22</v>
       </c>
-      <c r="AV22"/>
-      <c r="AW22" t="n">
+      <c r="AW22"/>
+      <c r="AX22" t="n">
         <v>17</v>
       </c>
-      <c r="AX22" t="n">
+      <c r="AY22" t="n">
         <v>82</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -2696,10 +2735,10 @@
       <c r="AM23"/>
       <c r="AN23"/>
       <c r="AO23"/>
-      <c r="AP23" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ23"/>
+      <c r="AP23"/>
+      <c r="AQ23" t="n">
+        <v>1</v>
+      </c>
       <c r="AR23"/>
       <c r="AS23"/>
       <c r="AT23"/>
@@ -2707,10 +2746,11 @@
       <c r="AV23"/>
       <c r="AW23"/>
       <c r="AX23"/>
+      <c r="AY23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -2748,7 +2788,9 @@
         <v>6</v>
       </c>
       <c r="AG24"/>
-      <c r="AH24"/>
+      <c r="AH24" t="n">
+        <v>2</v>
+      </c>
       <c r="AI24"/>
       <c r="AJ24"/>
       <c r="AK24"/>
@@ -2765,10 +2807,11 @@
       <c r="AV24"/>
       <c r="AW24"/>
       <c r="AX24"/>
+      <c r="AY24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -2811,20 +2854,21 @@
       <c r="AN25"/>
       <c r="AO25"/>
       <c r="AP25"/>
-      <c r="AQ25" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR25"/>
+      <c r="AQ25"/>
+      <c r="AR25" t="n">
+        <v>1</v>
+      </c>
       <c r="AS25"/>
       <c r="AT25"/>
       <c r="AU25"/>
       <c r="AV25"/>
       <c r="AW25"/>
       <c r="AX25"/>
+      <c r="AY25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B26"/>
       <c r="C26"/>
@@ -2877,10 +2921,11 @@
       <c r="AV26"/>
       <c r="AW26"/>
       <c r="AX26"/>
+      <c r="AY26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B27" t="n">
         <v>1</v>
@@ -2941,30 +2986,31 @@
       <c r="AH27"/>
       <c r="AI27"/>
       <c r="AJ27"/>
-      <c r="AK27" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL27"/>
+      <c r="AK27"/>
+      <c r="AL27" t="n">
+        <v>1</v>
+      </c>
       <c r="AM27"/>
       <c r="AN27"/>
       <c r="AO27"/>
       <c r="AP27"/>
       <c r="AQ27"/>
-      <c r="AR27" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS27"/>
+      <c r="AR27"/>
+      <c r="AS27" t="n">
+        <v>1</v>
+      </c>
       <c r="AT27"/>
       <c r="AU27"/>
       <c r="AV27"/>
       <c r="AW27"/>
-      <c r="AX27" t="n">
+      <c r="AX27"/>
+      <c r="AY27" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B28" t="n">
         <v>2</v>
@@ -3023,10 +3069,11 @@
       <c r="AV28"/>
       <c r="AW28"/>
       <c r="AX28"/>
+      <c r="AY28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B29" t="n">
         <v>4</v>
@@ -3097,46 +3144,47 @@
       </c>
       <c r="AI29"/>
       <c r="AJ29"/>
-      <c r="AK29" t="n">
-        <v>1</v>
-      </c>
+      <c r="AK29"/>
       <c r="AL29" t="n">
         <v>1</v>
       </c>
       <c r="AM29" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN29" t="n">
         <v>10</v>
       </c>
-      <c r="AN29" t="n">
+      <c r="AO29" t="n">
         <v>8</v>
       </c>
-      <c r="AO29" t="n">
-        <v>2</v>
-      </c>
       <c r="AP29" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ29" t="n">
         <v>6</v>
       </c>
-      <c r="AQ29" t="n">
-        <v>2</v>
-      </c>
       <c r="AR29" t="n">
         <v>2</v>
       </c>
       <c r="AS29" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT29" t="n">
         <v>5</v>
       </c>
-      <c r="AT29"/>
       <c r="AU29"/>
       <c r="AV29"/>
-      <c r="AW29" t="n">
-        <v>3</v>
-      </c>
+      <c r="AW29"/>
       <c r="AX29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY29" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B30" t="n">
         <v>27</v>
@@ -3209,54 +3257,57 @@
       </c>
       <c r="AG30"/>
       <c r="AH30" t="n">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="AI30"/>
       <c r="AJ30" t="n">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="AK30" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM30" t="n">
         <v>8</v>
       </c>
-      <c r="AM30" t="n">
+      <c r="AN30" t="n">
         <v>7</v>
       </c>
-      <c r="AN30" t="n">
+      <c r="AO30" t="n">
         <v>5</v>
       </c>
-      <c r="AO30" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP30"/>
-      <c r="AQ30" t="n">
+      <c r="AP30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ30"/>
+      <c r="AR30" t="n">
         <v>6</v>
       </c>
-      <c r="AR30" t="n">
+      <c r="AS30" t="n">
         <v>5</v>
       </c>
-      <c r="AS30" t="n">
+      <c r="AT30" t="n">
         <v>7</v>
       </c>
-      <c r="AT30" t="n">
+      <c r="AU30" t="n">
         <v>4</v>
       </c>
-      <c r="AU30" t="n">
+      <c r="AV30" t="n">
         <v>5</v>
       </c>
-      <c r="AV30"/>
-      <c r="AW30" t="n">
+      <c r="AW30"/>
+      <c r="AX30" t="n">
         <v>20</v>
       </c>
-      <c r="AX30" t="n">
+      <c r="AY30" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B31" t="n">
         <v>110</v>
@@ -3326,16 +3377,14 @@
         <v>25</v>
       </c>
       <c r="AI31"/>
-      <c r="AJ31" t="n">
-        <v>1</v>
-      </c>
+      <c r="AJ31"/>
       <c r="AK31" t="n">
         <v>1</v>
       </c>
-      <c r="AL31"/>
-      <c r="AM31" t="n">
-        <v>3</v>
-      </c>
+      <c r="AL31" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM31"/>
       <c r="AN31" t="n">
         <v>3</v>
       </c>
@@ -3343,34 +3392,37 @@
         <v>3</v>
       </c>
       <c r="AP31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ31" t="n">
         <v>6</v>
       </c>
-      <c r="AQ31" t="n">
+      <c r="AR31" t="n">
         <v>8</v>
       </c>
-      <c r="AR31" t="n">
-        <v>3</v>
-      </c>
       <c r="AS31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT31" t="n">
         <v>9</v>
       </c>
-      <c r="AT31" t="n">
+      <c r="AU31" t="n">
         <v>4</v>
       </c>
-      <c r="AU31" t="n">
+      <c r="AV31" t="n">
         <v>8</v>
       </c>
-      <c r="AV31"/>
-      <c r="AW31" t="n">
+      <c r="AW31"/>
+      <c r="AX31" t="n">
         <v>17</v>
       </c>
-      <c r="AX31" t="n">
+      <c r="AY31" t="n">
         <v>57</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B32" t="n">
         <v>30</v>
@@ -3442,24 +3494,24 @@
       <c r="AG32" t="n">
         <v>1</v>
       </c>
-      <c r="AH32"/>
+      <c r="AH32" t="n">
+        <v>50</v>
+      </c>
       <c r="AI32" t="n">
         <v>1</v>
       </c>
-      <c r="AJ32" t="n">
+      <c r="AJ32"/>
+      <c r="AK32" t="n">
         <v>8</v>
       </c>
-      <c r="AK32" t="n">
-        <v>3</v>
-      </c>
       <c r="AL32" t="n">
         <v>3</v>
       </c>
       <c r="AM32" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AN32" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AO32" t="n">
         <v>6</v>
@@ -3468,31 +3520,34 @@
         <v>6</v>
       </c>
       <c r="AQ32" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AR32" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS32" t="n">
         <v>4</v>
       </c>
-      <c r="AS32" t="n">
+      <c r="AT32" t="n">
         <v>14</v>
       </c>
-      <c r="AT32" t="n">
+      <c r="AU32" t="n">
         <v>8</v>
       </c>
-      <c r="AU32" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV32"/>
-      <c r="AW32" t="n">
+      <c r="AV32" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW32"/>
+      <c r="AX32" t="n">
         <v>7</v>
       </c>
-      <c r="AX32" t="n">
+      <c r="AY32" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
@@ -3547,10 +3602,11 @@
       <c r="AV33"/>
       <c r="AW33"/>
       <c r="AX33"/>
+      <c r="AY33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B34" t="n">
         <v>13</v>
@@ -3625,58 +3681,59 @@
       </c>
       <c r="AG34"/>
       <c r="AH34" t="n">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="AI34" t="n">
         <v>2</v>
       </c>
-      <c r="AJ34" t="n">
-        <v>2</v>
-      </c>
+      <c r="AJ34"/>
       <c r="AK34" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AL34" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AM34" t="n">
         <v>4</v>
       </c>
       <c r="AN34" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AO34" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP34" t="n">
         <v>4</v>
       </c>
-      <c r="AP34" t="n">
-        <v>1</v>
-      </c>
       <c r="AQ34" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AR34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS34" t="n">
         <v>4</v>
       </c>
-      <c r="AS34" t="n">
+      <c r="AT34" t="n">
         <v>7</v>
       </c>
-      <c r="AT34" t="n">
+      <c r="AU34" t="n">
         <v>16</v>
       </c>
-      <c r="AU34" t="n">
+      <c r="AV34" t="n">
         <v>7</v>
       </c>
-      <c r="AV34"/>
-      <c r="AW34" t="n">
+      <c r="AW34"/>
+      <c r="AX34" t="n">
         <v>24</v>
       </c>
-      <c r="AX34" t="n">
+      <c r="AY34" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B35"/>
       <c r="C35"/>
@@ -3729,34 +3786,35 @@
       <c r="AH35"/>
       <c r="AI35"/>
       <c r="AJ35"/>
-      <c r="AK35" t="n">
-        <v>2</v>
-      </c>
-      <c r="AL35"/>
+      <c r="AK35"/>
+      <c r="AL35" t="n">
+        <v>2</v>
+      </c>
       <c r="AM35"/>
       <c r="AN35"/>
-      <c r="AO35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP35"/>
-      <c r="AQ35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR35"/>
+      <c r="AO35"/>
+      <c r="AP35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ35"/>
+      <c r="AR35" t="n">
+        <v>1</v>
+      </c>
       <c r="AS35"/>
-      <c r="AT35" t="n">
-        <v>1</v>
-      </c>
+      <c r="AT35"/>
       <c r="AU35" t="n">
         <v>1</v>
       </c>
-      <c r="AV35"/>
+      <c r="AV35" t="n">
+        <v>1</v>
+      </c>
       <c r="AW35"/>
       <c r="AX35"/>
+      <c r="AY35"/>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B36"/>
       <c r="C36"/>
@@ -3818,39 +3876,42 @@
       <c r="AI36" t="n">
         <v>1</v>
       </c>
-      <c r="AJ36"/>
+      <c r="AJ36" t="n">
+        <v>24</v>
+      </c>
       <c r="AK36"/>
-      <c r="AL36" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL36"/>
       <c r="AM36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN36" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO36"/>
-      <c r="AP36" t="n">
-        <v>2</v>
-      </c>
-      <c r="AQ36"/>
-      <c r="AR36" t="n">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AO36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP36"/>
+      <c r="AQ36" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR36"/>
       <c r="AS36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT36" t="n">
         <v>5</v>
       </c>
-      <c r="AT36" t="n">
-        <v>3</v>
-      </c>
       <c r="AU36" t="n">
         <v>3</v>
       </c>
-      <c r="AV36"/>
-      <c r="AW36" t="n">
-        <v>1</v>
-      </c>
+      <c r="AV36" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW36"/>
       <c r="AX36" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY36" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
17th April 3rd update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/state/ncov19state_long.xlsx
+++ b/covid19_data/excel/state/ncov19state_long.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t xml:space="preserve">detectedstate</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t xml:space="preserve">Chhattisgarh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dadra and Nagar Haveli</t>
   </si>
   <si>
     <t xml:space="preserve">Delhi</t>
@@ -772,7 +769,9 @@
       <c r="K2"/>
       <c r="L2"/>
       <c r="M2"/>
-      <c r="N2"/>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
       <c r="O2"/>
       <c r="P2" t="n">
         <v>1</v>
@@ -1380,364 +1379,420 @@
       <c r="A10" t="s">
         <v>59</v>
       </c>
-      <c r="B10"/>
+      <c r="B10" t="n">
+        <v>32</v>
+      </c>
       <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>141</v>
+      </c>
       <c r="F10"/>
       <c r="G10"/>
-      <c r="H10"/>
+      <c r="H10" t="n">
+        <v>93</v>
+      </c>
       <c r="I10"/>
-      <c r="J10"/>
-      <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
+      <c r="J10" t="n">
+        <v>59</v>
+      </c>
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>58</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1</v>
+      </c>
       <c r="N10" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="O10"/>
-      <c r="P10"/>
+      <c r="P10" t="n">
+        <v>51</v>
+      </c>
       <c r="Q10"/>
-      <c r="R10"/>
-      <c r="S10"/>
-      <c r="T10"/>
+      <c r="R10" t="n">
+        <v>93</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1</v>
+      </c>
+      <c r="T10" t="n">
+        <v>51</v>
+      </c>
       <c r="U10"/>
-      <c r="V10"/>
-      <c r="W10"/>
-      <c r="X10"/>
-      <c r="Y10"/>
-      <c r="Z10"/>
-      <c r="AA10"/>
-      <c r="AB10"/>
+      <c r="V10" t="n">
+        <v>183</v>
+      </c>
+      <c r="W10" t="n">
+        <v>1</v>
+      </c>
+      <c r="X10" t="n">
+        <v>166</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>85</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>356</v>
+      </c>
       <c r="AC10"/>
-      <c r="AD10"/>
+      <c r="AD10" t="n">
+        <v>51</v>
+      </c>
       <c r="AE10"/>
-      <c r="AF10"/>
+      <c r="AF10" t="n">
+        <v>17</v>
+      </c>
       <c r="AG10"/>
-      <c r="AH10"/>
-      <c r="AI10"/>
+      <c r="AH10" t="n">
+        <v>62</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>3</v>
+      </c>
       <c r="AJ10"/>
-      <c r="AK10"/>
-      <c r="AL10"/>
-      <c r="AM10"/>
-      <c r="AN10"/>
-      <c r="AO10"/>
-      <c r="AP10"/>
+      <c r="AK10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>6</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>7</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>2</v>
+      </c>
       <c r="AQ10"/>
-      <c r="AR10"/>
-      <c r="AS10"/>
-      <c r="AT10"/>
-      <c r="AU10"/>
-      <c r="AV10"/>
+      <c r="AR10" t="n">
+        <v>5</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>9</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>23</v>
+      </c>
       <c r="AW10"/>
-      <c r="AX10"/>
-      <c r="AY10"/>
+      <c r="AX10" t="n">
+        <v>25</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>60</v>
       </c>
-      <c r="B11" t="n">
-        <v>32</v>
-      </c>
+      <c r="B11"/>
       <c r="C11"/>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="n">
-        <v>141</v>
-      </c>
+      <c r="D11"/>
+      <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11" t="n">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="I11"/>
       <c r="J11" t="n">
-        <v>59</v>
-      </c>
-      <c r="K11" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" t="n">
-        <v>58</v>
-      </c>
-      <c r="M11" t="n">
-        <v>1</v>
-      </c>
-      <c r="N11" t="n">
-        <v>22</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
       <c r="O11"/>
-      <c r="P11" t="n">
-        <v>51</v>
-      </c>
+      <c r="P11"/>
       <c r="Q11"/>
-      <c r="R11" t="n">
-        <v>93</v>
-      </c>
-      <c r="S11" t="n">
-        <v>1</v>
-      </c>
-      <c r="T11" t="n">
-        <v>51</v>
-      </c>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
       <c r="U11"/>
-      <c r="V11" t="n">
-        <v>183</v>
-      </c>
-      <c r="W11" t="n">
-        <v>1</v>
-      </c>
-      <c r="X11" t="n">
-        <v>166</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>85</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>356</v>
-      </c>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+      <c r="Z11"/>
+      <c r="AA11"/>
+      <c r="AB11"/>
       <c r="AC11"/>
-      <c r="AD11" t="n">
-        <v>51</v>
-      </c>
+      <c r="AD11"/>
       <c r="AE11"/>
-      <c r="AF11" t="n">
-        <v>17</v>
-      </c>
+      <c r="AF11"/>
       <c r="AG11"/>
-      <c r="AH11" t="n">
-        <v>62</v>
-      </c>
-      <c r="AI11" t="n">
-        <v>3</v>
-      </c>
+      <c r="AH11"/>
+      <c r="AI11"/>
       <c r="AJ11"/>
-      <c r="AK11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL11" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM11" t="n">
-        <v>6</v>
-      </c>
-      <c r="AN11" t="n">
-        <v>7</v>
-      </c>
-      <c r="AO11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP11" t="n">
-        <v>2</v>
-      </c>
+      <c r="AK11"/>
+      <c r="AL11"/>
+      <c r="AM11"/>
+      <c r="AN11"/>
+      <c r="AO11"/>
+      <c r="AP11"/>
       <c r="AQ11"/>
       <c r="AR11" t="n">
-        <v>5</v>
-      </c>
-      <c r="AS11" t="n">
-        <v>4</v>
-      </c>
-      <c r="AT11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU11" t="n">
-        <v>9</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="AS11"/>
+      <c r="AT11"/>
+      <c r="AU11"/>
       <c r="AV11" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="AW11"/>
-      <c r="AX11" t="n">
-        <v>25</v>
-      </c>
-      <c r="AY11" t="n">
-        <v>23</v>
-      </c>
+      <c r="AX11"/>
+      <c r="AY11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>61</v>
       </c>
-      <c r="B12"/>
+      <c r="B12" t="n">
+        <v>13</v>
+      </c>
       <c r="C12"/>
       <c r="D12"/>
-      <c r="E12"/>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
       <c r="F12"/>
       <c r="G12"/>
       <c r="H12" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I12"/>
       <c r="J12" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="K12"/>
-      <c r="L12"/>
+      <c r="L12" t="n">
+        <v>20</v>
+      </c>
       <c r="M12"/>
-      <c r="N12"/>
+      <c r="N12" t="n">
+        <v>18</v>
+      </c>
       <c r="O12"/>
-      <c r="P12"/>
+      <c r="P12" t="n">
+        <v>29</v>
+      </c>
       <c r="Q12"/>
-      <c r="R12"/>
+      <c r="R12" t="n">
+        <v>11</v>
+      </c>
       <c r="S12"/>
-      <c r="T12"/>
+      <c r="T12" t="n">
+        <v>76</v>
+      </c>
       <c r="U12"/>
-      <c r="V12"/>
+      <c r="V12" t="n">
+        <v>116</v>
+      </c>
       <c r="W12"/>
-      <c r="X12"/>
+      <c r="X12" t="n">
+        <v>90</v>
+      </c>
       <c r="Y12"/>
-      <c r="Z12"/>
+      <c r="Z12" t="n">
+        <v>48</v>
+      </c>
       <c r="AA12"/>
-      <c r="AB12"/>
+      <c r="AB12" t="n">
+        <v>56</v>
+      </c>
       <c r="AC12"/>
-      <c r="AD12"/>
+      <c r="AD12" t="n">
+        <v>78</v>
+      </c>
       <c r="AE12"/>
-      <c r="AF12"/>
+      <c r="AF12" t="n">
+        <v>116</v>
+      </c>
       <c r="AG12"/>
-      <c r="AH12"/>
+      <c r="AH12" t="n">
+        <v>163</v>
+      </c>
       <c r="AI12"/>
-      <c r="AJ12"/>
+      <c r="AJ12" t="n">
+        <v>92</v>
+      </c>
       <c r="AK12"/>
-      <c r="AL12"/>
-      <c r="AM12"/>
-      <c r="AN12"/>
-      <c r="AO12"/>
-      <c r="AP12"/>
-      <c r="AQ12"/>
+      <c r="AL12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>5</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>7</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>12</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>6</v>
+      </c>
       <c r="AR12" t="n">
-        <v>3</v>
-      </c>
-      <c r="AS12"/>
-      <c r="AT12"/>
-      <c r="AU12"/>
+        <v>2</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>6</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>8</v>
+      </c>
       <c r="AV12" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AW12"/>
-      <c r="AX12"/>
-      <c r="AY12"/>
+      <c r="AX12" t="n">
+        <v>7</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="n">
-        <v>13</v>
-      </c>
+      <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F13"/>
       <c r="G13"/>
       <c r="H13" t="n">
-        <v>7</v>
-      </c>
-      <c r="I13"/>
+        <v>9</v>
+      </c>
+      <c r="I13" t="n">
+        <v>14</v>
+      </c>
       <c r="J13" t="n">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="K13"/>
       <c r="L13" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="M13"/>
       <c r="N13" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="O13"/>
       <c r="P13" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="Q13"/>
       <c r="R13" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="S13"/>
       <c r="T13" t="n">
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="U13"/>
       <c r="V13" t="n">
-        <v>116</v>
+        <v>6</v>
       </c>
       <c r="W13"/>
       <c r="X13" t="n">
-        <v>90</v>
+        <v>3</v>
       </c>
       <c r="Y13"/>
       <c r="Z13" t="n">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="AA13"/>
       <c r="AB13" t="n">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="AC13"/>
       <c r="AD13" t="n">
-        <v>78</v>
+        <v>2</v>
       </c>
       <c r="AE13"/>
       <c r="AF13" t="n">
-        <v>116</v>
+        <v>6</v>
       </c>
       <c r="AG13"/>
       <c r="AH13" t="n">
-        <v>163</v>
-      </c>
-      <c r="AI13"/>
+        <v>11</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>1</v>
+      </c>
       <c r="AJ13" t="n">
-        <v>92</v>
-      </c>
-      <c r="AK13"/>
-      <c r="AL13" t="n">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL13"/>
       <c r="AM13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AN13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO13"/>
+      <c r="AP13" t="n">
         <v>7</v>
       </c>
-      <c r="AO13" t="n">
-        <v>4</v>
-      </c>
-      <c r="AP13" t="n">
-        <v>12</v>
-      </c>
       <c r="AQ13" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AR13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS13" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AT13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AU13" t="n">
-        <v>8</v>
-      </c>
-      <c r="AV13" t="n">
-        <v>8</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AV13"/>
       <c r="AW13"/>
       <c r="AX13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY13" t="n">
         <v>7</v>
-      </c>
-      <c r="AY13" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -1748,374 +1803,390 @@
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="H14" t="n">
-        <v>9</v>
-      </c>
-      <c r="I14" t="n">
-        <v>14</v>
-      </c>
+      <c r="H14"/>
+      <c r="I14"/>
       <c r="J14" t="n">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="K14"/>
       <c r="L14" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M14"/>
       <c r="N14" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="O14"/>
       <c r="P14" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="Q14"/>
-      <c r="R14" t="n">
-        <v>24</v>
-      </c>
+      <c r="R14"/>
       <c r="S14"/>
       <c r="T14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U14"/>
-      <c r="V14" t="n">
-        <v>6</v>
-      </c>
+      <c r="V14"/>
       <c r="W14"/>
       <c r="X14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y14"/>
-      <c r="Z14" t="n">
-        <v>16</v>
-      </c>
+      <c r="Z14"/>
       <c r="AA14"/>
-      <c r="AB14" t="n">
-        <v>1</v>
-      </c>
+      <c r="AB14"/>
       <c r="AC14"/>
       <c r="AD14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE14"/>
       <c r="AF14" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AG14"/>
-      <c r="AH14" t="n">
-        <v>11</v>
-      </c>
-      <c r="AI14" t="n">
-        <v>1</v>
-      </c>
+      <c r="AH14"/>
+      <c r="AI14"/>
       <c r="AJ14"/>
-      <c r="AK14" t="n">
-        <v>2</v>
-      </c>
+      <c r="AK14"/>
       <c r="AL14"/>
       <c r="AM14" t="n">
         <v>2</v>
       </c>
-      <c r="AN14" t="n">
-        <v>2</v>
-      </c>
+      <c r="AN14"/>
       <c r="AO14"/>
       <c r="AP14" t="n">
-        <v>7</v>
-      </c>
-      <c r="AQ14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AR14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU14" t="n">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AQ14"/>
+      <c r="AR14"/>
+      <c r="AS14"/>
+      <c r="AT14"/>
+      <c r="AU14"/>
       <c r="AV14"/>
       <c r="AW14"/>
-      <c r="AX14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY14" t="n">
-        <v>7</v>
-      </c>
+      <c r="AX14"/>
+      <c r="AY14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="B15"/>
+      <c r="B15" t="n">
+        <v>7</v>
+      </c>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>
-      <c r="H15"/>
+      <c r="H15" t="n">
+        <v>5</v>
+      </c>
       <c r="I15"/>
       <c r="J15" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="K15"/>
       <c r="L15" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="M15"/>
       <c r="N15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O15"/>
       <c r="P15" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="Q15"/>
-      <c r="R15"/>
-      <c r="S15"/>
+      <c r="R15" t="n">
+        <v>33</v>
+      </c>
+      <c r="S15" t="n">
+        <v>1</v>
+      </c>
       <c r="T15" t="n">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="U15"/>
-      <c r="V15"/>
+      <c r="V15" t="n">
+        <v>23</v>
+      </c>
       <c r="W15"/>
       <c r="X15" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="Y15"/>
-      <c r="Z15"/>
-      <c r="AA15"/>
-      <c r="AB15"/>
+      <c r="Z15" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB15" t="n">
+        <v>25</v>
+      </c>
       <c r="AC15"/>
       <c r="AD15" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AE15"/>
       <c r="AF15" t="n">
-        <v>2</v>
-      </c>
-      <c r="AG15"/>
-      <c r="AH15"/>
+        <v>22</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>14</v>
+      </c>
       <c r="AI15"/>
       <c r="AJ15"/>
-      <c r="AK15"/>
+      <c r="AK15" t="n">
+        <v>1</v>
+      </c>
       <c r="AL15"/>
-      <c r="AM15" t="n">
-        <v>2</v>
-      </c>
+      <c r="AM15"/>
       <c r="AN15"/>
       <c r="AO15"/>
-      <c r="AP15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ15"/>
-      <c r="AR15"/>
-      <c r="AS15"/>
-      <c r="AT15"/>
-      <c r="AU15"/>
-      <c r="AV15"/>
+      <c r="AP15"/>
+      <c r="AQ15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>5</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU15" t="n">
+        <v>13</v>
+      </c>
+      <c r="AV15" t="n">
+        <v>5</v>
+      </c>
       <c r="AW15"/>
-      <c r="AX15"/>
-      <c r="AY15"/>
+      <c r="AX15" t="n">
+        <v>11</v>
+      </c>
+      <c r="AY15" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
         <v>65</v>
       </c>
-      <c r="B16" t="n">
-        <v>7</v>
-      </c>
+      <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
-      <c r="H16" t="n">
-        <v>5</v>
-      </c>
+      <c r="H16"/>
       <c r="I16"/>
-      <c r="J16" t="n">
-        <v>17</v>
-      </c>
+      <c r="J16"/>
       <c r="K16"/>
       <c r="L16" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="M16"/>
       <c r="N16" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O16"/>
-      <c r="P16" t="n">
-        <v>16</v>
-      </c>
+      <c r="P16"/>
       <c r="Q16"/>
-      <c r="R16" t="n">
-        <v>33</v>
-      </c>
-      <c r="S16" t="n">
-        <v>1</v>
-      </c>
+      <c r="R16"/>
+      <c r="S16"/>
       <c r="T16" t="n">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="U16"/>
       <c r="V16" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="W16"/>
       <c r="X16" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="Y16"/>
       <c r="Z16" t="n">
-        <v>21</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AA16"/>
       <c r="AB16" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="AC16"/>
       <c r="AD16" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AE16"/>
       <c r="AF16" t="n">
-        <v>22</v>
-      </c>
-      <c r="AG16" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AG16"/>
       <c r="AH16" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="AI16"/>
       <c r="AJ16"/>
-      <c r="AK16" t="n">
-        <v>1</v>
-      </c>
+      <c r="AK16"/>
       <c r="AL16"/>
       <c r="AM16"/>
       <c r="AN16"/>
       <c r="AO16"/>
       <c r="AP16"/>
-      <c r="AQ16" t="n">
-        <v>2</v>
-      </c>
-      <c r="AR16" t="n">
-        <v>5</v>
-      </c>
-      <c r="AS16" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT16" t="n">
-        <v>6</v>
-      </c>
-      <c r="AU16" t="n">
-        <v>13</v>
-      </c>
-      <c r="AV16" t="n">
-        <v>5</v>
-      </c>
+      <c r="AQ16"/>
+      <c r="AR16"/>
+      <c r="AS16"/>
+      <c r="AT16"/>
+      <c r="AU16"/>
+      <c r="AV16"/>
       <c r="AW16"/>
-      <c r="AX16" t="n">
-        <v>11</v>
-      </c>
+      <c r="AX16"/>
       <c r="AY16" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
         <v>66</v>
       </c>
-      <c r="B17"/>
+      <c r="B17" t="n">
+        <v>9</v>
+      </c>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
-      <c r="H17"/>
+      <c r="H17" t="n">
+        <v>4</v>
+      </c>
       <c r="I17"/>
-      <c r="J17"/>
+      <c r="J17" t="n">
+        <v>16</v>
+      </c>
       <c r="K17"/>
       <c r="L17" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="M17"/>
       <c r="N17" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="O17"/>
-      <c r="P17"/>
+      <c r="P17" t="n">
+        <v>12</v>
+      </c>
       <c r="Q17"/>
-      <c r="R17"/>
-      <c r="S17"/>
+      <c r="R17" t="n">
+        <v>6</v>
+      </c>
+      <c r="S17" t="n">
+        <v>1</v>
+      </c>
       <c r="T17" t="n">
-        <v>9</v>
-      </c>
-      <c r="U17"/>
+        <v>16</v>
+      </c>
+      <c r="U17" t="n">
+        <v>3</v>
+      </c>
       <c r="V17" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="W17"/>
       <c r="X17" t="n">
-        <v>3</v>
-      </c>
-      <c r="Y17"/>
+        <v>8</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>1</v>
+      </c>
       <c r="Z17" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA17"/>
+        <v>17</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>1</v>
+      </c>
       <c r="AB17" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="AC17"/>
       <c r="AD17" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="AE17"/>
       <c r="AF17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG17"/>
+        <v>19</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>1</v>
+      </c>
       <c r="AH17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI17"/>
-      <c r="AJ17"/>
-      <c r="AK17"/>
-      <c r="AL17"/>
+        <v>36</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>4</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>44</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>1</v>
+      </c>
       <c r="AM17"/>
-      <c r="AN17"/>
-      <c r="AO17"/>
-      <c r="AP17"/>
-      <c r="AQ17"/>
-      <c r="AR17"/>
-      <c r="AS17"/>
-      <c r="AT17"/>
-      <c r="AU17"/>
-      <c r="AV17"/>
+      <c r="AN17" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>6</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>7</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>8</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>10</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>9</v>
+      </c>
+      <c r="AU17" t="n">
+        <v>12</v>
+      </c>
+      <c r="AV17" t="n">
+        <v>7</v>
+      </c>
       <c r="AW17"/>
-      <c r="AX17"/>
+      <c r="AX17" t="n">
+        <v>5</v>
+      </c>
       <c r="AY17" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
@@ -2123,571 +2194,505 @@
         <v>67</v>
       </c>
       <c r="B18" t="n">
-        <v>9</v>
-      </c>
-      <c r="C18"/>
+        <v>24</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
       <c r="D18"/>
       <c r="E18" t="n">
-        <v>14</v>
-      </c>
-      <c r="F18"/>
+        <v>21</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
       <c r="G18"/>
       <c r="H18" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I18"/>
       <c r="J18" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="K18"/>
       <c r="L18" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M18"/>
       <c r="N18" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O18"/>
       <c r="P18" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>5</v>
+      </c>
+      <c r="R18" t="n">
+        <v>9</v>
+      </c>
+      <c r="S18" t="n">
+        <v>1</v>
+      </c>
+      <c r="T18" t="n">
         <v>12</v>
       </c>
-      <c r="Q18"/>
-      <c r="R18" t="n">
-        <v>6</v>
-      </c>
-      <c r="S18" t="n">
-        <v>1</v>
-      </c>
-      <c r="T18" t="n">
-        <v>16</v>
-      </c>
       <c r="U18" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="V18" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="W18"/>
       <c r="X18" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Y18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z18" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="AA18" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AB18" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="AC18"/>
       <c r="AD18" t="n">
-        <v>13</v>
-      </c>
-      <c r="AE18"/>
+        <v>8</v>
+      </c>
+      <c r="AE18" t="n">
+        <v>2</v>
+      </c>
       <c r="AF18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>3</v>
+      </c>
+      <c r="AH18" t="n">
+        <v>7</v>
+      </c>
+      <c r="AI18"/>
+      <c r="AJ18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK18"/>
+      <c r="AL18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>12</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>12</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>15</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>28</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>14</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>9</v>
+      </c>
+      <c r="AS18" t="n">
         <v>19</v>
       </c>
-      <c r="AG18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH18" t="n">
-        <v>36</v>
-      </c>
-      <c r="AI18" t="n">
-        <v>4</v>
-      </c>
-      <c r="AJ18" t="n">
-        <v>38</v>
-      </c>
-      <c r="AK18" t="n">
-        <v>3</v>
-      </c>
-      <c r="AL18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM18"/>
-      <c r="AN18" t="n">
-        <v>5</v>
-      </c>
-      <c r="AO18" t="n">
+      <c r="AT18" t="n">
+        <v>39</v>
+      </c>
+      <c r="AU18" t="n">
         <v>6</v>
       </c>
-      <c r="AP18" t="n">
+      <c r="AV18" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX18" t="n">
+        <v>32</v>
+      </c>
+      <c r="AY18" t="n">
         <v>7</v>
-      </c>
-      <c r="AQ18" t="n">
-        <v>8</v>
-      </c>
-      <c r="AR18" t="n">
-        <v>10</v>
-      </c>
-      <c r="AS18" t="n">
-        <v>4</v>
-      </c>
-      <c r="AT18" t="n">
-        <v>9</v>
-      </c>
-      <c r="AU18" t="n">
-        <v>12</v>
-      </c>
-      <c r="AV18" t="n">
-        <v>7</v>
-      </c>
-      <c r="AW18"/>
-      <c r="AX18" t="n">
-        <v>5</v>
-      </c>
-      <c r="AY18" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
         <v>68</v>
       </c>
-      <c r="B19" t="n">
-        <v>24</v>
-      </c>
-      <c r="C19" t="n">
-        <v>1</v>
-      </c>
+      <c r="B19"/>
+      <c r="C19"/>
       <c r="D19"/>
-      <c r="E19" t="n">
-        <v>21</v>
-      </c>
-      <c r="F19" t="n">
-        <v>1</v>
-      </c>
+      <c r="E19"/>
+      <c r="F19"/>
       <c r="G19"/>
       <c r="H19" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I19"/>
-      <c r="J19" t="n">
-        <v>11</v>
-      </c>
+      <c r="J19"/>
       <c r="K19"/>
-      <c r="L19" t="n">
-        <v>8</v>
-      </c>
+      <c r="L19"/>
       <c r="M19"/>
-      <c r="N19" t="n">
-        <v>13</v>
-      </c>
-      <c r="O19"/>
-      <c r="P19" t="n">
-        <v>8</v>
-      </c>
-      <c r="Q19" t="n">
+      <c r="N19"/>
+      <c r="O19" t="n">
+        <v>2</v>
+      </c>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19" t="n">
+        <v>1</v>
+      </c>
+      <c r="W19" t="n">
+        <v>1</v>
+      </c>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AB19" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC19"/>
+      <c r="AD19"/>
+      <c r="AE19"/>
+      <c r="AF19" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG19"/>
+      <c r="AH19"/>
+      <c r="AI19" t="n">
         <v>5</v>
       </c>
-      <c r="R19" t="n">
-        <v>9</v>
-      </c>
-      <c r="S19" t="n">
-        <v>1</v>
-      </c>
-      <c r="T19" t="n">
-        <v>12</v>
-      </c>
-      <c r="U19" t="n">
-        <v>8</v>
-      </c>
-      <c r="V19" t="n">
-        <v>7</v>
-      </c>
-      <c r="W19"/>
-      <c r="X19" t="n">
-        <v>10</v>
-      </c>
-      <c r="Y19" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>2</v>
-      </c>
-      <c r="AA19" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB19" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC19"/>
-      <c r="AD19" t="n">
-        <v>8</v>
-      </c>
-      <c r="AE19" t="n">
-        <v>2</v>
-      </c>
-      <c r="AF19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG19" t="n">
-        <v>3</v>
-      </c>
-      <c r="AH19" t="n">
-        <v>7</v>
-      </c>
-      <c r="AI19"/>
       <c r="AJ19"/>
       <c r="AK19"/>
-      <c r="AL19" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL19"/>
       <c r="AM19" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="AN19" t="n">
-        <v>12</v>
-      </c>
-      <c r="AO19" t="n">
-        <v>15</v>
-      </c>
-      <c r="AP19" t="n">
-        <v>28</v>
-      </c>
-      <c r="AQ19" t="n">
-        <v>14</v>
-      </c>
-      <c r="AR19" t="n">
-        <v>9</v>
-      </c>
-      <c r="AS19" t="n">
-        <v>19</v>
-      </c>
-      <c r="AT19" t="n">
-        <v>39</v>
-      </c>
-      <c r="AU19" t="n">
-        <v>6</v>
-      </c>
-      <c r="AV19" t="n">
-        <v>20</v>
-      </c>
-      <c r="AW19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX19" t="n">
-        <v>32</v>
-      </c>
-      <c r="AY19" t="n">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="AO19"/>
+      <c r="AP19"/>
+      <c r="AQ19"/>
+      <c r="AR19"/>
+      <c r="AS19"/>
+      <c r="AT19"/>
+      <c r="AU19"/>
+      <c r="AV19"/>
+      <c r="AW19"/>
+      <c r="AX19"/>
+      <c r="AY19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
         <v>69</v>
       </c>
-      <c r="B20"/>
+      <c r="B20" t="n">
+        <v>32</v>
+      </c>
       <c r="C20"/>
       <c r="D20"/>
-      <c r="E20"/>
+      <c r="E20" t="n">
+        <v>9</v>
+      </c>
       <c r="F20"/>
       <c r="G20"/>
       <c r="H20" t="n">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="I20"/>
-      <c r="J20"/>
+      <c r="J20" t="n">
+        <v>25</v>
+      </c>
       <c r="K20"/>
-      <c r="L20"/>
+      <c r="L20" t="n">
+        <v>14</v>
+      </c>
       <c r="M20"/>
-      <c r="N20"/>
-      <c r="O20" t="n">
-        <v>2</v>
-      </c>
-      <c r="P20"/>
+      <c r="N20" t="n">
+        <v>63</v>
+      </c>
+      <c r="O20"/>
+      <c r="P20" t="n">
+        <v>34</v>
+      </c>
       <c r="Q20"/>
-      <c r="R20"/>
+      <c r="R20" t="n">
+        <v>51</v>
+      </c>
       <c r="S20"/>
-      <c r="T20"/>
+      <c r="T20" t="n">
+        <v>70</v>
+      </c>
       <c r="U20"/>
       <c r="V20" t="n">
-        <v>1</v>
-      </c>
-      <c r="W20" t="n">
-        <v>1</v>
-      </c>
-      <c r="X20"/>
+        <v>40</v>
+      </c>
+      <c r="W20"/>
+      <c r="X20" t="n">
+        <v>78</v>
+      </c>
       <c r="Y20"/>
-      <c r="Z20"/>
+      <c r="Z20" t="n">
+        <v>33</v>
+      </c>
       <c r="AA20"/>
       <c r="AB20" t="n">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="AC20"/>
-      <c r="AD20"/>
+      <c r="AD20" t="n">
+        <v>127</v>
+      </c>
       <c r="AE20"/>
       <c r="AF20" t="n">
-        <v>1</v>
+        <v>197</v>
       </c>
       <c r="AG20"/>
-      <c r="AH20"/>
-      <c r="AI20" t="n">
-        <v>5</v>
-      </c>
+      <c r="AH20" t="n">
+        <v>226</v>
+      </c>
+      <c r="AI20"/>
       <c r="AJ20"/>
       <c r="AK20"/>
       <c r="AL20"/>
       <c r="AM20" t="n">
-        <v>2</v>
-      </c>
-      <c r="AN20" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO20"/>
+        <v>4</v>
+      </c>
+      <c r="AN20"/>
+      <c r="AO20" t="n">
+        <v>2</v>
+      </c>
       <c r="AP20"/>
-      <c r="AQ20"/>
-      <c r="AR20"/>
-      <c r="AS20"/>
-      <c r="AT20"/>
-      <c r="AU20"/>
+      <c r="AQ20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR20" t="n">
+        <v>8</v>
+      </c>
+      <c r="AS20" t="n">
+        <v>5</v>
+      </c>
+      <c r="AT20" t="n">
+        <v>9</v>
+      </c>
+      <c r="AU20" t="n">
+        <v>10</v>
+      </c>
       <c r="AV20"/>
       <c r="AW20"/>
-      <c r="AX20"/>
-      <c r="AY20"/>
+      <c r="AX20" t="n">
+        <v>8</v>
+      </c>
+      <c r="AY20" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
         <v>70</v>
       </c>
       <c r="B21" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21" t="n">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="F21"/>
       <c r="G21"/>
       <c r="H21" t="n">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="K21"/>
       <c r="L21" t="n">
-        <v>14</v>
+        <v>112</v>
       </c>
       <c r="M21"/>
       <c r="N21" t="n">
-        <v>63</v>
+        <v>121</v>
       </c>
       <c r="O21"/>
       <c r="P21" t="n">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="Q21"/>
       <c r="R21" t="n">
-        <v>51</v>
-      </c>
-      <c r="S21"/>
+        <v>117</v>
+      </c>
+      <c r="S21" t="n">
+        <v>2</v>
+      </c>
       <c r="T21" t="n">
-        <v>70</v>
-      </c>
-      <c r="U21"/>
+        <v>229</v>
+      </c>
+      <c r="U21" t="n">
+        <v>3</v>
+      </c>
       <c r="V21" t="n">
-        <v>40</v>
-      </c>
-      <c r="W21"/>
+        <v>210</v>
+      </c>
+      <c r="W21" t="n">
+        <v>6</v>
+      </c>
       <c r="X21" t="n">
-        <v>78</v>
-      </c>
-      <c r="Y21"/>
+        <v>187</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>3</v>
+      </c>
       <c r="Z21" t="n">
-        <v>33</v>
-      </c>
-      <c r="AA21"/>
+        <v>221</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>3</v>
+      </c>
       <c r="AB21" t="n">
-        <v>52</v>
-      </c>
-      <c r="AC21"/>
+        <v>352</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>9</v>
+      </c>
       <c r="AD21" t="n">
-        <v>127</v>
-      </c>
-      <c r="AE21"/>
+        <v>350</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>6</v>
+      </c>
       <c r="AF21" t="n">
-        <v>197</v>
-      </c>
-      <c r="AG21"/>
+        <v>232</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>7</v>
+      </c>
       <c r="AH21" t="n">
-        <v>226</v>
-      </c>
-      <c r="AI21"/>
+        <v>286</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>2</v>
+      </c>
       <c r="AJ21"/>
-      <c r="AK21"/>
-      <c r="AL21"/>
+      <c r="AK21" t="n">
+        <v>4</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>3</v>
+      </c>
       <c r="AM21" t="n">
         <v>4</v>
       </c>
-      <c r="AN21"/>
+      <c r="AN21" t="n">
+        <v>12</v>
+      </c>
       <c r="AO21" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP21"/>
+        <v>10</v>
+      </c>
+      <c r="AP21" t="n">
+        <v>15</v>
+      </c>
       <c r="AQ21" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="AR21" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="AS21" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AT21" t="n">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="AU21" t="n">
-        <v>10</v>
-      </c>
-      <c r="AV21"/>
+        <v>28</v>
+      </c>
+      <c r="AV21" t="n">
+        <v>22</v>
+      </c>
       <c r="AW21"/>
       <c r="AX21" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="AY21" t="n">
-        <v>19</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
         <v>71</v>
       </c>
-      <c r="B22" t="n">
-        <v>33</v>
-      </c>
+      <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
       <c r="E22" t="n">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="F22"/>
       <c r="G22"/>
-      <c r="H22" t="n">
-        <v>64</v>
-      </c>
+      <c r="H22"/>
       <c r="I22"/>
-      <c r="J22" t="n">
-        <v>148</v>
-      </c>
+      <c r="J22"/>
       <c r="K22"/>
-      <c r="L22" t="n">
-        <v>112</v>
-      </c>
+      <c r="L22"/>
       <c r="M22"/>
-      <c r="N22" t="n">
-        <v>121</v>
-      </c>
+      <c r="N22"/>
       <c r="O22"/>
-      <c r="P22" t="n">
-        <v>150</v>
-      </c>
+      <c r="P22"/>
       <c r="Q22"/>
-      <c r="R22" t="n">
-        <v>117</v>
-      </c>
-      <c r="S22" t="n">
-        <v>2</v>
-      </c>
-      <c r="T22" t="n">
-        <v>229</v>
-      </c>
-      <c r="U22" t="n">
-        <v>3</v>
-      </c>
-      <c r="V22" t="n">
-        <v>210</v>
-      </c>
-      <c r="W22" t="n">
-        <v>6</v>
-      </c>
-      <c r="X22" t="n">
-        <v>187</v>
-      </c>
-      <c r="Y22" t="n">
-        <v>3</v>
-      </c>
-      <c r="Z22" t="n">
-        <v>221</v>
-      </c>
-      <c r="AA22" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB22" t="n">
-        <v>352</v>
-      </c>
-      <c r="AC22" t="n">
-        <v>9</v>
-      </c>
-      <c r="AD22" t="n">
-        <v>350</v>
-      </c>
-      <c r="AE22" t="n">
-        <v>6</v>
-      </c>
-      <c r="AF22" t="n">
-        <v>232</v>
-      </c>
-      <c r="AG22" t="n">
-        <v>7</v>
-      </c>
-      <c r="AH22" t="n">
-        <v>286</v>
-      </c>
-      <c r="AI22" t="n">
-        <v>2</v>
-      </c>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+      <c r="Z22"/>
+      <c r="AA22"/>
+      <c r="AB22"/>
+      <c r="AC22"/>
+      <c r="AD22"/>
+      <c r="AE22"/>
+      <c r="AF22"/>
+      <c r="AG22"/>
+      <c r="AH22"/>
+      <c r="AI22"/>
       <c r="AJ22"/>
-      <c r="AK22" t="n">
-        <v>4</v>
-      </c>
-      <c r="AL22" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM22" t="n">
-        <v>4</v>
-      </c>
-      <c r="AN22" t="n">
-        <v>12</v>
-      </c>
-      <c r="AO22" t="n">
-        <v>10</v>
-      </c>
-      <c r="AP22" t="n">
-        <v>15</v>
-      </c>
+      <c r="AK22"/>
+      <c r="AL22"/>
+      <c r="AM22"/>
+      <c r="AN22"/>
+      <c r="AO22"/>
+      <c r="AP22"/>
       <c r="AQ22" t="n">
-        <v>18</v>
-      </c>
-      <c r="AR22" t="n">
-        <v>15</v>
-      </c>
-      <c r="AS22" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT22" t="n">
-        <v>28</v>
-      </c>
-      <c r="AU22" t="n">
-        <v>28</v>
-      </c>
-      <c r="AV22" t="n">
-        <v>22</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AR22"/>
+      <c r="AS22"/>
+      <c r="AT22"/>
+      <c r="AU22"/>
+      <c r="AV22"/>
       <c r="AW22"/>
-      <c r="AX22" t="n">
-        <v>17</v>
-      </c>
-      <c r="AY22" t="n">
-        <v>82</v>
-      </c>
+      <c r="AX22"/>
+      <c r="AY22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -2696,9 +2701,7 @@
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
-      <c r="E23" t="n">
-        <v>1</v>
-      </c>
+      <c r="E23"/>
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
@@ -2721,13 +2724,19 @@
       <c r="Y23"/>
       <c r="Z23"/>
       <c r="AA23"/>
-      <c r="AB23"/>
+      <c r="AB23" t="n">
+        <v>1</v>
+      </c>
       <c r="AC23"/>
       <c r="AD23"/>
       <c r="AE23"/>
-      <c r="AF23"/>
+      <c r="AF23" t="n">
+        <v>6</v>
+      </c>
       <c r="AG23"/>
-      <c r="AH23"/>
+      <c r="AH23" t="n">
+        <v>2</v>
+      </c>
       <c r="AI23"/>
       <c r="AJ23"/>
       <c r="AK23"/>
@@ -2736,9 +2745,7 @@
       <c r="AN23"/>
       <c r="AO23"/>
       <c r="AP23"/>
-      <c r="AQ23" t="n">
-        <v>1</v>
-      </c>
+      <c r="AQ23"/>
       <c r="AR23"/>
       <c r="AS23"/>
       <c r="AT23"/>
@@ -2778,19 +2785,13 @@
       <c r="Y24"/>
       <c r="Z24"/>
       <c r="AA24"/>
-      <c r="AB24" t="n">
-        <v>1</v>
-      </c>
+      <c r="AB24"/>
       <c r="AC24"/>
       <c r="AD24"/>
       <c r="AE24"/>
-      <c r="AF24" t="n">
-        <v>6</v>
-      </c>
+      <c r="AF24"/>
       <c r="AG24"/>
-      <c r="AH24" t="n">
-        <v>2</v>
-      </c>
+      <c r="AH24"/>
       <c r="AI24"/>
       <c r="AJ24"/>
       <c r="AK24"/>
@@ -2800,7 +2801,9 @@
       <c r="AO24"/>
       <c r="AP24"/>
       <c r="AQ24"/>
-      <c r="AR24"/>
+      <c r="AR24" t="n">
+        <v>1</v>
+      </c>
       <c r="AS24"/>
       <c r="AT24"/>
       <c r="AU24"/>
@@ -2837,7 +2840,9 @@
       <c r="W25"/>
       <c r="X25"/>
       <c r="Y25"/>
-      <c r="Z25"/>
+      <c r="Z25" t="n">
+        <v>1</v>
+      </c>
       <c r="AA25"/>
       <c r="AB25"/>
       <c r="AC25"/>
@@ -2855,9 +2860,7 @@
       <c r="AO25"/>
       <c r="AP25"/>
       <c r="AQ25"/>
-      <c r="AR25" t="n">
-        <v>1</v>
-      </c>
+      <c r="AR25"/>
       <c r="AS25"/>
       <c r="AT25"/>
       <c r="AU25"/>
@@ -2870,316 +2873,384 @@
       <c r="A26" t="s">
         <v>75</v>
       </c>
-      <c r="B26"/>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
       <c r="C26"/>
       <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26"/>
-      <c r="H26"/>
+      <c r="H26" t="n">
+        <v>15</v>
+      </c>
       <c r="I26"/>
-      <c r="J26"/>
+      <c r="J26" t="n">
+        <v>1</v>
+      </c>
       <c r="K26"/>
-      <c r="L26"/>
+      <c r="L26" t="n">
+        <v>18</v>
+      </c>
       <c r="M26"/>
-      <c r="N26"/>
+      <c r="N26" t="n">
+        <v>1</v>
+      </c>
       <c r="O26"/>
-      <c r="P26"/>
+      <c r="P26" t="n">
+        <v>2</v>
+      </c>
       <c r="Q26"/>
       <c r="R26"/>
       <c r="S26"/>
-      <c r="T26"/>
+      <c r="T26" t="n">
+        <v>6</v>
+      </c>
       <c r="U26"/>
-      <c r="V26"/>
+      <c r="V26" t="n">
+        <v>2</v>
+      </c>
       <c r="W26"/>
-      <c r="X26"/>
+      <c r="X26" t="n">
+        <v>4</v>
+      </c>
       <c r="Y26"/>
-      <c r="Z26" t="n">
-        <v>1</v>
-      </c>
+      <c r="Z26"/>
       <c r="AA26"/>
-      <c r="AB26"/>
+      <c r="AB26" t="n">
+        <v>1</v>
+      </c>
       <c r="AC26"/>
-      <c r="AD26"/>
+      <c r="AD26" t="n">
+        <v>5</v>
+      </c>
       <c r="AE26"/>
       <c r="AF26"/>
-      <c r="AG26"/>
+      <c r="AG26" t="n">
+        <v>1</v>
+      </c>
       <c r="AH26"/>
       <c r="AI26"/>
       <c r="AJ26"/>
       <c r="AK26"/>
-      <c r="AL26"/>
+      <c r="AL26" t="n">
+        <v>1</v>
+      </c>
       <c r="AM26"/>
       <c r="AN26"/>
       <c r="AO26"/>
       <c r="AP26"/>
       <c r="AQ26"/>
       <c r="AR26"/>
-      <c r="AS26"/>
+      <c r="AS26" t="n">
+        <v>1</v>
+      </c>
       <c r="AT26"/>
       <c r="AU26"/>
       <c r="AV26"/>
       <c r="AW26"/>
       <c r="AX26"/>
-      <c r="AY26"/>
+      <c r="AY26" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
         <v>76</v>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27"/>
       <c r="D27"/>
-      <c r="E27"/>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="H27" t="n">
-        <v>15</v>
-      </c>
+      <c r="H27"/>
       <c r="I27"/>
-      <c r="J27" t="n">
-        <v>1</v>
-      </c>
+      <c r="J27"/>
       <c r="K27"/>
-      <c r="L27" t="n">
-        <v>18</v>
-      </c>
+      <c r="L27"/>
       <c r="M27"/>
-      <c r="N27" t="n">
-        <v>1</v>
-      </c>
+      <c r="N27"/>
       <c r="O27"/>
-      <c r="P27" t="n">
-        <v>2</v>
-      </c>
+      <c r="P27"/>
       <c r="Q27"/>
       <c r="R27"/>
       <c r="S27"/>
-      <c r="T27" t="n">
-        <v>6</v>
-      </c>
+      <c r="T27"/>
       <c r="U27"/>
       <c r="V27" t="n">
         <v>2</v>
       </c>
       <c r="W27"/>
-      <c r="X27" t="n">
-        <v>4</v>
-      </c>
+      <c r="X27"/>
       <c r="Y27"/>
       <c r="Z27"/>
       <c r="AA27"/>
-      <c r="AB27" t="n">
-        <v>1</v>
-      </c>
+      <c r="AB27"/>
       <c r="AC27"/>
-      <c r="AD27" t="n">
-        <v>5</v>
-      </c>
+      <c r="AD27"/>
       <c r="AE27"/>
       <c r="AF27"/>
-      <c r="AG27" t="n">
-        <v>1</v>
-      </c>
+      <c r="AG27"/>
       <c r="AH27"/>
-      <c r="AI27"/>
+      <c r="AI27" t="n">
+        <v>1</v>
+      </c>
       <c r="AJ27"/>
       <c r="AK27"/>
-      <c r="AL27" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL27"/>
       <c r="AM27"/>
       <c r="AN27"/>
       <c r="AO27"/>
       <c r="AP27"/>
       <c r="AQ27"/>
       <c r="AR27"/>
-      <c r="AS27" t="n">
-        <v>1</v>
-      </c>
+      <c r="AS27"/>
       <c r="AT27"/>
       <c r="AU27"/>
       <c r="AV27"/>
       <c r="AW27"/>
       <c r="AX27"/>
-      <c r="AY27" t="n">
-        <v>1</v>
-      </c>
+      <c r="AY27"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
         <v>77</v>
       </c>
       <c r="B28" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F28"/>
       <c r="G28"/>
-      <c r="H28"/>
+      <c r="H28" t="n">
+        <v>6</v>
+      </c>
       <c r="I28"/>
-      <c r="J28"/>
+      <c r="J28" t="n">
+        <v>12</v>
+      </c>
       <c r="K28"/>
-      <c r="L28"/>
+      <c r="L28" t="n">
+        <v>3</v>
+      </c>
       <c r="M28"/>
-      <c r="N28"/>
+      <c r="N28" t="n">
+        <v>11</v>
+      </c>
       <c r="O28"/>
-      <c r="P28"/>
+      <c r="P28" t="n">
+        <v>20</v>
+      </c>
       <c r="Q28"/>
-      <c r="R28"/>
-      <c r="S28"/>
-      <c r="T28"/>
+      <c r="R28" t="n">
+        <v>7</v>
+      </c>
+      <c r="S28" t="n">
+        <v>1</v>
+      </c>
+      <c r="T28" t="n">
+        <v>24</v>
+      </c>
       <c r="U28"/>
       <c r="V28" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="W28"/>
-      <c r="X28"/>
+      <c r="X28" t="n">
+        <v>7</v>
+      </c>
       <c r="Y28"/>
-      <c r="Z28"/>
+      <c r="Z28" t="n">
+        <v>12</v>
+      </c>
       <c r="AA28"/>
-      <c r="AB28"/>
+      <c r="AB28" t="n">
+        <v>6</v>
+      </c>
       <c r="AC28"/>
-      <c r="AD28"/>
+      <c r="AD28" t="n">
+        <v>8</v>
+      </c>
       <c r="AE28"/>
-      <c r="AF28"/>
+      <c r="AF28" t="n">
+        <v>2</v>
+      </c>
       <c r="AG28"/>
-      <c r="AH28"/>
-      <c r="AI28" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ28"/>
+      <c r="AH28" t="n">
+        <v>11</v>
+      </c>
+      <c r="AI28"/>
+      <c r="AJ28" t="n">
+        <v>14</v>
+      </c>
       <c r="AK28"/>
-      <c r="AL28"/>
-      <c r="AM28"/>
-      <c r="AN28"/>
-      <c r="AO28"/>
-      <c r="AP28"/>
-      <c r="AQ28"/>
-      <c r="AR28"/>
-      <c r="AS28"/>
-      <c r="AT28"/>
+      <c r="AL28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>10</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>8</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>6</v>
+      </c>
+      <c r="AR28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT28" t="n">
+        <v>5</v>
+      </c>
       <c r="AU28"/>
       <c r="AV28"/>
       <c r="AW28"/>
-      <c r="AX28"/>
-      <c r="AY28"/>
+      <c r="AX28" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY28" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
         <v>78</v>
       </c>
       <c r="B29" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F29"/>
-      <c r="G29"/>
+      <c r="G29" t="n">
+        <v>1</v>
+      </c>
       <c r="H29" t="n">
-        <v>6</v>
-      </c>
-      <c r="I29"/>
+        <v>46</v>
+      </c>
+      <c r="I29" t="n">
+        <v>1</v>
+      </c>
       <c r="J29" t="n">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="K29"/>
       <c r="L29" t="n">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="M29"/>
       <c r="N29" t="n">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="O29"/>
       <c r="P29" t="n">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="Q29"/>
       <c r="R29" t="n">
-        <v>7</v>
-      </c>
-      <c r="S29" t="n">
-        <v>1</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="S29"/>
       <c r="T29" t="n">
-        <v>24</v>
-      </c>
-      <c r="U29"/>
+        <v>80</v>
+      </c>
+      <c r="U29" t="n">
+        <v>1</v>
+      </c>
       <c r="V29" t="n">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="W29"/>
       <c r="X29" t="n">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="Y29"/>
       <c r="Z29" t="n">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="AA29"/>
       <c r="AB29" t="n">
-        <v>6</v>
-      </c>
-      <c r="AC29"/>
+        <v>93</v>
+      </c>
+      <c r="AC29" t="n">
+        <v>1</v>
+      </c>
       <c r="AD29" t="n">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="AE29"/>
       <c r="AF29" t="n">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="AG29"/>
       <c r="AH29" t="n">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="AI29"/>
-      <c r="AJ29"/>
-      <c r="AK29"/>
+      <c r="AJ29" t="n">
+        <v>62</v>
+      </c>
+      <c r="AK29" t="n">
+        <v>3</v>
+      </c>
       <c r="AL29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM29" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AN29" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AO29" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AP29" t="n">
-        <v>2</v>
-      </c>
-      <c r="AQ29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ29"/>
+      <c r="AR29" t="n">
         <v>6</v>
       </c>
-      <c r="AR29" t="n">
-        <v>2</v>
-      </c>
       <c r="AS29" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AT29" t="n">
+        <v>7</v>
+      </c>
+      <c r="AU29" t="n">
+        <v>4</v>
+      </c>
+      <c r="AV29" t="n">
         <v>5</v>
       </c>
-      <c r="AU29"/>
-      <c r="AV29"/>
       <c r="AW29"/>
       <c r="AX29" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="AY29" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30">
@@ -3187,122 +3258,116 @@
         <v>79</v>
       </c>
       <c r="B30" t="n">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30" t="n">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="F30"/>
-      <c r="G30" t="n">
-        <v>1</v>
-      </c>
+      <c r="G30"/>
       <c r="H30" t="n">
-        <v>46</v>
-      </c>
-      <c r="I30" t="n">
-        <v>1</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="I30"/>
       <c r="J30" t="n">
-        <v>27</v>
+        <v>74</v>
       </c>
       <c r="K30"/>
       <c r="L30" t="n">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="M30"/>
       <c r="N30" t="n">
-        <v>35</v>
-      </c>
-      <c r="O30"/>
+        <v>50</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1</v>
+      </c>
       <c r="P30" t="n">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="Q30"/>
       <c r="R30" t="n">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="S30"/>
       <c r="T30" t="n">
-        <v>80</v>
-      </c>
-      <c r="U30" t="n">
-        <v>1</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="U30"/>
       <c r="V30" t="n">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="W30"/>
       <c r="X30" t="n">
-        <v>139</v>
+        <v>58</v>
       </c>
       <c r="Y30"/>
       <c r="Z30" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="AA30"/>
       <c r="AB30" t="n">
-        <v>93</v>
-      </c>
-      <c r="AC30" t="n">
-        <v>1</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="AC30"/>
       <c r="AD30" t="n">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="AE30"/>
       <c r="AF30" t="n">
-        <v>71</v>
+        <v>38</v>
       </c>
       <c r="AG30"/>
       <c r="AH30" t="n">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="AI30"/>
       <c r="AJ30" t="n">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="AK30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AL30" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM30"/>
+      <c r="AN30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ30" t="n">
+        <v>6</v>
+      </c>
+      <c r="AR30" t="n">
         <v>8</v>
       </c>
-      <c r="AN30" t="n">
-        <v>7</v>
-      </c>
-      <c r="AO30" t="n">
-        <v>5</v>
-      </c>
-      <c r="AP30" t="n">
-        <v>3</v>
-      </c>
-      <c r="AQ30"/>
-      <c r="AR30" t="n">
-        <v>6</v>
-      </c>
       <c r="AS30" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AT30" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AU30" t="n">
         <v>4</v>
       </c>
       <c r="AV30" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AW30"/>
       <c r="AX30" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AY30" t="n">
-        <v>14</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31">
@@ -3310,426 +3375,396 @@
         <v>80</v>
       </c>
       <c r="B31" t="n">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="C31"/>
-      <c r="D31"/>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
       <c r="E31" t="n">
-        <v>75</v>
+        <v>27</v>
       </c>
       <c r="F31"/>
       <c r="G31"/>
       <c r="H31" t="n">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="I31"/>
       <c r="J31" t="n">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="K31"/>
       <c r="L31" t="n">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="M31"/>
       <c r="N31" t="n">
-        <v>50</v>
-      </c>
-      <c r="O31" t="n">
-        <v>1</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="O31"/>
       <c r="P31" t="n">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="Q31"/>
       <c r="R31" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="S31"/>
       <c r="T31" t="n">
-        <v>96</v>
+        <v>18</v>
       </c>
       <c r="U31"/>
       <c r="V31" t="n">
-        <v>77</v>
+        <v>16</v>
       </c>
       <c r="W31"/>
       <c r="X31" t="n">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="Y31"/>
       <c r="Z31" t="n">
-        <v>106</v>
+        <v>28</v>
       </c>
       <c r="AA31"/>
       <c r="AB31" t="n">
-        <v>98</v>
-      </c>
-      <c r="AC31"/>
+        <v>61</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>1</v>
+      </c>
       <c r="AD31" t="n">
-        <v>31</v>
-      </c>
-      <c r="AE31"/>
+        <v>52</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>1</v>
+      </c>
       <c r="AF31" t="n">
-        <v>38</v>
-      </c>
-      <c r="AG31"/>
+        <v>6</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>1</v>
+      </c>
       <c r="AH31" t="n">
-        <v>25</v>
-      </c>
-      <c r="AI31"/>
+        <v>50</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>1</v>
+      </c>
       <c r="AJ31"/>
       <c r="AK31" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AL31" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM31"/>
+        <v>3</v>
+      </c>
+      <c r="AM31" t="n">
+        <v>3</v>
+      </c>
       <c r="AN31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AO31" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AP31" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AQ31" t="n">
         <v>6</v>
       </c>
       <c r="AR31" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS31" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT31" t="n">
+        <v>14</v>
+      </c>
+      <c r="AU31" t="n">
         <v>8</v>
       </c>
-      <c r="AS31" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT31" t="n">
-        <v>9</v>
-      </c>
-      <c r="AU31" t="n">
-        <v>4</v>
-      </c>
       <c r="AV31" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AW31"/>
       <c r="AX31" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="AY31" t="n">
-        <v>57</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
         <v>81</v>
       </c>
-      <c r="B32" t="n">
-        <v>30</v>
-      </c>
+      <c r="B32"/>
       <c r="C32"/>
-      <c r="D32" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" t="n">
-        <v>27</v>
-      </c>
+      <c r="D32"/>
+      <c r="E32"/>
       <c r="F32"/>
       <c r="G32"/>
-      <c r="H32" t="n">
-        <v>75</v>
-      </c>
+      <c r="H32"/>
       <c r="I32"/>
-      <c r="J32" t="n">
-        <v>43</v>
-      </c>
+      <c r="J32"/>
       <c r="K32"/>
-      <c r="L32" t="n">
-        <v>62</v>
-      </c>
+      <c r="L32"/>
       <c r="M32"/>
       <c r="N32" t="n">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="O32"/>
-      <c r="P32" t="n">
-        <v>40</v>
-      </c>
+      <c r="P32"/>
       <c r="Q32"/>
-      <c r="R32" t="n">
-        <v>49</v>
-      </c>
+      <c r="R32"/>
       <c r="S32"/>
-      <c r="T32" t="n">
-        <v>18</v>
-      </c>
+      <c r="T32"/>
       <c r="U32"/>
       <c r="V32" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="W32"/>
-      <c r="X32" t="n">
-        <v>16</v>
-      </c>
+      <c r="X32"/>
       <c r="Y32"/>
-      <c r="Z32" t="n">
-        <v>28</v>
-      </c>
+      <c r="Z32"/>
       <c r="AA32"/>
-      <c r="AB32" t="n">
-        <v>61</v>
-      </c>
-      <c r="AC32" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD32" t="n">
-        <v>52</v>
-      </c>
-      <c r="AE32" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF32" t="n">
-        <v>6</v>
-      </c>
-      <c r="AG32" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH32" t="n">
-        <v>50</v>
-      </c>
-      <c r="AI32" t="n">
-        <v>1</v>
-      </c>
+      <c r="AB32"/>
+      <c r="AC32"/>
+      <c r="AD32"/>
+      <c r="AE32"/>
+      <c r="AF32"/>
+      <c r="AG32"/>
+      <c r="AH32"/>
+      <c r="AI32"/>
       <c r="AJ32"/>
-      <c r="AK32" t="n">
-        <v>8</v>
-      </c>
-      <c r="AL32" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM32" t="n">
-        <v>3</v>
-      </c>
-      <c r="AN32" t="n">
-        <v>2</v>
-      </c>
-      <c r="AO32" t="n">
-        <v>6</v>
-      </c>
-      <c r="AP32" t="n">
-        <v>6</v>
-      </c>
-      <c r="AQ32" t="n">
-        <v>6</v>
-      </c>
-      <c r="AR32" t="n">
-        <v>2</v>
-      </c>
-      <c r="AS32" t="n">
-        <v>4</v>
-      </c>
-      <c r="AT32" t="n">
-        <v>14</v>
-      </c>
-      <c r="AU32" t="n">
-        <v>8</v>
-      </c>
-      <c r="AV32" t="n">
-        <v>3</v>
-      </c>
+      <c r="AK32"/>
+      <c r="AL32"/>
+      <c r="AM32"/>
+      <c r="AN32"/>
+      <c r="AO32"/>
+      <c r="AP32"/>
+      <c r="AQ32"/>
+      <c r="AR32"/>
+      <c r="AS32"/>
+      <c r="AT32"/>
+      <c r="AU32"/>
+      <c r="AV32"/>
       <c r="AW32"/>
-      <c r="AX32" t="n">
-        <v>7</v>
-      </c>
-      <c r="AY32" t="n">
-        <v>20</v>
-      </c>
+      <c r="AX32"/>
+      <c r="AY32"/>
     </row>
     <row r="33">
       <c r="A33" t="s">
         <v>82</v>
       </c>
-      <c r="B33"/>
+      <c r="B33" t="n">
+        <v>13</v>
+      </c>
       <c r="C33"/>
       <c r="D33"/>
-      <c r="E33"/>
+      <c r="E33" t="n">
+        <v>11</v>
+      </c>
       <c r="F33"/>
       <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33"/>
-      <c r="L33"/>
+      <c r="H33" t="n">
+        <v>46</v>
+      </c>
+      <c r="I33" t="n">
+        <v>7</v>
+      </c>
+      <c r="J33" t="n">
+        <v>60</v>
+      </c>
+      <c r="K33" t="n">
+        <v>1</v>
+      </c>
+      <c r="L33" t="n">
+        <v>44</v>
+      </c>
       <c r="M33"/>
       <c r="N33" t="n">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="O33"/>
-      <c r="P33"/>
+      <c r="P33" t="n">
+        <v>27</v>
+      </c>
       <c r="Q33"/>
-      <c r="R33"/>
-      <c r="S33"/>
-      <c r="T33"/>
+      <c r="R33" t="n">
+        <v>29</v>
+      </c>
+      <c r="S33" t="n">
+        <v>2</v>
+      </c>
+      <c r="T33" t="n">
+        <v>49</v>
+      </c>
       <c r="U33"/>
       <c r="V33" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="W33"/>
-      <c r="X33"/>
-      <c r="Y33"/>
-      <c r="Z33"/>
-      <c r="AA33"/>
-      <c r="AB33"/>
+      <c r="X33" t="n">
+        <v>19</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>75</v>
+      </c>
       <c r="AC33"/>
-      <c r="AD33"/>
+      <c r="AD33" t="n">
+        <v>102</v>
+      </c>
       <c r="AE33"/>
-      <c r="AF33"/>
+      <c r="AF33" t="n">
+        <v>75</v>
+      </c>
       <c r="AG33"/>
-      <c r="AH33"/>
-      <c r="AI33"/>
-      <c r="AJ33"/>
-      <c r="AK33"/>
-      <c r="AL33"/>
-      <c r="AM33"/>
-      <c r="AN33"/>
-      <c r="AO33"/>
-      <c r="AP33"/>
-      <c r="AQ33"/>
-      <c r="AR33"/>
-      <c r="AS33"/>
-      <c r="AT33"/>
-      <c r="AU33"/>
-      <c r="AV33"/>
+      <c r="AH33" t="n">
+        <v>70</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>41</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM33" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN33" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO33" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP33" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS33" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT33" t="n">
+        <v>7</v>
+      </c>
+      <c r="AU33" t="n">
+        <v>16</v>
+      </c>
+      <c r="AV33" t="n">
+        <v>7</v>
+      </c>
       <c r="AW33"/>
-      <c r="AX33"/>
-      <c r="AY33"/>
+      <c r="AX33" t="n">
+        <v>24</v>
+      </c>
+      <c r="AY33" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
         <v>83</v>
       </c>
-      <c r="B34" t="n">
-        <v>13</v>
-      </c>
+      <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F34"/>
       <c r="G34"/>
       <c r="H34" t="n">
-        <v>46</v>
-      </c>
-      <c r="I34" t="n">
-        <v>7</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="I34"/>
       <c r="J34" t="n">
-        <v>60</v>
-      </c>
-      <c r="K34" t="n">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="K34"/>
       <c r="L34" t="n">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="M34"/>
       <c r="N34" t="n">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="O34"/>
-      <c r="P34" t="n">
-        <v>27</v>
-      </c>
+      <c r="P34"/>
       <c r="Q34"/>
       <c r="R34" t="n">
-        <v>29</v>
-      </c>
-      <c r="S34" t="n">
-        <v>2</v>
-      </c>
-      <c r="T34" t="n">
-        <v>49</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="S34"/>
+      <c r="T34"/>
       <c r="U34"/>
-      <c r="V34" t="n">
-        <v>23</v>
-      </c>
+      <c r="V34"/>
       <c r="W34"/>
-      <c r="X34" t="n">
-        <v>19</v>
-      </c>
-      <c r="Y34" t="n">
-        <v>2</v>
-      </c>
-      <c r="Z34" t="n">
-        <v>31</v>
-      </c>
-      <c r="AA34" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB34" t="n">
-        <v>75</v>
-      </c>
+      <c r="X34"/>
+      <c r="Y34"/>
+      <c r="Z34"/>
+      <c r="AA34"/>
+      <c r="AB34"/>
       <c r="AC34"/>
       <c r="AD34" t="n">
-        <v>102</v>
-      </c>
-      <c r="AE34"/>
-      <c r="AF34" t="n">
-        <v>75</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF34"/>
       <c r="AG34"/>
-      <c r="AH34" t="n">
-        <v>70</v>
-      </c>
-      <c r="AI34" t="n">
-        <v>2</v>
-      </c>
-      <c r="AJ34"/>
-      <c r="AK34" t="n">
-        <v>2</v>
-      </c>
+      <c r="AH34"/>
+      <c r="AI34"/>
+      <c r="AJ34" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK34"/>
       <c r="AL34" t="n">
-        <v>3</v>
-      </c>
-      <c r="AM34" t="n">
-        <v>4</v>
-      </c>
-      <c r="AN34" t="n">
-        <v>4</v>
-      </c>
-      <c r="AO34" t="n">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AM34"/>
+      <c r="AN34"/>
+      <c r="AO34"/>
       <c r="AP34" t="n">
-        <v>4</v>
-      </c>
-      <c r="AQ34" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AQ34"/>
       <c r="AR34" t="n">
-        <v>3</v>
-      </c>
-      <c r="AS34" t="n">
-        <v>4</v>
-      </c>
-      <c r="AT34" t="n">
-        <v>7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="AS34"/>
+      <c r="AT34"/>
       <c r="AU34" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="AV34" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AW34"/>
-      <c r="AX34" t="n">
-        <v>24</v>
-      </c>
-      <c r="AY34" t="n">
-        <v>8</v>
-      </c>
+      <c r="AX34"/>
+      <c r="AY34"/>
     </row>
     <row r="35">
       <c r="A35" t="s">
@@ -3739,179 +3774,98 @@
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="F35"/>
       <c r="G35"/>
-      <c r="H35" t="n">
-        <v>6</v>
-      </c>
+      <c r="H35"/>
       <c r="I35"/>
-      <c r="J35" t="n">
-        <v>6</v>
-      </c>
+      <c r="J35"/>
       <c r="K35"/>
       <c r="L35" t="n">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="M35"/>
-      <c r="N35" t="n">
-        <v>5</v>
-      </c>
+      <c r="N35"/>
       <c r="O35"/>
-      <c r="P35"/>
+      <c r="P35" t="n">
+        <v>11</v>
+      </c>
       <c r="Q35"/>
       <c r="R35" t="n">
+        <v>8</v>
+      </c>
+      <c r="S35"/>
+      <c r="T35" t="n">
         <v>4</v>
       </c>
-      <c r="S35"/>
-      <c r="T35"/>
       <c r="U35"/>
-      <c r="V35"/>
+      <c r="V35" t="n">
+        <v>13</v>
+      </c>
       <c r="W35"/>
-      <c r="X35"/>
+      <c r="X35" t="n">
+        <v>10</v>
+      </c>
       <c r="Y35"/>
-      <c r="Z35"/>
+      <c r="Z35" t="n">
+        <v>8</v>
+      </c>
       <c r="AA35"/>
-      <c r="AB35"/>
+      <c r="AB35" t="n">
+        <v>18</v>
+      </c>
       <c r="AC35"/>
       <c r="AD35" t="n">
-        <v>2</v>
-      </c>
-      <c r="AE35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF35"/>
+        <v>38</v>
+      </c>
+      <c r="AE35"/>
+      <c r="AF35" t="n">
+        <v>23</v>
+      </c>
       <c r="AG35"/>
-      <c r="AH35"/>
-      <c r="AI35"/>
-      <c r="AJ35"/>
+      <c r="AH35" t="n">
+        <v>18</v>
+      </c>
+      <c r="AI35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ35" t="n">
+        <v>24</v>
+      </c>
       <c r="AK35"/>
-      <c r="AL35" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM35"/>
-      <c r="AN35"/>
-      <c r="AO35"/>
-      <c r="AP35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ35"/>
-      <c r="AR35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS35"/>
-      <c r="AT35"/>
+      <c r="AL35"/>
+      <c r="AM35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN35" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO35" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP35"/>
+      <c r="AQ35" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR35"/>
+      <c r="AS35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT35" t="n">
+        <v>5</v>
+      </c>
       <c r="AU35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AV35" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AW35"/>
-      <c r="AX35"/>
-      <c r="AY35"/>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>85</v>
-      </c>
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36" t="n">
-        <v>16</v>
-      </c>
-      <c r="F36"/>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36" t="n">
-        <v>27</v>
-      </c>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36" t="n">
-        <v>11</v>
-      </c>
-      <c r="Q36"/>
-      <c r="R36" t="n">
-        <v>8</v>
-      </c>
-      <c r="S36"/>
-      <c r="T36" t="n">
-        <v>4</v>
-      </c>
-      <c r="U36"/>
-      <c r="V36" t="n">
-        <v>13</v>
-      </c>
-      <c r="W36"/>
-      <c r="X36" t="n">
-        <v>10</v>
-      </c>
-      <c r="Y36"/>
-      <c r="Z36" t="n">
-        <v>8</v>
-      </c>
-      <c r="AA36"/>
-      <c r="AB36" t="n">
-        <v>18</v>
-      </c>
-      <c r="AC36"/>
-      <c r="AD36" t="n">
-        <v>38</v>
-      </c>
-      <c r="AE36"/>
-      <c r="AF36" t="n">
-        <v>23</v>
-      </c>
-      <c r="AG36"/>
-      <c r="AH36" t="n">
-        <v>18</v>
-      </c>
-      <c r="AI36" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ36" t="n">
-        <v>24</v>
-      </c>
-      <c r="AK36"/>
-      <c r="AL36"/>
-      <c r="AM36" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN36" t="n">
-        <v>2</v>
-      </c>
-      <c r="AO36" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP36"/>
-      <c r="AQ36" t="n">
-        <v>2</v>
-      </c>
-      <c r="AR36"/>
-      <c r="AS36" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT36" t="n">
-        <v>5</v>
-      </c>
-      <c r="AU36" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV36" t="n">
-        <v>3</v>
-      </c>
-      <c r="AW36"/>
-      <c r="AX36" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY36" t="n">
+      <c r="AX35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY35" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
19th April 1st update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/state/ncov19state_long.xlsx
+++ b/covid19_data/excel/state/ncov19state_long.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t xml:space="preserve">detectedstate</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t xml:space="preserve">18/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">19/03/2020</t>
@@ -752,10 +755,13 @@
       <c r="AY1" t="s">
         <v>50</v>
       </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
@@ -811,10 +817,11 @@
       <c r="AW2"/>
       <c r="AX2"/>
       <c r="AY2"/>
+      <c r="AZ2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -863,25 +870,26 @@
       <c r="AP3"/>
       <c r="AQ3"/>
       <c r="AR3"/>
-      <c r="AS3" t="n">
-        <v>1</v>
-      </c>
+      <c r="AS3"/>
       <c r="AT3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU3" t="n">
         <v>5</v>
       </c>
-      <c r="AU3" t="n">
-        <v>3</v>
-      </c>
-      <c r="AV3"/>
+      <c r="AV3" t="n">
+        <v>3</v>
+      </c>
       <c r="AW3"/>
-      <c r="AX3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY3"/>
+      <c r="AX3"/>
+      <c r="AY3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B4" t="n">
         <v>67</v>
@@ -956,14 +964,14 @@
       </c>
       <c r="AK4"/>
       <c r="AL4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM4"/>
-      <c r="AN4" t="n">
-        <v>2</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN4"/>
       <c r="AO4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AP4" t="n">
         <v>1</v>
@@ -972,31 +980,34 @@
         <v>1</v>
       </c>
       <c r="AR4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AU4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV4" t="n">
         <v>6</v>
       </c>
-      <c r="AV4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AW4"/>
-      <c r="AX4" t="n">
-        <v>2</v>
-      </c>
+      <c r="AW4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX4"/>
       <c r="AY4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ4" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -1050,10 +1061,11 @@
       <c r="AW5"/>
       <c r="AX5"/>
       <c r="AY5"/>
+      <c r="AZ5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B6" t="n">
         <v>15</v>
@@ -1120,13 +1132,14 @@
       <c r="AV6"/>
       <c r="AW6"/>
       <c r="AX6"/>
-      <c r="AY6" t="n">
+      <c r="AY6"/>
+      <c r="AZ6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -1186,42 +1199,45 @@
         <v>11</v>
       </c>
       <c r="AI7"/>
-      <c r="AJ7"/>
+      <c r="AJ7" t="n">
+        <v>2</v>
+      </c>
       <c r="AK7"/>
       <c r="AL7"/>
       <c r="AM7"/>
       <c r="AN7"/>
-      <c r="AO7" t="n">
-        <v>2</v>
-      </c>
+      <c r="AO7"/>
       <c r="AP7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ7"/>
-      <c r="AR7" t="n">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR7"/>
       <c r="AS7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AT7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AU7" t="n">
         <v>2</v>
       </c>
       <c r="AV7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AW7" t="n">
         <v>4</v>
       </c>
-      <c r="AW7"/>
       <c r="AX7"/>
-      <c r="AY7" t="n">
+      <c r="AY7"/>
+      <c r="AZ7" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -1267,38 +1283,39 @@
       <c r="AI8"/>
       <c r="AJ8"/>
       <c r="AK8"/>
-      <c r="AL8" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL8"/>
       <c r="AM8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN8" t="n">
         <v>4</v>
       </c>
-      <c r="AN8"/>
-      <c r="AO8" t="n">
-        <v>1</v>
-      </c>
+      <c r="AO8"/>
       <c r="AP8" t="n">
         <v>1</v>
       </c>
-      <c r="AQ8"/>
+      <c r="AQ8" t="n">
+        <v>1</v>
+      </c>
       <c r="AR8"/>
       <c r="AS8"/>
-      <c r="AT8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU8"/>
+      <c r="AT8"/>
+      <c r="AU8" t="n">
+        <v>1</v>
+      </c>
       <c r="AV8"/>
       <c r="AW8"/>
-      <c r="AX8" t="n">
+      <c r="AX8"/>
+      <c r="AY8" t="n">
         <v>5</v>
       </c>
-      <c r="AY8" t="n">
+      <c r="AZ8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -1348,36 +1365,37 @@
       <c r="AI9"/>
       <c r="AJ9"/>
       <c r="AK9"/>
-      <c r="AL9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM9"/>
+      <c r="AL9"/>
+      <c r="AM9" t="n">
+        <v>1</v>
+      </c>
       <c r="AN9"/>
       <c r="AO9"/>
       <c r="AP9"/>
       <c r="AQ9"/>
-      <c r="AR9" t="n">
-        <v>2</v>
-      </c>
+      <c r="AR9"/>
       <c r="AS9" t="n">
-        <v>3</v>
-      </c>
-      <c r="AT9"/>
-      <c r="AU9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV9"/>
+        <v>2</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU9"/>
+      <c r="AV9" t="n">
+        <v>1</v>
+      </c>
       <c r="AW9"/>
-      <c r="AX9" t="n">
-        <v>1</v>
-      </c>
+      <c r="AX9"/>
       <c r="AY9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B10" t="n">
         <v>32</v>
@@ -1467,48 +1485,49 @@
       <c r="AK10" t="n">
         <v>1</v>
       </c>
-      <c r="AL10" t="n">
-        <v>3</v>
-      </c>
+      <c r="AL10"/>
       <c r="AM10" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN10" t="n">
         <v>6</v>
       </c>
-      <c r="AN10" t="n">
+      <c r="AO10" t="n">
         <v>7</v>
       </c>
-      <c r="AO10" t="n">
-        <v>1</v>
-      </c>
       <c r="AP10" t="n">
-        <v>2</v>
-      </c>
-      <c r="AQ10"/>
-      <c r="AR10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR10"/>
+      <c r="AS10" t="n">
         <v>5</v>
       </c>
-      <c r="AS10" t="n">
+      <c r="AT10" t="n">
         <v>4</v>
       </c>
-      <c r="AT10" t="n">
-        <v>1</v>
-      </c>
       <c r="AU10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV10" t="n">
         <v>9</v>
       </c>
-      <c r="AV10" t="n">
+      <c r="AW10" t="n">
         <v>23</v>
       </c>
-      <c r="AW10"/>
-      <c r="AX10" t="n">
+      <c r="AX10"/>
+      <c r="AY10" t="n">
         <v>25</v>
       </c>
-      <c r="AY10" t="n">
+      <c r="AZ10" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
@@ -1556,22 +1575,23 @@
       <c r="AO11"/>
       <c r="AP11"/>
       <c r="AQ11"/>
-      <c r="AR11" t="n">
-        <v>3</v>
-      </c>
-      <c r="AS11"/>
+      <c r="AR11"/>
+      <c r="AS11" t="n">
+        <v>3</v>
+      </c>
       <c r="AT11"/>
       <c r="AU11"/>
-      <c r="AV11" t="n">
-        <v>2</v>
-      </c>
-      <c r="AW11"/>
+      <c r="AV11"/>
+      <c r="AW11" t="n">
+        <v>2</v>
+      </c>
       <c r="AX11"/>
       <c r="AY11"/>
+      <c r="AZ11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" t="n">
         <v>13</v>
@@ -1644,49 +1664,52 @@
       </c>
       <c r="AK12"/>
       <c r="AL12" t="n">
-        <v>2</v>
+        <v>173</v>
       </c>
       <c r="AM12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN12" t="n">
         <v>5</v>
       </c>
-      <c r="AN12" t="n">
+      <c r="AO12" t="n">
         <v>7</v>
       </c>
-      <c r="AO12" t="n">
+      <c r="AP12" t="n">
         <v>4</v>
       </c>
-      <c r="AP12" t="n">
+      <c r="AQ12" t="n">
         <v>12</v>
       </c>
-      <c r="AQ12" t="n">
+      <c r="AR12" t="n">
         <v>6</v>
       </c>
-      <c r="AR12" t="n">
-        <v>2</v>
-      </c>
       <c r="AS12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT12" t="n">
         <v>6</v>
       </c>
-      <c r="AT12" t="n">
-        <v>3</v>
-      </c>
       <c r="AU12" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AV12" t="n">
         <v>8</v>
       </c>
-      <c r="AW12"/>
-      <c r="AX12" t="n">
+      <c r="AW12" t="n">
+        <v>8</v>
+      </c>
+      <c r="AX12"/>
+      <c r="AY12" t="n">
         <v>7</v>
       </c>
-      <c r="AY12" t="n">
+      <c r="AZ12" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -1763,21 +1786,19 @@
         <v>2</v>
       </c>
       <c r="AL13"/>
-      <c r="AM13" t="n">
-        <v>2</v>
-      </c>
+      <c r="AM13"/>
       <c r="AN13" t="n">
         <v>2</v>
       </c>
-      <c r="AO13"/>
-      <c r="AP13" t="n">
+      <c r="AO13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP13"/>
+      <c r="AQ13" t="n">
         <v>7</v>
       </c>
-      <c r="AQ13" t="n">
-        <v>2</v>
-      </c>
       <c r="AR13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AS13" t="n">
         <v>1</v>
@@ -1786,20 +1807,23 @@
         <v>1</v>
       </c>
       <c r="AU13" t="n">
-        <v>2</v>
-      </c>
-      <c r="AV13"/>
+        <v>1</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>2</v>
+      </c>
       <c r="AW13"/>
-      <c r="AX13" t="n">
-        <v>1</v>
-      </c>
+      <c r="AX13"/>
       <c r="AY13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ13" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -1853,18 +1877,20 @@
       <c r="AG14"/>
       <c r="AH14"/>
       <c r="AI14"/>
-      <c r="AJ14"/>
+      <c r="AJ14" t="n">
+        <v>3</v>
+      </c>
       <c r="AK14"/>
       <c r="AL14"/>
-      <c r="AM14" t="n">
-        <v>2</v>
-      </c>
-      <c r="AN14"/>
+      <c r="AM14"/>
+      <c r="AN14" t="n">
+        <v>2</v>
+      </c>
       <c r="AO14"/>
-      <c r="AP14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ14"/>
+      <c r="AP14"/>
+      <c r="AQ14" t="n">
+        <v>1</v>
+      </c>
       <c r="AR14"/>
       <c r="AS14"/>
       <c r="AT14"/>
@@ -1873,10 +1899,11 @@
       <c r="AW14"/>
       <c r="AX14"/>
       <c r="AY14"/>
+      <c r="AZ14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B15" t="n">
         <v>7</v>
@@ -1961,35 +1988,36 @@
       <c r="AN15"/>
       <c r="AO15"/>
       <c r="AP15"/>
-      <c r="AQ15" t="n">
-        <v>2</v>
-      </c>
+      <c r="AQ15"/>
       <c r="AR15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS15" t="n">
         <v>5</v>
       </c>
-      <c r="AS15" t="n">
-        <v>3</v>
-      </c>
       <c r="AT15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU15" t="n">
         <v>6</v>
       </c>
-      <c r="AU15" t="n">
+      <c r="AV15" t="n">
         <v>13</v>
       </c>
-      <c r="AV15" t="n">
+      <c r="AW15" t="n">
         <v>5</v>
       </c>
-      <c r="AW15"/>
-      <c r="AX15" t="n">
+      <c r="AX15"/>
+      <c r="AY15" t="n">
         <v>11</v>
       </c>
-      <c r="AY15" t="n">
+      <c r="AZ15" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
@@ -2064,13 +2092,14 @@
       <c r="AV16"/>
       <c r="AW16"/>
       <c r="AX16"/>
-      <c r="AY16" t="n">
+      <c r="AY16"/>
+      <c r="AZ16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B17" t="n">
         <v>9</v>
@@ -2156,48 +2185,49 @@
       <c r="AK17" t="n">
         <v>3</v>
       </c>
-      <c r="AL17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM17"/>
-      <c r="AN17" t="n">
+      <c r="AL17"/>
+      <c r="AM17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN17"/>
+      <c r="AO17" t="n">
         <v>5</v>
       </c>
-      <c r="AO17" t="n">
+      <c r="AP17" t="n">
         <v>6</v>
       </c>
-      <c r="AP17" t="n">
+      <c r="AQ17" t="n">
         <v>7</v>
       </c>
-      <c r="AQ17" t="n">
+      <c r="AR17" t="n">
         <v>8</v>
       </c>
-      <c r="AR17" t="n">
+      <c r="AS17" t="n">
         <v>10</v>
       </c>
-      <c r="AS17" t="n">
+      <c r="AT17" t="n">
         <v>4</v>
       </c>
-      <c r="AT17" t="n">
+      <c r="AU17" t="n">
         <v>9</v>
       </c>
-      <c r="AU17" t="n">
+      <c r="AV17" t="n">
         <v>12</v>
       </c>
-      <c r="AV17" t="n">
+      <c r="AW17" t="n">
         <v>7</v>
       </c>
-      <c r="AW17"/>
-      <c r="AX17" t="n">
+      <c r="AX17"/>
+      <c r="AY17" t="n">
         <v>5</v>
       </c>
-      <c r="AY17" t="n">
+      <c r="AZ17" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B18" t="n">
         <v>24</v>
@@ -2287,52 +2317,53 @@
         <v>1</v>
       </c>
       <c r="AK18"/>
-      <c r="AL18" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL18"/>
       <c r="AM18" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="AN18" t="n">
         <v>12</v>
       </c>
       <c r="AO18" t="n">
+        <v>12</v>
+      </c>
+      <c r="AP18" t="n">
         <v>15</v>
       </c>
-      <c r="AP18" t="n">
+      <c r="AQ18" t="n">
         <v>28</v>
       </c>
-      <c r="AQ18" t="n">
+      <c r="AR18" t="n">
         <v>14</v>
       </c>
-      <c r="AR18" t="n">
+      <c r="AS18" t="n">
         <v>9</v>
       </c>
-      <c r="AS18" t="n">
+      <c r="AT18" t="n">
         <v>19</v>
       </c>
-      <c r="AT18" t="n">
+      <c r="AU18" t="n">
         <v>39</v>
       </c>
-      <c r="AU18" t="n">
+      <c r="AV18" t="n">
         <v>6</v>
       </c>
-      <c r="AV18" t="n">
+      <c r="AW18" t="n">
         <v>20</v>
       </c>
-      <c r="AW18" t="n">
-        <v>1</v>
-      </c>
       <c r="AX18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY18" t="n">
         <v>32</v>
       </c>
-      <c r="AY18" t="n">
+      <c r="AZ18" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B19"/>
       <c r="C19"/>
@@ -2385,13 +2416,13 @@
       <c r="AJ19"/>
       <c r="AK19"/>
       <c r="AL19"/>
-      <c r="AM19" t="n">
-        <v>2</v>
-      </c>
+      <c r="AM19"/>
       <c r="AN19" t="n">
-        <v>3</v>
-      </c>
-      <c r="AO19"/>
+        <v>2</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>3</v>
+      </c>
       <c r="AP19"/>
       <c r="AQ19"/>
       <c r="AR19"/>
@@ -2402,10 +2433,11 @@
       <c r="AW19"/>
       <c r="AX19"/>
       <c r="AY19"/>
+      <c r="AZ19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B20" t="n">
         <v>32</v>
@@ -2477,42 +2509,45 @@
         <v>146</v>
       </c>
       <c r="AK20"/>
-      <c r="AL20"/>
-      <c r="AM20" t="n">
+      <c r="AL20" t="n">
+        <v>45</v>
+      </c>
+      <c r="AM20"/>
+      <c r="AN20" t="n">
         <v>4</v>
       </c>
-      <c r="AN20"/>
-      <c r="AO20" t="n">
-        <v>2</v>
-      </c>
-      <c r="AP20"/>
-      <c r="AQ20" t="n">
-        <v>1</v>
-      </c>
+      <c r="AO20"/>
+      <c r="AP20" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ20"/>
       <c r="AR20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS20" t="n">
         <v>8</v>
       </c>
-      <c r="AS20" t="n">
+      <c r="AT20" t="n">
         <v>5</v>
       </c>
-      <c r="AT20" t="n">
+      <c r="AU20" t="n">
         <v>9</v>
       </c>
-      <c r="AU20" t="n">
+      <c r="AV20" t="n">
         <v>10</v>
       </c>
-      <c r="AV20"/>
       <c r="AW20"/>
-      <c r="AX20" t="n">
+      <c r="AX20"/>
+      <c r="AY20" t="n">
         <v>8</v>
       </c>
-      <c r="AY20" t="n">
+      <c r="AZ20" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B21" t="n">
         <v>33</v>
@@ -2598,54 +2633,57 @@
       <c r="AI21" t="n">
         <v>2</v>
       </c>
-      <c r="AJ21"/>
+      <c r="AJ21" t="n">
+        <v>118</v>
+      </c>
       <c r="AK21" t="n">
         <v>4</v>
       </c>
-      <c r="AL21" t="n">
-        <v>3</v>
-      </c>
+      <c r="AL21"/>
       <c r="AM21" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN21" t="n">
         <v>4</v>
       </c>
-      <c r="AN21" t="n">
+      <c r="AO21" t="n">
         <v>12</v>
       </c>
-      <c r="AO21" t="n">
+      <c r="AP21" t="n">
         <v>10</v>
       </c>
-      <c r="AP21" t="n">
+      <c r="AQ21" t="n">
         <v>15</v>
       </c>
-      <c r="AQ21" t="n">
+      <c r="AR21" t="n">
         <v>18</v>
       </c>
-      <c r="AR21" t="n">
+      <c r="AS21" t="n">
         <v>15</v>
       </c>
-      <c r="AS21" t="n">
-        <v>3</v>
-      </c>
       <c r="AT21" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="AU21" t="n">
         <v>28</v>
       </c>
       <c r="AV21" t="n">
+        <v>28</v>
+      </c>
+      <c r="AW21" t="n">
         <v>22</v>
       </c>
-      <c r="AW21"/>
-      <c r="AX21" t="n">
+      <c r="AX21"/>
+      <c r="AY21" t="n">
         <v>17</v>
       </c>
-      <c r="AY21" t="n">
+      <c r="AZ21" t="n">
         <v>82</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -2690,10 +2728,10 @@
       <c r="AN22"/>
       <c r="AO22"/>
       <c r="AP22"/>
-      <c r="AQ22" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR22"/>
+      <c r="AQ22"/>
+      <c r="AR22" t="n">
+        <v>1</v>
+      </c>
       <c r="AS22"/>
       <c r="AT22"/>
       <c r="AU22"/>
@@ -2701,10 +2739,11 @@
       <c r="AW22"/>
       <c r="AX22"/>
       <c r="AY22"/>
+      <c r="AZ22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -2748,7 +2787,9 @@
       <c r="AI23"/>
       <c r="AJ23"/>
       <c r="AK23"/>
-      <c r="AL23"/>
+      <c r="AL23" t="n">
+        <v>2</v>
+      </c>
       <c r="AM23"/>
       <c r="AN23"/>
       <c r="AO23"/>
@@ -2762,10 +2803,11 @@
       <c r="AW23"/>
       <c r="AX23"/>
       <c r="AY23"/>
+      <c r="AZ23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -2809,20 +2851,21 @@
       <c r="AO24"/>
       <c r="AP24"/>
       <c r="AQ24"/>
-      <c r="AR24" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS24"/>
+      <c r="AR24"/>
+      <c r="AS24" t="n">
+        <v>1</v>
+      </c>
       <c r="AT24"/>
       <c r="AU24"/>
       <c r="AV24"/>
       <c r="AW24"/>
       <c r="AX24"/>
       <c r="AY24"/>
+      <c r="AZ24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B25"/>
       <c r="C25"/>
@@ -2876,10 +2919,11 @@
       <c r="AW25"/>
       <c r="AX25"/>
       <c r="AY25"/>
+      <c r="AZ25"/>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B26" t="n">
         <v>1</v>
@@ -2941,30 +2985,31 @@
       <c r="AI26"/>
       <c r="AJ26"/>
       <c r="AK26"/>
-      <c r="AL26" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM26"/>
+      <c r="AL26"/>
+      <c r="AM26" t="n">
+        <v>1</v>
+      </c>
       <c r="AN26"/>
       <c r="AO26"/>
       <c r="AP26"/>
       <c r="AQ26"/>
       <c r="AR26"/>
-      <c r="AS26" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT26"/>
+      <c r="AS26"/>
+      <c r="AT26" t="n">
+        <v>1</v>
+      </c>
       <c r="AU26"/>
       <c r="AV26"/>
       <c r="AW26"/>
       <c r="AX26"/>
-      <c r="AY26" t="n">
+      <c r="AY26"/>
+      <c r="AZ26" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B27" t="n">
         <v>2</v>
@@ -3024,10 +3069,11 @@
       <c r="AW27"/>
       <c r="AX27"/>
       <c r="AY27"/>
+      <c r="AZ27"/>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B28" t="n">
         <v>4</v>
@@ -3101,46 +3147,47 @@
         <v>14</v>
       </c>
       <c r="AK28"/>
-      <c r="AL28" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL28"/>
       <c r="AM28" t="n">
         <v>1</v>
       </c>
       <c r="AN28" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO28" t="n">
         <v>10</v>
       </c>
-      <c r="AO28" t="n">
+      <c r="AP28" t="n">
         <v>8</v>
       </c>
-      <c r="AP28" t="n">
-        <v>2</v>
-      </c>
       <c r="AQ28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR28" t="n">
         <v>6</v>
       </c>
-      <c r="AR28" t="n">
-        <v>2</v>
-      </c>
       <c r="AS28" t="n">
         <v>2</v>
       </c>
       <c r="AT28" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU28" t="n">
         <v>5</v>
       </c>
-      <c r="AU28"/>
       <c r="AV28"/>
       <c r="AW28"/>
-      <c r="AX28" t="n">
-        <v>3</v>
-      </c>
+      <c r="AX28"/>
       <c r="AY28" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ28" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B29" t="n">
         <v>27</v>
@@ -3223,47 +3270,50 @@
         <v>3</v>
       </c>
       <c r="AL29" t="n">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="AM29" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN29" t="n">
         <v>8</v>
       </c>
-      <c r="AN29" t="n">
+      <c r="AO29" t="n">
         <v>7</v>
       </c>
-      <c r="AO29" t="n">
+      <c r="AP29" t="n">
         <v>5</v>
       </c>
-      <c r="AP29" t="n">
-        <v>3</v>
-      </c>
-      <c r="AQ29"/>
-      <c r="AR29" t="n">
+      <c r="AQ29" t="n">
+        <v>3</v>
+      </c>
+      <c r="AR29"/>
+      <c r="AS29" t="n">
         <v>6</v>
       </c>
-      <c r="AS29" t="n">
+      <c r="AT29" t="n">
         <v>5</v>
       </c>
-      <c r="AT29" t="n">
+      <c r="AU29" t="n">
         <v>7</v>
       </c>
-      <c r="AU29" t="n">
+      <c r="AV29" t="n">
         <v>4</v>
       </c>
-      <c r="AV29" t="n">
+      <c r="AW29" t="n">
         <v>5</v>
       </c>
-      <c r="AW29"/>
-      <c r="AX29" t="n">
+      <c r="AX29"/>
+      <c r="AY29" t="n">
         <v>20</v>
       </c>
-      <c r="AY29" t="n">
+      <c r="AZ29" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B30" t="n">
         <v>110</v>
@@ -3339,13 +3389,11 @@
       <c r="AK30" t="n">
         <v>1</v>
       </c>
-      <c r="AL30" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM30"/>
-      <c r="AN30" t="n">
-        <v>3</v>
-      </c>
+      <c r="AL30"/>
+      <c r="AM30" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN30"/>
       <c r="AO30" t="n">
         <v>3</v>
       </c>
@@ -3353,34 +3401,37 @@
         <v>3</v>
       </c>
       <c r="AQ30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AR30" t="n">
         <v>6</v>
       </c>
-      <c r="AR30" t="n">
+      <c r="AS30" t="n">
         <v>8</v>
       </c>
-      <c r="AS30" t="n">
-        <v>3</v>
-      </c>
       <c r="AT30" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU30" t="n">
         <v>9</v>
       </c>
-      <c r="AU30" t="n">
+      <c r="AV30" t="n">
         <v>4</v>
       </c>
-      <c r="AV30" t="n">
+      <c r="AW30" t="n">
         <v>8</v>
       </c>
-      <c r="AW30"/>
-      <c r="AX30" t="n">
+      <c r="AX30"/>
+      <c r="AY30" t="n">
         <v>17</v>
       </c>
-      <c r="AY30" t="n">
+      <c r="AZ30" t="n">
         <v>57</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B31" t="n">
         <v>30</v>
@@ -3464,17 +3515,15 @@
       <c r="AK31" t="n">
         <v>8</v>
       </c>
-      <c r="AL31" t="n">
-        <v>3</v>
-      </c>
+      <c r="AL31"/>
       <c r="AM31" t="n">
         <v>3</v>
       </c>
       <c r="AN31" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AO31" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AP31" t="n">
         <v>6</v>
@@ -3483,31 +3532,34 @@
         <v>6</v>
       </c>
       <c r="AR31" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AS31" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT31" t="n">
         <v>4</v>
       </c>
-      <c r="AT31" t="n">
+      <c r="AU31" t="n">
         <v>14</v>
       </c>
-      <c r="AU31" t="n">
+      <c r="AV31" t="n">
         <v>8</v>
       </c>
-      <c r="AV31" t="n">
-        <v>3</v>
-      </c>
-      <c r="AW31"/>
-      <c r="AX31" t="n">
+      <c r="AW31" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX31"/>
+      <c r="AY31" t="n">
         <v>7</v>
       </c>
-      <c r="AY31" t="n">
+      <c r="AZ31" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B32"/>
       <c r="C32"/>
@@ -3563,10 +3615,11 @@
       <c r="AW32"/>
       <c r="AX32"/>
       <c r="AY32"/>
+      <c r="AZ32"/>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B33" t="n">
         <v>13</v>
@@ -3652,50 +3705,51 @@
       <c r="AK33" t="n">
         <v>2</v>
       </c>
-      <c r="AL33" t="n">
-        <v>3</v>
-      </c>
+      <c r="AL33"/>
       <c r="AM33" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AN33" t="n">
         <v>4</v>
       </c>
       <c r="AO33" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AP33" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ33" t="n">
         <v>4</v>
       </c>
-      <c r="AQ33" t="n">
-        <v>1</v>
-      </c>
       <c r="AR33" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AS33" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT33" t="n">
         <v>4</v>
       </c>
-      <c r="AT33" t="n">
+      <c r="AU33" t="n">
         <v>7</v>
       </c>
-      <c r="AU33" t="n">
+      <c r="AV33" t="n">
         <v>16</v>
       </c>
-      <c r="AV33" t="n">
+      <c r="AW33" t="n">
         <v>7</v>
       </c>
-      <c r="AW33"/>
-      <c r="AX33" t="n">
+      <c r="AX33"/>
+      <c r="AY33" t="n">
         <v>24</v>
       </c>
-      <c r="AY33" t="n">
+      <c r="AZ33" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B34"/>
       <c r="C34"/>
@@ -3751,34 +3805,35 @@
         <v>3</v>
       </c>
       <c r="AK34"/>
-      <c r="AL34" t="n">
-        <v>2</v>
-      </c>
-      <c r="AM34"/>
+      <c r="AL34"/>
+      <c r="AM34" t="n">
+        <v>2</v>
+      </c>
       <c r="AN34"/>
       <c r="AO34"/>
-      <c r="AP34" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ34"/>
-      <c r="AR34" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS34"/>
+      <c r="AP34"/>
+      <c r="AQ34" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR34"/>
+      <c r="AS34" t="n">
+        <v>1</v>
+      </c>
       <c r="AT34"/>
-      <c r="AU34" t="n">
-        <v>1</v>
-      </c>
+      <c r="AU34"/>
       <c r="AV34" t="n">
         <v>1</v>
       </c>
-      <c r="AW34"/>
+      <c r="AW34" t="n">
+        <v>1</v>
+      </c>
       <c r="AX34"/>
       <c r="AY34"/>
+      <c r="AZ34"/>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B35"/>
       <c r="C35"/>
@@ -3844,38 +3899,41 @@
         <v>24</v>
       </c>
       <c r="AK35"/>
-      <c r="AL35"/>
-      <c r="AM35" t="n">
-        <v>1</v>
-      </c>
+      <c r="AL35" t="n">
+        <v>32</v>
+      </c>
+      <c r="AM35"/>
       <c r="AN35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AO35" t="n">
-        <v>3</v>
-      </c>
-      <c r="AP35"/>
-      <c r="AQ35" t="n">
-        <v>2</v>
-      </c>
-      <c r="AR35"/>
-      <c r="AS35" t="n">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AP35" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ35"/>
+      <c r="AR35" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS35"/>
       <c r="AT35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU35" t="n">
         <v>5</v>
       </c>
-      <c r="AU35" t="n">
-        <v>3</v>
-      </c>
       <c r="AV35" t="n">
         <v>3</v>
       </c>
-      <c r="AW35"/>
-      <c r="AX35" t="n">
-        <v>1</v>
-      </c>
+      <c r="AW35" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX35"/>
       <c r="AY35" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ35" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2nd update 24th April
</commit_message>
<xml_diff>
--- a/covid19_data/excel/state/ncov19state_long.xlsx
+++ b/covid19_data/excel/state/ncov19state_long.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t xml:space="preserve">detectedstate</t>
   </si>
@@ -155,7 +155,13 @@
     <t xml:space="preserve">23/03/2020</t>
   </si>
   <si>
+    <t xml:space="preserve">23/04/2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">24/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">25/03/2020</t>
@@ -779,10 +785,16 @@
       <c r="BD1" t="s">
         <v>55</v>
       </c>
+      <c r="BE1" t="s">
+        <v>56</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
@@ -836,17 +848,21 @@
       <c r="AU2"/>
       <c r="AV2"/>
       <c r="AW2"/>
-      <c r="AX2"/>
+      <c r="AX2" t="n">
+        <v>108</v>
+      </c>
       <c r="AY2"/>
       <c r="AZ2"/>
       <c r="BA2"/>
       <c r="BB2"/>
       <c r="BC2"/>
       <c r="BD2"/>
+      <c r="BE2"/>
+      <c r="BF2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -904,29 +920,37 @@
         <v>1</v>
       </c>
       <c r="AS3"/>
-      <c r="AT3"/>
+      <c r="AT3" t="n">
+        <v>1</v>
+      </c>
       <c r="AU3"/>
-      <c r="AV3"/>
+      <c r="AV3" t="n">
+        <v>4</v>
+      </c>
       <c r="AW3"/>
       <c r="AX3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY3" t="n">
         <v>5</v>
       </c>
+      <c r="AY3"/>
       <c r="AZ3" t="n">
-        <v>3</v>
-      </c>
-      <c r="BA3"/>
-      <c r="BB3"/>
-      <c r="BC3" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>5</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>3</v>
+      </c>
+      <c r="BC3"/>
       <c r="BD3"/>
+      <c r="BE3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B4" t="n">
         <v>67</v>
@@ -1022,39 +1046,47 @@
       <c r="AS4" t="n">
         <v>1</v>
       </c>
-      <c r="AT4"/>
+      <c r="AT4" t="n">
+        <v>56</v>
+      </c>
       <c r="AU4" t="n">
         <v>1</v>
       </c>
       <c r="AV4" t="n">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="AW4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AX4" t="n">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="AY4" t="n">
         <v>2</v>
       </c>
       <c r="AZ4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BB4" t="n">
         <v>6</v>
       </c>
-      <c r="BA4" t="n">
-        <v>2</v>
-      </c>
-      <c r="BB4"/>
       <c r="BC4" t="n">
         <v>2</v>
       </c>
-      <c r="BD4" t="n">
+      <c r="BD4"/>
+      <c r="BE4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BF4" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -1113,10 +1145,12 @@
       <c r="BB5"/>
       <c r="BC5"/>
       <c r="BD5"/>
+      <c r="BE5"/>
+      <c r="BF5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B6" t="n">
         <v>15</v>
@@ -1182,7 +1216,9 @@
       <c r="AS6"/>
       <c r="AT6"/>
       <c r="AU6"/>
-      <c r="AV6"/>
+      <c r="AV6" t="n">
+        <v>1</v>
+      </c>
       <c r="AW6"/>
       <c r="AX6"/>
       <c r="AY6"/>
@@ -1190,13 +1226,15 @@
       <c r="BA6"/>
       <c r="BB6"/>
       <c r="BC6"/>
-      <c r="BD6" t="n">
+      <c r="BD6"/>
+      <c r="BE6"/>
+      <c r="BF6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -1278,35 +1316,43 @@
       <c r="AS7" t="n">
         <v>2</v>
       </c>
-      <c r="AT7"/>
+      <c r="AT7" t="n">
+        <v>17</v>
+      </c>
       <c r="AU7" t="n">
         <v>1</v>
       </c>
-      <c r="AV7"/>
-      <c r="AW7" t="n">
-        <v>1</v>
-      </c>
+      <c r="AV7" t="n">
+        <v>27</v>
+      </c>
+      <c r="AW7"/>
       <c r="AX7" t="n">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="AY7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AZ7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BA7" t="n">
+        <v>2</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>2</v>
+      </c>
+      <c r="BC7" t="n">
         <v>4</v>
       </c>
-      <c r="BB7"/>
-      <c r="BC7"/>
-      <c r="BD7" t="n">
+      <c r="BD7"/>
+      <c r="BE7"/>
+      <c r="BF7" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -1379,22 +1425,24 @@
       <c r="AV8"/>
       <c r="AW8"/>
       <c r="AX8"/>
-      <c r="AY8" t="n">
-        <v>1</v>
-      </c>
+      <c r="AY8"/>
       <c r="AZ8"/>
-      <c r="BA8"/>
+      <c r="BA8" t="n">
+        <v>1</v>
+      </c>
       <c r="BB8"/>
-      <c r="BC8" t="n">
+      <c r="BC8"/>
+      <c r="BD8"/>
+      <c r="BE8" t="n">
         <v>5</v>
       </c>
-      <c r="BD8" t="n">
+      <c r="BF8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -1457,28 +1505,30 @@
       <c r="AT9"/>
       <c r="AU9"/>
       <c r="AV9"/>
-      <c r="AW9" t="n">
-        <v>2</v>
-      </c>
-      <c r="AX9" t="n">
-        <v>3</v>
-      </c>
-      <c r="AY9"/>
+      <c r="AW9"/>
+      <c r="AX9"/>
+      <c r="AY9" t="n">
+        <v>2</v>
+      </c>
       <c r="AZ9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="BA9"/>
-      <c r="BB9"/>
-      <c r="BC9" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD9" t="n">
+      <c r="BB9" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC9"/>
+      <c r="BD9"/>
+      <c r="BE9" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B10" t="n">
         <v>32</v>
@@ -1592,37 +1642,43 @@
       <c r="AS10" t="n">
         <v>1</v>
       </c>
-      <c r="AT10"/>
+      <c r="AT10" t="n">
+        <v>92</v>
+      </c>
       <c r="AU10" t="n">
         <v>2</v>
       </c>
-      <c r="AV10"/>
-      <c r="AW10" t="n">
+      <c r="AV10" t="n">
+        <v>128</v>
+      </c>
+      <c r="AW10"/>
+      <c r="AX10"/>
+      <c r="AY10" t="n">
         <v>5</v>
       </c>
-      <c r="AX10" t="n">
+      <c r="AZ10" t="n">
         <v>4</v>
       </c>
-      <c r="AY10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ10" t="n">
+      <c r="BA10" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB10" t="n">
         <v>9</v>
       </c>
-      <c r="BA10" t="n">
+      <c r="BC10" t="n">
         <v>23</v>
       </c>
-      <c r="BB10"/>
-      <c r="BC10" t="n">
+      <c r="BD10"/>
+      <c r="BE10" t="n">
         <v>25</v>
       </c>
-      <c r="BD10" t="n">
+      <c r="BF10" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
@@ -1675,22 +1731,24 @@
       <c r="AT11"/>
       <c r="AU11"/>
       <c r="AV11"/>
-      <c r="AW11" t="n">
-        <v>3</v>
-      </c>
+      <c r="AW11"/>
       <c r="AX11"/>
-      <c r="AY11"/>
+      <c r="AY11" t="n">
+        <v>3</v>
+      </c>
       <c r="AZ11"/>
-      <c r="BA11" t="n">
-        <v>2</v>
-      </c>
+      <c r="BA11"/>
       <c r="BB11"/>
-      <c r="BC11"/>
+      <c r="BC11" t="n">
+        <v>2</v>
+      </c>
       <c r="BD11"/>
+      <c r="BE11"/>
+      <c r="BF11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B12" t="n">
         <v>13</v>
@@ -1786,39 +1844,47 @@
       <c r="AS12" t="n">
         <v>4</v>
       </c>
-      <c r="AT12"/>
+      <c r="AT12" t="n">
+        <v>229</v>
+      </c>
       <c r="AU12" t="n">
         <v>12</v>
       </c>
       <c r="AV12" t="n">
+        <v>217</v>
+      </c>
+      <c r="AW12" t="n">
         <v>6</v>
       </c>
-      <c r="AW12" t="n">
-        <v>2</v>
-      </c>
       <c r="AX12" t="n">
+        <v>191</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ12" t="n">
         <v>6</v>
       </c>
-      <c r="AY12" t="n">
-        <v>3</v>
-      </c>
-      <c r="AZ12" t="n">
+      <c r="BA12" t="n">
+        <v>3</v>
+      </c>
+      <c r="BB12" t="n">
         <v>8</v>
       </c>
-      <c r="BA12" t="n">
+      <c r="BC12" t="n">
         <v>8</v>
       </c>
-      <c r="BB12"/>
-      <c r="BC12" t="n">
+      <c r="BD12"/>
+      <c r="BE12" t="n">
         <v>7</v>
       </c>
-      <c r="BD12" t="n">
+      <c r="BF12" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -1914,37 +1980,45 @@
         <v>4</v>
       </c>
       <c r="AS13"/>
-      <c r="AT13"/>
+      <c r="AT13" t="n">
+        <v>9</v>
+      </c>
       <c r="AU13" t="n">
         <v>7</v>
       </c>
       <c r="AV13" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AW13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AX13" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AY13" t="n">
         <v>1</v>
       </c>
       <c r="AZ13" t="n">
-        <v>2</v>
-      </c>
-      <c r="BA13"/>
-      <c r="BB13"/>
-      <c r="BC13" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD13" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA13" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB13" t="n">
+        <v>2</v>
+      </c>
+      <c r="BC13"/>
+      <c r="BD13"/>
+      <c r="BE13" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF13" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -2018,7 +2092,9 @@
       <c r="AU14" t="n">
         <v>1</v>
       </c>
-      <c r="AV14"/>
+      <c r="AV14" t="n">
+        <v>1</v>
+      </c>
       <c r="AW14"/>
       <c r="AX14"/>
       <c r="AY14"/>
@@ -2027,10 +2103,12 @@
       <c r="BB14"/>
       <c r="BC14"/>
       <c r="BD14"/>
+      <c r="BE14"/>
+      <c r="BF14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B15" t="n">
         <v>7</v>
@@ -2126,37 +2204,45 @@
         <v>12</v>
       </c>
       <c r="AS15"/>
-      <c r="AT15"/>
+      <c r="AT15" t="n">
+        <v>27</v>
+      </c>
       <c r="AU15"/>
       <c r="AV15" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="AW15" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX15" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY15" t="n">
         <v>5</v>
       </c>
-      <c r="AX15" t="n">
-        <v>3</v>
-      </c>
-      <c r="AY15" t="n">
+      <c r="AZ15" t="n">
+        <v>3</v>
+      </c>
+      <c r="BA15" t="n">
         <v>6</v>
       </c>
-      <c r="AZ15" t="n">
+      <c r="BB15" t="n">
         <v>13</v>
       </c>
-      <c r="BA15" t="n">
+      <c r="BC15" t="n">
         <v>5</v>
       </c>
-      <c r="BB15"/>
-      <c r="BC15" t="n">
+      <c r="BD15"/>
+      <c r="BE15" t="n">
         <v>11</v>
       </c>
-      <c r="BD15" t="n">
+      <c r="BF15" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
@@ -2234,21 +2320,27 @@
       <c r="AS16"/>
       <c r="AT16"/>
       <c r="AU16"/>
-      <c r="AV16"/>
+      <c r="AV16" t="n">
+        <v>7</v>
+      </c>
       <c r="AW16"/>
-      <c r="AX16"/>
+      <c r="AX16" t="n">
+        <v>4</v>
+      </c>
       <c r="AY16"/>
       <c r="AZ16"/>
       <c r="BA16"/>
       <c r="BB16"/>
       <c r="BC16"/>
-      <c r="BD16" t="n">
+      <c r="BD16"/>
+      <c r="BE16"/>
+      <c r="BF16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B17" t="n">
         <v>9</v>
@@ -2356,39 +2448,47 @@
       <c r="AS17" t="n">
         <v>6</v>
       </c>
-      <c r="AT17"/>
+      <c r="AT17" t="n">
+        <v>9</v>
+      </c>
       <c r="AU17" t="n">
         <v>7</v>
       </c>
       <c r="AV17" t="n">
+        <v>18</v>
+      </c>
+      <c r="AW17" t="n">
         <v>8</v>
       </c>
-      <c r="AW17" t="n">
+      <c r="AX17" t="n">
+        <v>29</v>
+      </c>
+      <c r="AY17" t="n">
         <v>10</v>
       </c>
-      <c r="AX17" t="n">
+      <c r="AZ17" t="n">
         <v>4</v>
       </c>
-      <c r="AY17" t="n">
+      <c r="BA17" t="n">
         <v>9</v>
       </c>
-      <c r="AZ17" t="n">
+      <c r="BB17" t="n">
         <v>12</v>
       </c>
-      <c r="BA17" t="n">
+      <c r="BC17" t="n">
         <v>7</v>
       </c>
-      <c r="BB17"/>
-      <c r="BC17" t="n">
+      <c r="BD17"/>
+      <c r="BE17" t="n">
         <v>5</v>
       </c>
-      <c r="BD17" t="n">
+      <c r="BF17" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B18" t="n">
         <v>24</v>
@@ -2502,41 +2602,49 @@
       <c r="AS18" t="n">
         <v>15</v>
       </c>
-      <c r="AT18"/>
+      <c r="AT18" t="n">
+        <v>11</v>
+      </c>
       <c r="AU18" t="n">
         <v>28</v>
       </c>
       <c r="AV18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AW18" t="n">
         <v>14</v>
       </c>
-      <c r="AW18" t="n">
+      <c r="AX18" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY18" t="n">
         <v>9</v>
       </c>
-      <c r="AX18" t="n">
+      <c r="AZ18" t="n">
         <v>19</v>
       </c>
-      <c r="AY18" t="n">
+      <c r="BA18" t="n">
         <v>39</v>
       </c>
-      <c r="AZ18" t="n">
+      <c r="BB18" t="n">
         <v>6</v>
       </c>
-      <c r="BA18" t="n">
+      <c r="BC18" t="n">
         <v>20</v>
       </c>
-      <c r="BB18" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC18" t="n">
+      <c r="BD18" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE18" t="n">
         <v>32</v>
       </c>
-      <c r="BD18" t="n">
+      <c r="BF18" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B19"/>
       <c r="C19"/>
@@ -2611,10 +2719,12 @@
       <c r="BB19"/>
       <c r="BC19"/>
       <c r="BD19"/>
+      <c r="BE19"/>
+      <c r="BF19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B20" t="n">
         <v>32</v>
@@ -2706,35 +2816,43 @@
       <c r="AS20" t="n">
         <v>2</v>
       </c>
-      <c r="AT20"/>
+      <c r="AT20" t="n">
+        <v>35</v>
+      </c>
       <c r="AU20"/>
       <c r="AV20" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="AW20" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX20" t="n">
+        <v>159</v>
+      </c>
+      <c r="AY20" t="n">
         <v>8</v>
       </c>
-      <c r="AX20" t="n">
+      <c r="AZ20" t="n">
         <v>5</v>
       </c>
-      <c r="AY20" t="n">
+      <c r="BA20" t="n">
         <v>9</v>
       </c>
-      <c r="AZ20" t="n">
+      <c r="BB20" t="n">
         <v>10</v>
       </c>
-      <c r="BA20"/>
-      <c r="BB20"/>
-      <c r="BC20" t="n">
+      <c r="BC20"/>
+      <c r="BD20"/>
+      <c r="BE20" t="n">
         <v>8</v>
       </c>
-      <c r="BD20" t="n">
+      <c r="BF20" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B21" t="n">
         <v>33</v>
@@ -2850,39 +2968,47 @@
       <c r="AS21" t="n">
         <v>10</v>
       </c>
-      <c r="AT21"/>
+      <c r="AT21" t="n">
+        <v>431</v>
+      </c>
       <c r="AU21" t="n">
         <v>15</v>
       </c>
       <c r="AV21" t="n">
+        <v>778</v>
+      </c>
+      <c r="AW21" t="n">
         <v>18</v>
       </c>
-      <c r="AW21" t="n">
+      <c r="AX21" t="n">
+        <v>390</v>
+      </c>
+      <c r="AY21" t="n">
         <v>15</v>
       </c>
-      <c r="AX21" t="n">
-        <v>3</v>
-      </c>
-      <c r="AY21" t="n">
+      <c r="AZ21" t="n">
+        <v>3</v>
+      </c>
+      <c r="BA21" t="n">
         <v>28</v>
       </c>
-      <c r="AZ21" t="n">
+      <c r="BB21" t="n">
         <v>28</v>
       </c>
-      <c r="BA21" t="n">
+      <c r="BC21" t="n">
         <v>22</v>
       </c>
-      <c r="BB21"/>
-      <c r="BC21" t="n">
+      <c r="BD21"/>
+      <c r="BE21" t="n">
         <v>17</v>
       </c>
-      <c r="BD21" t="n">
+      <c r="BF21" t="n">
         <v>82</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -2932,10 +3058,10 @@
       <c r="AS22"/>
       <c r="AT22"/>
       <c r="AU22"/>
-      <c r="AV22" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW22"/>
+      <c r="AV22"/>
+      <c r="AW22" t="n">
+        <v>1</v>
+      </c>
       <c r="AX22"/>
       <c r="AY22"/>
       <c r="AZ22"/>
@@ -2943,10 +3069,12 @@
       <c r="BB22"/>
       <c r="BC22"/>
       <c r="BD22"/>
+      <c r="BE22"/>
+      <c r="BF22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -3013,10 +3141,12 @@
       <c r="BB23"/>
       <c r="BC23"/>
       <c r="BD23"/>
+      <c r="BE23"/>
+      <c r="BF23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -3065,20 +3195,22 @@
       <c r="AT24"/>
       <c r="AU24"/>
       <c r="AV24"/>
-      <c r="AW24" t="n">
-        <v>1</v>
-      </c>
+      <c r="AW24"/>
       <c r="AX24"/>
-      <c r="AY24"/>
+      <c r="AY24" t="n">
+        <v>1</v>
+      </c>
       <c r="AZ24"/>
       <c r="BA24"/>
       <c r="BB24"/>
       <c r="BC24"/>
       <c r="BD24"/>
+      <c r="BE24"/>
+      <c r="BF24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B25" t="n">
         <v>1</v>
@@ -3157,26 +3289,32 @@
       </c>
       <c r="AS25"/>
       <c r="AT25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AU25"/>
-      <c r="AV25"/>
+      <c r="AV25" t="n">
+        <v>6</v>
+      </c>
       <c r="AW25"/>
       <c r="AX25" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AY25"/>
-      <c r="AZ25"/>
+      <c r="AZ25" t="n">
+        <v>1</v>
+      </c>
       <c r="BA25"/>
       <c r="BB25"/>
       <c r="BC25"/>
-      <c r="BD25" t="n">
+      <c r="BD25"/>
+      <c r="BE25"/>
+      <c r="BF25" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B26" t="n">
         <v>2</v>
@@ -3241,10 +3379,12 @@
       <c r="BB26"/>
       <c r="BC26"/>
       <c r="BD26"/>
+      <c r="BE26"/>
+      <c r="BF26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B27" t="n">
         <v>4</v>
@@ -3342,35 +3482,43 @@
       <c r="AS27" t="n">
         <v>8</v>
       </c>
-      <c r="AT27"/>
+      <c r="AT27" t="n">
+        <v>27</v>
+      </c>
       <c r="AU27" t="n">
         <v>2</v>
       </c>
       <c r="AV27" t="n">
+        <v>5</v>
+      </c>
+      <c r="AW27" t="n">
         <v>6</v>
       </c>
-      <c r="AW27" t="n">
-        <v>2</v>
-      </c>
       <c r="AX27" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="AY27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ27" t="n">
+        <v>2</v>
+      </c>
+      <c r="BA27" t="n">
         <v>5</v>
       </c>
-      <c r="AZ27"/>
-      <c r="BA27"/>
       <c r="BB27"/>
-      <c r="BC27" t="n">
-        <v>3</v>
-      </c>
-      <c r="BD27" t="n">
+      <c r="BC27"/>
+      <c r="BD27"/>
+      <c r="BE27" t="n">
+        <v>3</v>
+      </c>
+      <c r="BF27" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B28" t="n">
         <v>27</v>
@@ -3476,37 +3624,45 @@
       <c r="AS28" t="n">
         <v>5</v>
       </c>
-      <c r="AT28"/>
+      <c r="AT28" t="n">
+        <v>153</v>
+      </c>
       <c r="AU28" t="n">
         <v>3</v>
       </c>
-      <c r="AV28"/>
-      <c r="AW28" t="n">
+      <c r="AV28" t="n">
+        <v>76</v>
+      </c>
+      <c r="AW28"/>
+      <c r="AX28" t="n">
+        <v>44</v>
+      </c>
+      <c r="AY28" t="n">
         <v>6</v>
       </c>
-      <c r="AX28" t="n">
+      <c r="AZ28" t="n">
         <v>5</v>
       </c>
-      <c r="AY28" t="n">
+      <c r="BA28" t="n">
         <v>7</v>
       </c>
-      <c r="AZ28" t="n">
+      <c r="BB28" t="n">
         <v>4</v>
       </c>
-      <c r="BA28" t="n">
+      <c r="BC28" t="n">
         <v>5</v>
       </c>
-      <c r="BB28"/>
-      <c r="BC28" t="n">
+      <c r="BD28"/>
+      <c r="BE28" t="n">
         <v>20</v>
       </c>
-      <c r="BD28" t="n">
+      <c r="BF28" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B29" t="n">
         <v>110</v>
@@ -3604,39 +3760,47 @@
       <c r="AS29" t="n">
         <v>3</v>
       </c>
-      <c r="AT29"/>
+      <c r="AT29" t="n">
+        <v>33</v>
+      </c>
       <c r="AU29" t="n">
         <v>3</v>
       </c>
       <c r="AV29" t="n">
+        <v>54</v>
+      </c>
+      <c r="AW29" t="n">
         <v>6</v>
       </c>
-      <c r="AW29" t="n">
+      <c r="AX29" t="n">
+        <v>72</v>
+      </c>
+      <c r="AY29" t="n">
         <v>8</v>
       </c>
-      <c r="AX29" t="n">
-        <v>3</v>
-      </c>
-      <c r="AY29" t="n">
+      <c r="AZ29" t="n">
+        <v>3</v>
+      </c>
+      <c r="BA29" t="n">
         <v>9</v>
       </c>
-      <c r="AZ29" t="n">
+      <c r="BB29" t="n">
         <v>4</v>
       </c>
-      <c r="BA29" t="n">
+      <c r="BC29" t="n">
         <v>8</v>
       </c>
-      <c r="BB29"/>
-      <c r="BC29" t="n">
+      <c r="BD29"/>
+      <c r="BE29" t="n">
         <v>17</v>
       </c>
-      <c r="BD29" t="n">
+      <c r="BF29" t="n">
         <v>57</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B30" t="n">
         <v>30</v>
@@ -3744,39 +3908,45 @@
       <c r="AS30" t="n">
         <v>6</v>
       </c>
-      <c r="AT30"/>
+      <c r="AT30" t="n">
+        <v>15</v>
+      </c>
       <c r="AU30" t="n">
         <v>6</v>
       </c>
       <c r="AV30" t="n">
+        <v>27</v>
+      </c>
+      <c r="AW30" t="n">
         <v>6</v>
       </c>
-      <c r="AW30" t="n">
-        <v>2</v>
-      </c>
-      <c r="AX30" t="n">
+      <c r="AX30"/>
+      <c r="AY30" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ30" t="n">
         <v>4</v>
       </c>
-      <c r="AY30" t="n">
+      <c r="BA30" t="n">
         <v>14</v>
       </c>
-      <c r="AZ30" t="n">
+      <c r="BB30" t="n">
         <v>8</v>
       </c>
-      <c r="BA30" t="n">
-        <v>3</v>
-      </c>
-      <c r="BB30"/>
       <c r="BC30" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD30"/>
+      <c r="BE30" t="n">
         <v>7</v>
       </c>
-      <c r="BD30" t="n">
+      <c r="BF30" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -3837,10 +4007,12 @@
       <c r="BB31"/>
       <c r="BC31"/>
       <c r="BD31"/>
+      <c r="BE31"/>
+      <c r="BF31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B32" t="n">
         <v>13</v>
@@ -3950,39 +4122,47 @@
       <c r="AS32" t="n">
         <v>2</v>
       </c>
-      <c r="AT32"/>
+      <c r="AT32" t="n">
+        <v>112</v>
+      </c>
       <c r="AU32" t="n">
         <v>4</v>
       </c>
       <c r="AV32" t="n">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="AW32" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AX32" t="n">
+        <v>111</v>
+      </c>
+      <c r="AY32" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ32" t="n">
         <v>4</v>
-      </c>
-      <c r="AY32" t="n">
-        <v>7</v>
-      </c>
-      <c r="AZ32" t="n">
-        <v>16</v>
       </c>
       <c r="BA32" t="n">
         <v>7</v>
       </c>
-      <c r="BB32"/>
+      <c r="BB32" t="n">
+        <v>16</v>
+      </c>
       <c r="BC32" t="n">
+        <v>7</v>
+      </c>
+      <c r="BD32"/>
+      <c r="BE32" t="n">
         <v>24</v>
       </c>
-      <c r="BD32" t="n">
+      <c r="BF32" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
@@ -4058,25 +4238,31 @@
       <c r="AU33" t="n">
         <v>1</v>
       </c>
-      <c r="AV33"/>
-      <c r="AW33" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX33"/>
-      <c r="AY33"/>
-      <c r="AZ33" t="n">
-        <v>1</v>
-      </c>
-      <c r="BA33" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB33"/>
-      <c r="BC33"/>
+      <c r="AV33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW33"/>
+      <c r="AX33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY33" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ33"/>
+      <c r="BA33"/>
+      <c r="BB33" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC33" t="n">
+        <v>1</v>
+      </c>
       <c r="BD33"/>
+      <c r="BE33"/>
+      <c r="BF33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B34"/>
       <c r="C34"/>
@@ -4169,26 +4355,32 @@
       </c>
       <c r="AU34"/>
       <c r="AV34" t="n">
-        <v>2</v>
-      </c>
-      <c r="AW34"/>
+        <v>33</v>
+      </c>
+      <c r="AW34" t="n">
+        <v>2</v>
+      </c>
       <c r="AX34" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY34" t="n">
+        <v>58</v>
+      </c>
+      <c r="AY34"/>
+      <c r="AZ34" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA34" t="n">
         <v>5</v>
       </c>
-      <c r="AZ34" t="n">
-        <v>3</v>
-      </c>
-      <c r="BA34" t="n">
-        <v>3</v>
-      </c>
-      <c r="BB34"/>
+      <c r="BB34" t="n">
+        <v>3</v>
+      </c>
       <c r="BC34" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD34" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD34"/>
+      <c r="BE34" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF34" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
25th April 2nd update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/state/ncov19state_long.xlsx
+++ b/covid19_data/excel/state/ncov19state_long.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t xml:space="preserve">detectedstate</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t xml:space="preserve">25/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">26/03/2020</t>
@@ -791,10 +794,13 @@
       <c r="BF1" t="s">
         <v>57</v>
       </c>
+      <c r="BG1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
@@ -848,9 +854,7 @@
       <c r="AU2"/>
       <c r="AV2"/>
       <c r="AW2"/>
-      <c r="AX2" t="n">
-        <v>108</v>
-      </c>
+      <c r="AX2"/>
       <c r="AY2"/>
       <c r="AZ2"/>
       <c r="BA2"/>
@@ -859,10 +863,11 @@
       <c r="BD2"/>
       <c r="BE2"/>
       <c r="BF2"/>
+      <c r="BG2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -929,28 +934,29 @@
       </c>
       <c r="AW3"/>
       <c r="AX3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AY3"/>
+      <c r="AZ3"/>
+      <c r="BA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB3" t="n">
         <v>5</v>
       </c>
-      <c r="AY3"/>
-      <c r="AZ3" t="n">
-        <v>1</v>
-      </c>
-      <c r="BA3" t="n">
-        <v>5</v>
-      </c>
-      <c r="BB3" t="n">
-        <v>3</v>
-      </c>
-      <c r="BC3"/>
+      <c r="BC3" t="n">
+        <v>3</v>
+      </c>
       <c r="BD3"/>
-      <c r="BE3" t="n">
-        <v>1</v>
-      </c>
-      <c r="BF3"/>
+      <c r="BE3"/>
+      <c r="BF3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" t="n">
         <v>67</v>
@@ -1065,28 +1071,31 @@
         <v>2</v>
       </c>
       <c r="AZ4" t="n">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="BA4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BB4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BC4" t="n">
         <v>6</v>
       </c>
-      <c r="BC4" t="n">
-        <v>2</v>
-      </c>
-      <c r="BD4"/>
-      <c r="BE4" t="n">
-        <v>2</v>
-      </c>
+      <c r="BD4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BE4"/>
       <c r="BF4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BG4" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -1147,10 +1156,11 @@
       <c r="BD5"/>
       <c r="BE5"/>
       <c r="BF5"/>
+      <c r="BG5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B6" t="n">
         <v>15</v>
@@ -1228,13 +1238,14 @@
       <c r="BC6"/>
       <c r="BD6"/>
       <c r="BE6"/>
-      <c r="BF6" t="n">
+      <c r="BF6"/>
+      <c r="BG6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -1327,32 +1338,33 @@
       </c>
       <c r="AW7"/>
       <c r="AX7" t="n">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="AY7" t="n">
         <v>1</v>
       </c>
-      <c r="AZ7" t="n">
-        <v>3</v>
-      </c>
+      <c r="AZ7"/>
       <c r="BA7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="BB7" t="n">
         <v>2</v>
       </c>
       <c r="BC7" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD7" t="n">
         <v>4</v>
       </c>
-      <c r="BD7"/>
       <c r="BE7"/>
-      <c r="BF7" t="n">
+      <c r="BF7"/>
+      <c r="BG7" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -1427,22 +1439,23 @@
       <c r="AX8"/>
       <c r="AY8"/>
       <c r="AZ8"/>
-      <c r="BA8" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB8"/>
+      <c r="BA8"/>
+      <c r="BB8" t="n">
+        <v>1</v>
+      </c>
       <c r="BC8"/>
       <c r="BD8"/>
-      <c r="BE8" t="n">
+      <c r="BE8"/>
+      <c r="BF8" t="n">
         <v>5</v>
       </c>
-      <c r="BF8" t="n">
+      <c r="BG8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -1511,24 +1524,27 @@
         <v>2</v>
       </c>
       <c r="AZ9" t="n">
-        <v>3</v>
-      </c>
-      <c r="BA9"/>
-      <c r="BB9" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC9"/>
+        <v>1</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>3</v>
+      </c>
+      <c r="BB9"/>
+      <c r="BC9" t="n">
+        <v>1</v>
+      </c>
       <c r="BD9"/>
-      <c r="BE9" t="n">
-        <v>1</v>
-      </c>
+      <c r="BE9"/>
       <c r="BF9" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B10" t="n">
         <v>32</v>
@@ -1652,33 +1668,36 @@
         <v>128</v>
       </c>
       <c r="AW10"/>
-      <c r="AX10"/>
+      <c r="AX10" t="n">
+        <v>138</v>
+      </c>
       <c r="AY10" t="n">
         <v>5</v>
       </c>
-      <c r="AZ10" t="n">
+      <c r="AZ10"/>
+      <c r="BA10" t="n">
         <v>4</v>
       </c>
-      <c r="BA10" t="n">
-        <v>1</v>
-      </c>
       <c r="BB10" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC10" t="n">
         <v>9</v>
       </c>
-      <c r="BC10" t="n">
+      <c r="BD10" t="n">
         <v>23</v>
       </c>
-      <c r="BD10"/>
-      <c r="BE10" t="n">
+      <c r="BE10"/>
+      <c r="BF10" t="n">
         <v>25</v>
       </c>
-      <c r="BF10" t="n">
+      <c r="BG10" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
@@ -1739,16 +1758,17 @@
       <c r="AZ11"/>
       <c r="BA11"/>
       <c r="BB11"/>
-      <c r="BC11" t="n">
-        <v>2</v>
-      </c>
-      <c r="BD11"/>
+      <c r="BC11"/>
+      <c r="BD11" t="n">
+        <v>2</v>
+      </c>
       <c r="BE11"/>
       <c r="BF11"/>
+      <c r="BG11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B12" t="n">
         <v>13</v>
@@ -1862,29 +1882,30 @@
       <c r="AY12" t="n">
         <v>2</v>
       </c>
-      <c r="AZ12" t="n">
+      <c r="AZ12"/>
+      <c r="BA12" t="n">
         <v>6</v>
       </c>
-      <c r="BA12" t="n">
-        <v>3</v>
-      </c>
       <c r="BB12" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="BC12" t="n">
         <v>8</v>
       </c>
-      <c r="BD12"/>
-      <c r="BE12" t="n">
+      <c r="BD12" t="n">
+        <v>8</v>
+      </c>
+      <c r="BE12"/>
+      <c r="BF12" t="n">
         <v>7</v>
       </c>
-      <c r="BF12" t="n">
+      <c r="BG12" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -1998,27 +2019,28 @@
       <c r="AY13" t="n">
         <v>1</v>
       </c>
-      <c r="AZ13" t="n">
-        <v>1</v>
-      </c>
+      <c r="AZ13"/>
       <c r="BA13" t="n">
         <v>1</v>
       </c>
       <c r="BB13" t="n">
-        <v>2</v>
-      </c>
-      <c r="BC13"/>
+        <v>1</v>
+      </c>
+      <c r="BC13" t="n">
+        <v>2</v>
+      </c>
       <c r="BD13"/>
-      <c r="BE13" t="n">
-        <v>1</v>
-      </c>
+      <c r="BE13"/>
       <c r="BF13" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG13" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -2105,10 +2127,11 @@
       <c r="BD14"/>
       <c r="BE14"/>
       <c r="BF14"/>
+      <c r="BG14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B15" t="n">
         <v>7</v>
@@ -2220,29 +2243,30 @@
       <c r="AY15" t="n">
         <v>5</v>
       </c>
-      <c r="AZ15" t="n">
-        <v>3</v>
-      </c>
+      <c r="AZ15"/>
       <c r="BA15" t="n">
+        <v>3</v>
+      </c>
+      <c r="BB15" t="n">
         <v>6</v>
       </c>
-      <c r="BB15" t="n">
+      <c r="BC15" t="n">
         <v>13</v>
       </c>
-      <c r="BC15" t="n">
+      <c r="BD15" t="n">
         <v>5</v>
       </c>
-      <c r="BD15"/>
-      <c r="BE15" t="n">
+      <c r="BE15"/>
+      <c r="BF15" t="n">
         <v>11</v>
       </c>
-      <c r="BF15" t="n">
+      <c r="BG15" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
@@ -2325,7 +2349,7 @@
       </c>
       <c r="AW16"/>
       <c r="AX16" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AY16"/>
       <c r="AZ16"/>
@@ -2334,13 +2358,14 @@
       <c r="BC16"/>
       <c r="BD16"/>
       <c r="BE16"/>
-      <c r="BF16" t="n">
+      <c r="BF16"/>
+      <c r="BG16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B17" t="n">
         <v>9</v>
@@ -2467,28 +2492,31 @@
         <v>10</v>
       </c>
       <c r="AZ17" t="n">
+        <v>15</v>
+      </c>
+      <c r="BA17" t="n">
         <v>4</v>
       </c>
-      <c r="BA17" t="n">
+      <c r="BB17" t="n">
         <v>9</v>
       </c>
-      <c r="BB17" t="n">
+      <c r="BC17" t="n">
         <v>12</v>
       </c>
-      <c r="BC17" t="n">
+      <c r="BD17" t="n">
         <v>7</v>
       </c>
-      <c r="BD17"/>
-      <c r="BE17" t="n">
+      <c r="BE17"/>
+      <c r="BF17" t="n">
         <v>5</v>
       </c>
-      <c r="BF17" t="n">
+      <c r="BG17" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B18" t="n">
         <v>24</v>
@@ -2620,31 +2648,32 @@
       <c r="AY18" t="n">
         <v>9</v>
       </c>
-      <c r="AZ18" t="n">
+      <c r="AZ18"/>
+      <c r="BA18" t="n">
         <v>19</v>
       </c>
-      <c r="BA18" t="n">
+      <c r="BB18" t="n">
         <v>39</v>
       </c>
-      <c r="BB18" t="n">
+      <c r="BC18" t="n">
         <v>6</v>
       </c>
-      <c r="BC18" t="n">
+      <c r="BD18" t="n">
         <v>20</v>
       </c>
-      <c r="BD18" t="n">
-        <v>1</v>
-      </c>
       <c r="BE18" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF18" t="n">
         <v>32</v>
       </c>
-      <c r="BF18" t="n">
+      <c r="BG18" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B19"/>
       <c r="C19"/>
@@ -2721,10 +2750,11 @@
       <c r="BD19"/>
       <c r="BE19"/>
       <c r="BF19"/>
+      <c r="BG19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B20" t="n">
         <v>32</v>
@@ -2832,27 +2862,28 @@
       <c r="AY20" t="n">
         <v>8</v>
       </c>
-      <c r="AZ20" t="n">
+      <c r="AZ20"/>
+      <c r="BA20" t="n">
         <v>5</v>
       </c>
-      <c r="BA20" t="n">
+      <c r="BB20" t="n">
         <v>9</v>
       </c>
-      <c r="BB20" t="n">
+      <c r="BC20" t="n">
         <v>10</v>
       </c>
-      <c r="BC20"/>
       <c r="BD20"/>
-      <c r="BE20" t="n">
+      <c r="BE20"/>
+      <c r="BF20" t="n">
         <v>8</v>
       </c>
-      <c r="BF20" t="n">
+      <c r="BG20" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B21" t="n">
         <v>33</v>
@@ -2986,29 +3017,30 @@
       <c r="AY21" t="n">
         <v>15</v>
       </c>
-      <c r="AZ21" t="n">
-        <v>3</v>
-      </c>
+      <c r="AZ21"/>
       <c r="BA21" t="n">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="BB21" t="n">
         <v>28</v>
       </c>
       <c r="BC21" t="n">
+        <v>28</v>
+      </c>
+      <c r="BD21" t="n">
         <v>22</v>
       </c>
-      <c r="BD21"/>
-      <c r="BE21" t="n">
+      <c r="BE21"/>
+      <c r="BF21" t="n">
         <v>17</v>
       </c>
-      <c r="BF21" t="n">
+      <c r="BG21" t="n">
         <v>82</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -3071,10 +3103,11 @@
       <c r="BD22"/>
       <c r="BE22"/>
       <c r="BF22"/>
+      <c r="BG22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -3143,10 +3176,11 @@
       <c r="BD23"/>
       <c r="BE23"/>
       <c r="BF23"/>
+      <c r="BG23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -3207,10 +3241,11 @@
       <c r="BD24"/>
       <c r="BE24"/>
       <c r="BF24"/>
+      <c r="BG24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B25" t="n">
         <v>1</v>
@@ -3300,21 +3335,22 @@
         <v>5</v>
       </c>
       <c r="AY25"/>
-      <c r="AZ25" t="n">
-        <v>1</v>
-      </c>
-      <c r="BA25"/>
+      <c r="AZ25"/>
+      <c r="BA25" t="n">
+        <v>1</v>
+      </c>
       <c r="BB25"/>
       <c r="BC25"/>
       <c r="BD25"/>
       <c r="BE25"/>
-      <c r="BF25" t="n">
+      <c r="BF25"/>
+      <c r="BG25" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B26" t="n">
         <v>2</v>
@@ -3381,10 +3417,11 @@
       <c r="BD26"/>
       <c r="BE26"/>
       <c r="BF26"/>
+      <c r="BG26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B27" t="n">
         <v>4</v>
@@ -3500,25 +3537,26 @@
       <c r="AY27" t="n">
         <v>2</v>
       </c>
-      <c r="AZ27" t="n">
-        <v>2</v>
-      </c>
+      <c r="AZ27"/>
       <c r="BA27" t="n">
+        <v>2</v>
+      </c>
+      <c r="BB27" t="n">
         <v>5</v>
       </c>
-      <c r="BB27"/>
       <c r="BC27"/>
       <c r="BD27"/>
-      <c r="BE27" t="n">
-        <v>3</v>
-      </c>
+      <c r="BE27"/>
       <c r="BF27" t="n">
+        <v>3</v>
+      </c>
+      <c r="BG27" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B28" t="n">
         <v>27</v>
@@ -3635,34 +3673,37 @@
       </c>
       <c r="AW28"/>
       <c r="AX28" t="n">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="AY28" t="n">
         <v>6</v>
       </c>
       <c r="AZ28" t="n">
+        <v>25</v>
+      </c>
+      <c r="BA28" t="n">
         <v>5</v>
       </c>
-      <c r="BA28" t="n">
+      <c r="BB28" t="n">
         <v>7</v>
       </c>
-      <c r="BB28" t="n">
+      <c r="BC28" t="n">
         <v>4</v>
       </c>
-      <c r="BC28" t="n">
+      <c r="BD28" t="n">
         <v>5</v>
       </c>
-      <c r="BD28"/>
-      <c r="BE28" t="n">
+      <c r="BE28"/>
+      <c r="BF28" t="n">
         <v>20</v>
       </c>
-      <c r="BF28" t="n">
+      <c r="BG28" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B29" t="n">
         <v>110</v>
@@ -3778,29 +3819,30 @@
       <c r="AY29" t="n">
         <v>8</v>
       </c>
-      <c r="AZ29" t="n">
-        <v>3</v>
-      </c>
+      <c r="AZ29"/>
       <c r="BA29" t="n">
+        <v>3</v>
+      </c>
+      <c r="BB29" t="n">
         <v>9</v>
       </c>
-      <c r="BB29" t="n">
+      <c r="BC29" t="n">
         <v>4</v>
       </c>
-      <c r="BC29" t="n">
+      <c r="BD29" t="n">
         <v>8</v>
       </c>
-      <c r="BD29"/>
-      <c r="BE29" t="n">
+      <c r="BE29"/>
+      <c r="BF29" t="n">
         <v>17</v>
       </c>
-      <c r="BF29" t="n">
+      <c r="BG29" t="n">
         <v>57</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B30" t="n">
         <v>30</v>
@@ -3920,33 +3962,36 @@
       <c r="AW30" t="n">
         <v>6</v>
       </c>
-      <c r="AX30"/>
+      <c r="AX30" t="n">
+        <v>13</v>
+      </c>
       <c r="AY30" t="n">
         <v>2</v>
       </c>
-      <c r="AZ30" t="n">
+      <c r="AZ30"/>
+      <c r="BA30" t="n">
         <v>4</v>
       </c>
-      <c r="BA30" t="n">
+      <c r="BB30" t="n">
         <v>14</v>
       </c>
-      <c r="BB30" t="n">
+      <c r="BC30" t="n">
         <v>8</v>
       </c>
-      <c r="BC30" t="n">
-        <v>3</v>
-      </c>
-      <c r="BD30"/>
-      <c r="BE30" t="n">
+      <c r="BD30" t="n">
+        <v>3</v>
+      </c>
+      <c r="BE30"/>
+      <c r="BF30" t="n">
         <v>7</v>
       </c>
-      <c r="BF30" t="n">
+      <c r="BG30" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -4009,10 +4054,11 @@
       <c r="BD31"/>
       <c r="BE31"/>
       <c r="BF31"/>
+      <c r="BG31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B32" t="n">
         <v>13</v>
@@ -4140,29 +4186,30 @@
       <c r="AY32" t="n">
         <v>3</v>
       </c>
-      <c r="AZ32" t="n">
+      <c r="AZ32"/>
+      <c r="BA32" t="n">
         <v>4</v>
       </c>
-      <c r="BA32" t="n">
+      <c r="BB32" t="n">
         <v>7</v>
       </c>
-      <c r="BB32" t="n">
+      <c r="BC32" t="n">
         <v>16</v>
       </c>
-      <c r="BC32" t="n">
+      <c r="BD32" t="n">
         <v>7</v>
       </c>
-      <c r="BD32"/>
-      <c r="BE32" t="n">
+      <c r="BE32"/>
+      <c r="BF32" t="n">
         <v>24</v>
       </c>
-      <c r="BF32" t="n">
+      <c r="BG32" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
@@ -4250,19 +4297,20 @@
       </c>
       <c r="AZ33"/>
       <c r="BA33"/>
-      <c r="BB33" t="n">
-        <v>1</v>
-      </c>
+      <c r="BB33"/>
       <c r="BC33" t="n">
         <v>1</v>
       </c>
-      <c r="BD33"/>
+      <c r="BD33" t="n">
+        <v>1</v>
+      </c>
       <c r="BE33"/>
       <c r="BF33"/>
+      <c r="BG33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B34"/>
       <c r="C34"/>
@@ -4365,22 +4413,25 @@
       </c>
       <c r="AY34"/>
       <c r="AZ34" t="n">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="BA34" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB34" t="n">
         <v>5</v>
       </c>
-      <c r="BB34" t="n">
-        <v>3</v>
-      </c>
       <c r="BC34" t="n">
         <v>3</v>
       </c>
-      <c r="BD34"/>
-      <c r="BE34" t="n">
-        <v>1</v>
-      </c>
+      <c r="BD34" t="n">
+        <v>3</v>
+      </c>
+      <c r="BE34"/>
       <c r="BF34" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG34" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
26th April 1st update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/state/ncov19state_long.xlsx
+++ b/covid19_data/excel/state/ncov19state_long.xlsx
@@ -2019,7 +2019,9 @@
       <c r="AY13" t="n">
         <v>1</v>
       </c>
-      <c r="AZ13"/>
+      <c r="AZ13" t="n">
+        <v>5</v>
+      </c>
       <c r="BA13" t="n">
         <v>1</v>
       </c>
@@ -2352,7 +2354,9 @@
         <v>6</v>
       </c>
       <c r="AY16"/>
-      <c r="AZ16"/>
+      <c r="AZ16" t="n">
+        <v>4</v>
+      </c>
       <c r="BA16"/>
       <c r="BB16"/>
       <c r="BC16"/>
@@ -2648,7 +2652,9 @@
       <c r="AY18" t="n">
         <v>9</v>
       </c>
-      <c r="AZ18"/>
+      <c r="AZ18" t="n">
+        <v>7</v>
+      </c>
       <c r="BA18" t="n">
         <v>19</v>
       </c>
@@ -3679,7 +3685,7 @@
         <v>6</v>
       </c>
       <c r="AZ28" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="BA28" t="n">
         <v>5</v>
@@ -4186,7 +4192,9 @@
       <c r="AY32" t="n">
         <v>3</v>
       </c>
-      <c r="AZ32"/>
+      <c r="AZ32" t="n">
+        <v>157</v>
+      </c>
       <c r="BA32" t="n">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
27th April 1st update
</commit_message>
<xml_diff>
--- a/covid19_data/excel/state/ncov19state_long.xlsx
+++ b/covid19_data/excel/state/ncov19state_long.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t xml:space="preserve">detectedstate</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t xml:space="preserve">26/03/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26/04/2020</t>
   </si>
   <si>
     <t xml:space="preserve">27/03/2020</t>
@@ -797,10 +800,13 @@
       <c r="BG1" t="s">
         <v>58</v>
       </c>
+      <c r="BH1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B2"/>
       <c r="C2"/>
@@ -818,9 +824,7 @@
         <v>1</v>
       </c>
       <c r="O2"/>
-      <c r="P2" t="n">
-        <v>1</v>
-      </c>
+      <c r="P2"/>
       <c r="Q2"/>
       <c r="R2"/>
       <c r="S2"/>
@@ -856,20 +860,21 @@
       <c r="AW2"/>
       <c r="AX2"/>
       <c r="AY2"/>
-      <c r="AZ2" t="n">
-        <v>118</v>
-      </c>
+      <c r="AZ2"/>
       <c r="BA2"/>
-      <c r="BB2"/>
+      <c r="BB2" t="n">
+        <v>1</v>
+      </c>
       <c r="BC2"/>
       <c r="BD2"/>
       <c r="BE2"/>
       <c r="BF2"/>
       <c r="BG2"/>
+      <c r="BH2"/>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B3"/>
       <c r="C3"/>
@@ -945,22 +950,23 @@
       <c r="BA3" t="n">
         <v>1</v>
       </c>
-      <c r="BB3" t="n">
+      <c r="BB3"/>
+      <c r="BC3" t="n">
         <v>5</v>
       </c>
-      <c r="BC3" t="n">
-        <v>3</v>
-      </c>
-      <c r="BD3"/>
+      <c r="BD3" t="n">
+        <v>3</v>
+      </c>
       <c r="BE3"/>
-      <c r="BF3" t="n">
-        <v>1</v>
-      </c>
-      <c r="BG3"/>
+      <c r="BF3"/>
+      <c r="BG3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH3"/>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B4" t="n">
         <v>67</v>
@@ -1081,25 +1087,28 @@
         <v>1</v>
       </c>
       <c r="BB4" t="n">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="BC4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD4" t="n">
         <v>6</v>
       </c>
-      <c r="BD4" t="n">
-        <v>2</v>
-      </c>
-      <c r="BE4"/>
-      <c r="BF4" t="n">
-        <v>2</v>
-      </c>
+      <c r="BE4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BF4"/>
       <c r="BG4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BH4" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
@@ -1161,10 +1170,11 @@
       <c r="BE5"/>
       <c r="BF5"/>
       <c r="BG5"/>
+      <c r="BH5"/>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B6" t="n">
         <v>15</v>
@@ -1243,13 +1253,14 @@
       <c r="BD6"/>
       <c r="BE6"/>
       <c r="BF6"/>
-      <c r="BG6" t="n">
+      <c r="BG6"/>
+      <c r="BH6" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" t="n">
         <v>3</v>
@@ -1353,24 +1364,25 @@
       <c r="BA7" t="n">
         <v>3</v>
       </c>
-      <c r="BB7" t="n">
-        <v>2</v>
-      </c>
+      <c r="BB7"/>
       <c r="BC7" t="n">
         <v>2</v>
       </c>
       <c r="BD7" t="n">
+        <v>2</v>
+      </c>
+      <c r="BE7" t="n">
         <v>4</v>
       </c>
-      <c r="BE7"/>
       <c r="BF7"/>
-      <c r="BG7" t="n">
+      <c r="BG7"/>
+      <c r="BH7" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B8" t="n">
         <v>2</v>
@@ -1448,22 +1460,23 @@
         <v>1</v>
       </c>
       <c r="BA8"/>
-      <c r="BB8" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC8"/>
+      <c r="BB8"/>
+      <c r="BC8" t="n">
+        <v>1</v>
+      </c>
       <c r="BD8"/>
       <c r="BE8"/>
-      <c r="BF8" t="n">
+      <c r="BF8"/>
+      <c r="BG8" t="n">
         <v>5</v>
       </c>
-      <c r="BG8" t="n">
+      <c r="BH8" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -1538,21 +1551,22 @@
         <v>3</v>
       </c>
       <c r="BB9"/>
-      <c r="BC9" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD9"/>
+      <c r="BC9"/>
+      <c r="BD9" t="n">
+        <v>1</v>
+      </c>
       <c r="BE9"/>
-      <c r="BF9" t="n">
-        <v>1</v>
-      </c>
+      <c r="BF9"/>
       <c r="BG9" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH9" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B10" t="n">
         <v>32</v>
@@ -1688,26 +1702,27 @@
       <c r="BA10" t="n">
         <v>4</v>
       </c>
-      <c r="BB10" t="n">
-        <v>1</v>
-      </c>
+      <c r="BB10"/>
       <c r="BC10" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD10" t="n">
         <v>9</v>
       </c>
-      <c r="BD10" t="n">
+      <c r="BE10" t="n">
         <v>23</v>
       </c>
-      <c r="BE10"/>
-      <c r="BF10" t="n">
+      <c r="BF10"/>
+      <c r="BG10" t="n">
         <v>25</v>
       </c>
-      <c r="BG10" t="n">
+      <c r="BH10" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B11"/>
       <c r="C11"/>
@@ -1769,16 +1784,17 @@
       <c r="BA11"/>
       <c r="BB11"/>
       <c r="BC11"/>
-      <c r="BD11" t="n">
-        <v>2</v>
-      </c>
-      <c r="BE11"/>
+      <c r="BD11"/>
+      <c r="BE11" t="n">
+        <v>2</v>
+      </c>
       <c r="BF11"/>
       <c r="BG11"/>
+      <c r="BH11"/>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B12" t="n">
         <v>13</v>
@@ -1898,26 +1914,27 @@
       <c r="BA12" t="n">
         <v>6</v>
       </c>
-      <c r="BB12" t="n">
-        <v>3</v>
-      </c>
+      <c r="BB12"/>
       <c r="BC12" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="BD12" t="n">
         <v>8</v>
       </c>
-      <c r="BE12"/>
-      <c r="BF12" t="n">
+      <c r="BE12" t="n">
+        <v>8</v>
+      </c>
+      <c r="BF12"/>
+      <c r="BG12" t="n">
         <v>7</v>
       </c>
-      <c r="BG12" t="n">
+      <c r="BH12" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
@@ -2037,24 +2054,25 @@
       <c r="BA13" t="n">
         <v>1</v>
       </c>
-      <c r="BB13" t="n">
-        <v>1</v>
-      </c>
+      <c r="BB13"/>
       <c r="BC13" t="n">
-        <v>2</v>
-      </c>
-      <c r="BD13"/>
+        <v>1</v>
+      </c>
+      <c r="BD13" t="n">
+        <v>2</v>
+      </c>
       <c r="BE13"/>
-      <c r="BF13" t="n">
-        <v>1</v>
-      </c>
+      <c r="BF13"/>
       <c r="BG13" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH13" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B14"/>
       <c r="C14"/>
@@ -2142,10 +2160,11 @@
       <c r="BE14"/>
       <c r="BF14"/>
       <c r="BG14"/>
+      <c r="BH14"/>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B15" t="n">
         <v>7</v>
@@ -2263,26 +2282,27 @@
       <c r="BA15" t="n">
         <v>3</v>
       </c>
-      <c r="BB15" t="n">
+      <c r="BB15"/>
+      <c r="BC15" t="n">
         <v>6</v>
       </c>
-      <c r="BC15" t="n">
+      <c r="BD15" t="n">
         <v>13</v>
       </c>
-      <c r="BD15" t="n">
+      <c r="BE15" t="n">
         <v>5</v>
       </c>
-      <c r="BE15"/>
-      <c r="BF15" t="n">
+      <c r="BF15"/>
+      <c r="BG15" t="n">
         <v>11</v>
       </c>
-      <c r="BG15" t="n">
+      <c r="BH15" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
@@ -2377,13 +2397,14 @@
       <c r="BD16"/>
       <c r="BE16"/>
       <c r="BF16"/>
-      <c r="BG16" t="n">
+      <c r="BG16"/>
+      <c r="BH16" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B17" t="n">
         <v>9</v>
@@ -2516,25 +2537,28 @@
         <v>4</v>
       </c>
       <c r="BB17" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC17" t="n">
         <v>9</v>
       </c>
-      <c r="BC17" t="n">
+      <c r="BD17" t="n">
         <v>12</v>
       </c>
-      <c r="BD17" t="n">
+      <c r="BE17" t="n">
         <v>7</v>
       </c>
-      <c r="BE17"/>
-      <c r="BF17" t="n">
+      <c r="BF17"/>
+      <c r="BG17" t="n">
         <v>5</v>
       </c>
-      <c r="BG17" t="n">
+      <c r="BH17" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B18" t="n">
         <v>24</v>
@@ -2567,7 +2591,7 @@
       </c>
       <c r="O18"/>
       <c r="P18" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q18" t="n">
         <v>5</v>
@@ -2672,28 +2696,29 @@
       <c r="BA18" t="n">
         <v>19</v>
       </c>
-      <c r="BB18" t="n">
+      <c r="BB18"/>
+      <c r="BC18" t="n">
         <v>39</v>
       </c>
-      <c r="BC18" t="n">
+      <c r="BD18" t="n">
         <v>6</v>
       </c>
-      <c r="BD18" t="n">
+      <c r="BE18" t="n">
         <v>20</v>
       </c>
-      <c r="BE18" t="n">
-        <v>1</v>
-      </c>
       <c r="BF18" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG18" t="n">
         <v>32</v>
       </c>
-      <c r="BG18" t="n">
+      <c r="BH18" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B19"/>
       <c r="C19"/>
@@ -2773,10 +2798,11 @@
       <c r="BE19"/>
       <c r="BF19"/>
       <c r="BG19"/>
+      <c r="BH19"/>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B20" t="n">
         <v>32</v>
@@ -2890,24 +2916,25 @@
       <c r="BA20" t="n">
         <v>5</v>
       </c>
-      <c r="BB20" t="n">
+      <c r="BB20"/>
+      <c r="BC20" t="n">
         <v>9</v>
       </c>
-      <c r="BC20" t="n">
+      <c r="BD20" t="n">
         <v>10</v>
       </c>
-      <c r="BD20"/>
       <c r="BE20"/>
-      <c r="BF20" t="n">
+      <c r="BF20"/>
+      <c r="BG20" t="n">
         <v>8</v>
       </c>
-      <c r="BG20" t="n">
+      <c r="BH20" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B21" t="n">
         <v>33</v>
@@ -3047,26 +3074,27 @@
       <c r="BA21" t="n">
         <v>3</v>
       </c>
-      <c r="BB21" t="n">
-        <v>28</v>
-      </c>
+      <c r="BB21"/>
       <c r="BC21" t="n">
         <v>28</v>
       </c>
       <c r="BD21" t="n">
+        <v>28</v>
+      </c>
+      <c r="BE21" t="n">
         <v>22</v>
       </c>
-      <c r="BE21"/>
-      <c r="BF21" t="n">
+      <c r="BF21"/>
+      <c r="BG21" t="n">
         <v>17</v>
       </c>
-      <c r="BG21" t="n">
+      <c r="BH21" t="n">
         <v>82</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B22"/>
       <c r="C22"/>
@@ -3130,10 +3158,11 @@
       <c r="BE22"/>
       <c r="BF22"/>
       <c r="BG22"/>
+      <c r="BH22"/>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B23"/>
       <c r="C23"/>
@@ -3203,10 +3232,11 @@
       <c r="BE23"/>
       <c r="BF23"/>
       <c r="BG23"/>
+      <c r="BH23"/>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B24"/>
       <c r="C24"/>
@@ -3268,10 +3298,11 @@
       <c r="BE24"/>
       <c r="BF24"/>
       <c r="BG24"/>
+      <c r="BH24"/>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B25" t="n">
         <v>1</v>
@@ -3367,18 +3398,21 @@
       <c r="BA25" t="n">
         <v>1</v>
       </c>
-      <c r="BB25"/>
+      <c r="BB25" t="n">
+        <v>3</v>
+      </c>
       <c r="BC25"/>
       <c r="BD25"/>
       <c r="BE25"/>
       <c r="BF25"/>
-      <c r="BG25" t="n">
+      <c r="BG25"/>
+      <c r="BH25" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B26" t="n">
         <v>2</v>
@@ -3448,10 +3482,11 @@
       <c r="BE26"/>
       <c r="BF26"/>
       <c r="BG26"/>
+      <c r="BH26"/>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B27" t="n">
         <v>4</v>
@@ -3573,22 +3608,23 @@
       <c r="BA27" t="n">
         <v>2</v>
       </c>
-      <c r="BB27" t="n">
+      <c r="BB27"/>
+      <c r="BC27" t="n">
         <v>5</v>
       </c>
-      <c r="BC27"/>
       <c r="BD27"/>
       <c r="BE27"/>
-      <c r="BF27" t="n">
-        <v>3</v>
-      </c>
+      <c r="BF27"/>
       <c r="BG27" t="n">
+        <v>3</v>
+      </c>
+      <c r="BH27" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B28" t="n">
         <v>27</v>
@@ -3717,25 +3753,28 @@
         <v>5</v>
       </c>
       <c r="BB28" t="n">
+        <v>58</v>
+      </c>
+      <c r="BC28" t="n">
         <v>7</v>
       </c>
-      <c r="BC28" t="n">
+      <c r="BD28" t="n">
         <v>4</v>
       </c>
-      <c r="BD28" t="n">
+      <c r="BE28" t="n">
         <v>5</v>
       </c>
-      <c r="BE28"/>
-      <c r="BF28" t="n">
+      <c r="BF28"/>
+      <c r="BG28" t="n">
         <v>20</v>
       </c>
-      <c r="BG28" t="n">
+      <c r="BH28" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B29" t="n">
         <v>110</v>
@@ -3857,26 +3896,27 @@
       <c r="BA29" t="n">
         <v>3</v>
       </c>
-      <c r="BB29" t="n">
+      <c r="BB29"/>
+      <c r="BC29" t="n">
         <v>9</v>
       </c>
-      <c r="BC29" t="n">
+      <c r="BD29" t="n">
         <v>4</v>
       </c>
-      <c r="BD29" t="n">
+      <c r="BE29" t="n">
         <v>8</v>
       </c>
-      <c r="BE29"/>
-      <c r="BF29" t="n">
+      <c r="BF29"/>
+      <c r="BG29" t="n">
         <v>17</v>
       </c>
-      <c r="BG29" t="n">
+      <c r="BH29" t="n">
         <v>57</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B30" t="n">
         <v>30</v>
@@ -4008,26 +4048,27 @@
       <c r="BA30" t="n">
         <v>4</v>
       </c>
-      <c r="BB30" t="n">
+      <c r="BB30"/>
+      <c r="BC30" t="n">
         <v>14</v>
       </c>
-      <c r="BC30" t="n">
+      <c r="BD30" t="n">
         <v>8</v>
       </c>
-      <c r="BD30" t="n">
-        <v>3</v>
-      </c>
-      <c r="BE30"/>
-      <c r="BF30" t="n">
+      <c r="BE30" t="n">
+        <v>3</v>
+      </c>
+      <c r="BF30"/>
+      <c r="BG30" t="n">
         <v>7</v>
       </c>
-      <c r="BG30" t="n">
+      <c r="BH30" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B31"/>
       <c r="C31"/>
@@ -4091,10 +4132,11 @@
       <c r="BE31"/>
       <c r="BF31"/>
       <c r="BG31"/>
+      <c r="BH31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B32" t="n">
         <v>13</v>
@@ -4228,26 +4270,27 @@
       <c r="BA32" t="n">
         <v>4</v>
       </c>
-      <c r="BB32" t="n">
+      <c r="BB32"/>
+      <c r="BC32" t="n">
         <v>7</v>
       </c>
-      <c r="BC32" t="n">
+      <c r="BD32" t="n">
         <v>16</v>
       </c>
-      <c r="BD32" t="n">
+      <c r="BE32" t="n">
         <v>7</v>
       </c>
-      <c r="BE32"/>
-      <c r="BF32" t="n">
+      <c r="BF32"/>
+      <c r="BG32" t="n">
         <v>24</v>
       </c>
-      <c r="BG32" t="n">
+      <c r="BH32" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B33"/>
       <c r="C33"/>
@@ -4335,20 +4378,23 @@
       </c>
       <c r="AZ33"/>
       <c r="BA33"/>
-      <c r="BB33"/>
-      <c r="BC33" t="n">
-        <v>1</v>
-      </c>
+      <c r="BB33" t="n">
+        <v>2</v>
+      </c>
+      <c r="BC33"/>
       <c r="BD33" t="n">
         <v>1</v>
       </c>
-      <c r="BE33"/>
+      <c r="BE33" t="n">
+        <v>1</v>
+      </c>
       <c r="BF33"/>
       <c r="BG33"/>
+      <c r="BH33"/>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B34"/>
       <c r="C34"/>
@@ -4457,19 +4503,22 @@
         <v>1</v>
       </c>
       <c r="BB34" t="n">
+        <v>40</v>
+      </c>
+      <c r="BC34" t="n">
         <v>5</v>
       </c>
-      <c r="BC34" t="n">
-        <v>3</v>
-      </c>
       <c r="BD34" t="n">
         <v>3</v>
       </c>
-      <c r="BE34"/>
-      <c r="BF34" t="n">
-        <v>1</v>
-      </c>
+      <c r="BE34" t="n">
+        <v>3</v>
+      </c>
+      <c r="BF34"/>
       <c r="BG34" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH34" t="n">
         <v>15</v>
       </c>
     </row>

</xml_diff>